<commit_message>
configurar y mejorar informes
</commit_message>
<xml_diff>
--- a/public/templates/report_template_project.xlsx
+++ b/public/templates/report_template_project.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gpro1\MyFiles\QuisVar\quisvar_proyect_ft\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcastillo\Documents\QuisVar\quisvar_proyect_ft\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457066FB-CDA5-40EE-A02B-64EC50E11805}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCA908E-26C9-45BC-9694-B2D1D080E3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="482" firstSheet="1" activeTab="1" xr2:uid="{F98A2DB2-54A5-485C-A701-CE43CF6B2BAF}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="364">
   <si>
     <t>ITEM</t>
   </si>
@@ -1596,24 +1596,6 @@
     <t>ING JUAN GONZALO QUISPE CONDORI</t>
   </si>
   <si>
-    <t>TOTAL DE DESCUENTO ASISTENCIA:</t>
-  </si>
-  <si>
-    <t>COSTO PARCIAL:</t>
-  </si>
-  <si>
-    <t>TOTAL DE DESCUENTO POR REPORTE:</t>
-  </si>
-  <si>
-    <t>LIQUIDO A PERCIBIR ADELANTO:</t>
-  </si>
-  <si>
-    <t>ADELANTO POR COSTO PARCIAL:</t>
-  </si>
-  <si>
-    <t>SALDO:</t>
-  </si>
-  <si>
     <t>FECHA DE INICIO</t>
   </si>
   <si>
@@ -1684,6 +1666,9 @@
   </si>
   <si>
     <t>Nivel4</t>
+  </si>
+  <si>
+    <t>sadsa</t>
   </si>
 </sst>
 </file>
@@ -1948,8 +1933,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color theme="2"/>
+      <u/>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
@@ -3127,7 +3113,7 @@
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="339">
+  <cellXfs count="330">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3651,30 +3637,6 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="9" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3732,12 +3694,6 @@
     <xf numFmtId="0" fontId="21" fillId="9" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="33" fillId="10" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="33" fillId="9" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3747,6 +3703,44 @@
     <xf numFmtId="0" fontId="21" fillId="9" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="33" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -3867,96 +3861,93 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4014,46 +4005,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -4422,174 +4381,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="269" t="s">
+      <c r="A1" s="273" t="s">
         <v>325</v>
       </c>
-      <c r="B1" s="268"/>
-      <c r="C1" s="268"/>
-      <c r="D1" s="268"/>
-      <c r="E1" s="268"/>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="268"/>
-      <c r="I1" s="268"/>
-      <c r="J1" s="268"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="268"/>
-      <c r="M1" s="268"/>
-      <c r="N1" s="268"/>
-      <c r="O1" s="267" t="s">
+      <c r="B1" s="272"/>
+      <c r="C1" s="272"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="272"/>
+      <c r="I1" s="272"/>
+      <c r="J1" s="272"/>
+      <c r="K1" s="272"/>
+      <c r="L1" s="272"/>
+      <c r="M1" s="272"/>
+      <c r="N1" s="272"/>
+      <c r="O1" s="271" t="s">
         <v>323</v>
       </c>
-      <c r="P1" s="267"/>
-      <c r="Q1" s="267"/>
-      <c r="R1" s="267"/>
-      <c r="S1" s="267"/>
-      <c r="T1" s="267"/>
-      <c r="U1" s="267"/>
-      <c r="V1" s="267"/>
-      <c r="W1" s="267"/>
-      <c r="X1" s="267"/>
-      <c r="Y1" s="267"/>
-      <c r="Z1" s="267"/>
-      <c r="AA1" s="267"/>
-      <c r="AB1" s="267"/>
-      <c r="AC1" s="267"/>
-      <c r="AD1" s="267"/>
-      <c r="AE1" s="267"/>
-      <c r="AF1" s="267"/>
-      <c r="AG1" s="267"/>
-      <c r="AH1" s="268" t="s">
+      <c r="P1" s="271"/>
+      <c r="Q1" s="271"/>
+      <c r="R1" s="271"/>
+      <c r="S1" s="271"/>
+      <c r="T1" s="271"/>
+      <c r="U1" s="271"/>
+      <c r="V1" s="271"/>
+      <c r="W1" s="271"/>
+      <c r="X1" s="271"/>
+      <c r="Y1" s="271"/>
+      <c r="Z1" s="271"/>
+      <c r="AA1" s="271"/>
+      <c r="AB1" s="271"/>
+      <c r="AC1" s="271"/>
+      <c r="AD1" s="271"/>
+      <c r="AE1" s="271"/>
+      <c r="AF1" s="271"/>
+      <c r="AG1" s="271"/>
+      <c r="AH1" s="272" t="s">
         <v>317</v>
       </c>
-      <c r="AI1" s="268"/>
-      <c r="AJ1" s="268"/>
-      <c r="AK1" s="268"/>
-      <c r="AL1" s="265" t="s">
+      <c r="AI1" s="272"/>
+      <c r="AJ1" s="272"/>
+      <c r="AK1" s="272"/>
+      <c r="AL1" s="269" t="s">
         <v>324</v>
       </c>
-      <c r="AM1" s="265"/>
-      <c r="AN1" s="265"/>
-      <c r="AO1" s="265"/>
-      <c r="AP1" s="265"/>
-      <c r="AQ1" s="265"/>
-      <c r="AR1" s="265"/>
-      <c r="AS1" s="265"/>
-      <c r="AT1" s="265"/>
-      <c r="AU1" s="265"/>
-      <c r="AV1" s="265"/>
-      <c r="AW1" s="265"/>
-      <c r="AX1" s="265"/>
-      <c r="AY1" s="265"/>
-      <c r="AZ1" s="265"/>
-      <c r="BA1" s="265"/>
-      <c r="BB1" s="265"/>
-      <c r="BC1" s="265"/>
-      <c r="BD1" s="266"/>
+      <c r="AM1" s="269"/>
+      <c r="AN1" s="269"/>
+      <c r="AO1" s="269"/>
+      <c r="AP1" s="269"/>
+      <c r="AQ1" s="269"/>
+      <c r="AR1" s="269"/>
+      <c r="AS1" s="269"/>
+      <c r="AT1" s="269"/>
+      <c r="AU1" s="269"/>
+      <c r="AV1" s="269"/>
+      <c r="AW1" s="269"/>
+      <c r="AX1" s="269"/>
+      <c r="AY1" s="269"/>
+      <c r="AZ1" s="269"/>
+      <c r="BA1" s="269"/>
+      <c r="BB1" s="269"/>
+      <c r="BC1" s="269"/>
+      <c r="BD1" s="270"/>
     </row>
     <row r="2" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="235" t="s">
+      <c r="A2" s="239" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="236"/>
+      <c r="B2" s="240"/>
       <c r="C2" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D2" s="239" t="s">
+      <c r="D2" s="243" t="s">
         <v>327</v>
       </c>
-      <c r="E2" s="239"/>
-      <c r="F2" s="271" t="s">
+      <c r="E2" s="243"/>
+      <c r="F2" s="275" t="s">
         <v>326</v>
       </c>
-      <c r="G2" s="271"/>
-      <c r="H2" s="271"/>
-      <c r="I2" s="271"/>
-      <c r="J2" s="271"/>
-      <c r="K2" s="271"/>
-      <c r="L2" s="271"/>
-      <c r="M2" s="271"/>
-      <c r="N2" s="271"/>
-      <c r="O2" s="271"/>
-      <c r="P2" s="271"/>
-      <c r="Q2" s="271"/>
-      <c r="R2" s="271"/>
-      <c r="S2" s="271"/>
-      <c r="T2" s="271"/>
-      <c r="U2" s="271"/>
-      <c r="V2" s="271"/>
-      <c r="W2" s="271"/>
-      <c r="X2" s="271"/>
-      <c r="Y2" s="271"/>
-      <c r="Z2" s="271"/>
-      <c r="AA2" s="271"/>
-      <c r="AB2" s="271"/>
-      <c r="AC2" s="271"/>
-      <c r="AD2" s="271"/>
-      <c r="AE2" s="271"/>
-      <c r="AF2" s="271"/>
-      <c r="AG2" s="271"/>
-      <c r="AH2" s="271"/>
-      <c r="AI2" s="271"/>
-      <c r="AJ2" s="271"/>
-      <c r="AK2" s="271"/>
-      <c r="AL2" s="271"/>
-      <c r="AM2" s="271"/>
-      <c r="AN2" s="271"/>
-      <c r="AO2" s="271"/>
-      <c r="AP2" s="271"/>
-      <c r="AQ2" s="271"/>
-      <c r="AR2" s="271"/>
-      <c r="AS2" s="271"/>
-      <c r="AT2" s="271"/>
-      <c r="AU2" s="271"/>
-      <c r="AV2" s="271"/>
-      <c r="AW2" s="271"/>
-      <c r="AX2" s="271"/>
-      <c r="AY2" s="271"/>
-      <c r="AZ2" s="271"/>
-      <c r="BA2" s="271"/>
-      <c r="BB2" s="271"/>
-      <c r="BC2" s="271"/>
-      <c r="BD2" s="272"/>
+      <c r="G2" s="275"/>
+      <c r="H2" s="275"/>
+      <c r="I2" s="275"/>
+      <c r="J2" s="275"/>
+      <c r="K2" s="275"/>
+      <c r="L2" s="275"/>
+      <c r="M2" s="275"/>
+      <c r="N2" s="275"/>
+      <c r="O2" s="275"/>
+      <c r="P2" s="275"/>
+      <c r="Q2" s="275"/>
+      <c r="R2" s="275"/>
+      <c r="S2" s="275"/>
+      <c r="T2" s="275"/>
+      <c r="U2" s="275"/>
+      <c r="V2" s="275"/>
+      <c r="W2" s="275"/>
+      <c r="X2" s="275"/>
+      <c r="Y2" s="275"/>
+      <c r="Z2" s="275"/>
+      <c r="AA2" s="275"/>
+      <c r="AB2" s="275"/>
+      <c r="AC2" s="275"/>
+      <c r="AD2" s="275"/>
+      <c r="AE2" s="275"/>
+      <c r="AF2" s="275"/>
+      <c r="AG2" s="275"/>
+      <c r="AH2" s="275"/>
+      <c r="AI2" s="275"/>
+      <c r="AJ2" s="275"/>
+      <c r="AK2" s="275"/>
+      <c r="AL2" s="275"/>
+      <c r="AM2" s="275"/>
+      <c r="AN2" s="275"/>
+      <c r="AO2" s="275"/>
+      <c r="AP2" s="275"/>
+      <c r="AQ2" s="275"/>
+      <c r="AR2" s="275"/>
+      <c r="AS2" s="275"/>
+      <c r="AT2" s="275"/>
+      <c r="AU2" s="275"/>
+      <c r="AV2" s="275"/>
+      <c r="AW2" s="275"/>
+      <c r="AX2" s="275"/>
+      <c r="AY2" s="275"/>
+      <c r="AZ2" s="275"/>
+      <c r="BA2" s="275"/>
+      <c r="BB2" s="275"/>
+      <c r="BC2" s="275"/>
+      <c r="BD2" s="276"/>
     </row>
     <row r="3" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="235" t="s">
+      <c r="A3" s="239" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="236"/>
+      <c r="B3" s="240"/>
       <c r="C3" s="141" t="s">
         <v>286</v>
       </c>
-      <c r="D3" s="264" t="s">
+      <c r="D3" s="268" t="s">
         <v>328</v>
       </c>
-      <c r="E3" s="264"/>
+      <c r="E3" s="268"/>
       <c r="F3" s="145">
         <v>75263586</v>
       </c>
       <c r="G3" s="145"/>
       <c r="H3" s="145"/>
-      <c r="I3" s="264" t="s">
+      <c r="I3" s="268" t="s">
         <v>332</v>
       </c>
-      <c r="J3" s="264"/>
-      <c r="K3" s="264"/>
-      <c r="L3" s="264"/>
-      <c r="M3" s="264"/>
-      <c r="N3" s="264"/>
-      <c r="O3" s="264"/>
-      <c r="P3" s="264"/>
-      <c r="Q3" s="264"/>
-      <c r="R3" s="274" t="s">
+      <c r="J3" s="268"/>
+      <c r="K3" s="268"/>
+      <c r="L3" s="268"/>
+      <c r="M3" s="268"/>
+      <c r="N3" s="268"/>
+      <c r="O3" s="268"/>
+      <c r="P3" s="268"/>
+      <c r="Q3" s="268"/>
+      <c r="R3" s="278" t="s">
         <v>334</v>
       </c>
-      <c r="S3" s="274"/>
-      <c r="T3" s="274"/>
-      <c r="U3" s="274"/>
-      <c r="V3" s="274"/>
-      <c r="W3" s="274"/>
-      <c r="X3" s="274"/>
+      <c r="S3" s="278"/>
+      <c r="T3" s="278"/>
+      <c r="U3" s="278"/>
+      <c r="V3" s="278"/>
+      <c r="W3" s="278"/>
+      <c r="X3" s="278"/>
       <c r="Y3" s="143"/>
       <c r="Z3" s="143"/>
       <c r="AA3" s="143"/>
@@ -4624,42 +4583,42 @@
       <c r="BD3" s="139"/>
     </row>
     <row r="4" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="235" t="s">
+      <c r="A4" s="239" t="s">
         <v>296</v>
       </c>
-      <c r="B4" s="236"/>
+      <c r="B4" s="240"/>
       <c r="C4" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D4" s="264" t="s">
+      <c r="D4" s="268" t="s">
         <v>329</v>
       </c>
-      <c r="E4" s="264"/>
+      <c r="E4" s="268"/>
       <c r="F4" s="145">
         <v>99826036</v>
       </c>
       <c r="G4" s="145"/>
       <c r="H4" s="145"/>
-      <c r="I4" s="264" t="s">
+      <c r="I4" s="268" t="s">
         <v>333</v>
       </c>
-      <c r="J4" s="264"/>
-      <c r="K4" s="264"/>
-      <c r="L4" s="264"/>
-      <c r="M4" s="264"/>
-      <c r="N4" s="264"/>
-      <c r="O4" s="264"/>
-      <c r="P4" s="264"/>
-      <c r="Q4" s="264"/>
-      <c r="R4" s="274" t="s">
+      <c r="J4" s="268"/>
+      <c r="K4" s="268"/>
+      <c r="L4" s="268"/>
+      <c r="M4" s="268"/>
+      <c r="N4" s="268"/>
+      <c r="O4" s="268"/>
+      <c r="P4" s="268"/>
+      <c r="Q4" s="268"/>
+      <c r="R4" s="278" t="s">
         <v>335</v>
       </c>
-      <c r="S4" s="274"/>
-      <c r="T4" s="274"/>
-      <c r="U4" s="274"/>
-      <c r="V4" s="274"/>
-      <c r="W4" s="274"/>
-      <c r="X4" s="274"/>
+      <c r="S4" s="278"/>
+      <c r="T4" s="278"/>
+      <c r="U4" s="278"/>
+      <c r="V4" s="278"/>
+      <c r="W4" s="278"/>
+      <c r="X4" s="278"/>
       <c r="Y4" s="143"/>
       <c r="Z4" s="143"/>
       <c r="AA4" s="143"/>
@@ -4694,35 +4653,35 @@
       <c r="BD4" s="139"/>
     </row>
     <row r="5" spans="1:56" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="237" t="s">
+      <c r="A5" s="241" t="s">
         <v>302</v>
       </c>
-      <c r="B5" s="238"/>
+      <c r="B5" s="242"/>
       <c r="C5" s="142" t="s">
         <v>288</v>
       </c>
-      <c r="D5" s="240" t="s">
+      <c r="D5" s="244" t="s">
         <v>330</v>
       </c>
-      <c r="E5" s="240"/>
-      <c r="F5" s="273" t="s">
+      <c r="E5" s="244"/>
+      <c r="F5" s="277" t="s">
         <v>331</v>
       </c>
-      <c r="G5" s="273"/>
-      <c r="H5" s="273"/>
-      <c r="I5" s="273"/>
-      <c r="J5" s="273"/>
-      <c r="K5" s="273"/>
-      <c r="L5" s="273"/>
-      <c r="M5" s="273"/>
-      <c r="N5" s="273"/>
-      <c r="O5" s="273"/>
-      <c r="P5" s="273"/>
-      <c r="Q5" s="273"/>
-      <c r="R5" s="273"/>
-      <c r="S5" s="273"/>
-      <c r="T5" s="273"/>
-      <c r="U5" s="273"/>
+      <c r="G5" s="277"/>
+      <c r="H5" s="277"/>
+      <c r="I5" s="277"/>
+      <c r="J5" s="277"/>
+      <c r="K5" s="277"/>
+      <c r="L5" s="277"/>
+      <c r="M5" s="277"/>
+      <c r="N5" s="277"/>
+      <c r="O5" s="277"/>
+      <c r="P5" s="277"/>
+      <c r="Q5" s="277"/>
+      <c r="R5" s="277"/>
+      <c r="S5" s="277"/>
+      <c r="T5" s="277"/>
+      <c r="U5" s="277"/>
       <c r="V5" s="144"/>
       <c r="W5" s="144"/>
       <c r="X5" s="144"/>
@@ -4760,101 +4719,101 @@
       <c r="BD5" s="140"/>
     </row>
     <row r="6" spans="1:56" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="244" t="s">
+      <c r="A6" s="248" t="s">
         <v>310</v>
       </c>
-      <c r="B6" s="246" t="s">
+      <c r="B6" s="250" t="s">
         <v>160</v>
       </c>
-      <c r="C6" s="246" t="s">
+      <c r="C6" s="250" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="246" t="s">
+      <c r="D6" s="250" t="s">
         <v>292</v>
       </c>
-      <c r="E6" s="253" t="s">
+      <c r="E6" s="257" t="s">
         <v>159</v>
       </c>
-      <c r="F6" s="254"/>
-      <c r="G6" s="251" t="s">
+      <c r="F6" s="258"/>
+      <c r="G6" s="255" t="s">
         <v>293</v>
       </c>
-      <c r="H6" s="241" t="s">
+      <c r="H6" s="245" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="242"/>
-      <c r="J6" s="242"/>
-      <c r="K6" s="242"/>
-      <c r="L6" s="242"/>
-      <c r="M6" s="242"/>
-      <c r="N6" s="243"/>
-      <c r="O6" s="241" t="s">
+      <c r="I6" s="246"/>
+      <c r="J6" s="246"/>
+      <c r="K6" s="246"/>
+      <c r="L6" s="246"/>
+      <c r="M6" s="246"/>
+      <c r="N6" s="247"/>
+      <c r="O6" s="245" t="s">
         <v>136</v>
       </c>
-      <c r="P6" s="242"/>
-      <c r="Q6" s="242"/>
-      <c r="R6" s="242"/>
-      <c r="S6" s="242"/>
-      <c r="T6" s="242"/>
-      <c r="U6" s="243"/>
-      <c r="V6" s="241" t="s">
+      <c r="P6" s="246"/>
+      <c r="Q6" s="246"/>
+      <c r="R6" s="246"/>
+      <c r="S6" s="246"/>
+      <c r="T6" s="246"/>
+      <c r="U6" s="247"/>
+      <c r="V6" s="245" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="242"/>
-      <c r="X6" s="242"/>
-      <c r="Y6" s="242"/>
-      <c r="Z6" s="242"/>
-      <c r="AA6" s="242"/>
-      <c r="AB6" s="243"/>
-      <c r="AC6" s="241" t="s">
+      <c r="W6" s="246"/>
+      <c r="X6" s="246"/>
+      <c r="Y6" s="246"/>
+      <c r="Z6" s="246"/>
+      <c r="AA6" s="246"/>
+      <c r="AB6" s="247"/>
+      <c r="AC6" s="245" t="s">
         <v>137</v>
       </c>
-      <c r="AD6" s="242"/>
-      <c r="AE6" s="242"/>
-      <c r="AF6" s="242"/>
-      <c r="AG6" s="242"/>
-      <c r="AH6" s="242"/>
-      <c r="AI6" s="243"/>
-      <c r="AJ6" s="241" t="s">
+      <c r="AD6" s="246"/>
+      <c r="AE6" s="246"/>
+      <c r="AF6" s="246"/>
+      <c r="AG6" s="246"/>
+      <c r="AH6" s="246"/>
+      <c r="AI6" s="247"/>
+      <c r="AJ6" s="245" t="s">
         <v>84</v>
       </c>
-      <c r="AK6" s="242"/>
-      <c r="AL6" s="242"/>
-      <c r="AM6" s="242"/>
-      <c r="AN6" s="242"/>
-      <c r="AO6" s="242"/>
-      <c r="AP6" s="243"/>
-      <c r="AQ6" s="241" t="s">
+      <c r="AK6" s="246"/>
+      <c r="AL6" s="246"/>
+      <c r="AM6" s="246"/>
+      <c r="AN6" s="246"/>
+      <c r="AO6" s="246"/>
+      <c r="AP6" s="247"/>
+      <c r="AQ6" s="245" t="s">
         <v>138</v>
       </c>
-      <c r="AR6" s="242"/>
-      <c r="AS6" s="242"/>
-      <c r="AT6" s="242"/>
-      <c r="AU6" s="242"/>
-      <c r="AV6" s="242"/>
-      <c r="AW6" s="243"/>
-      <c r="AX6" s="241" t="s">
+      <c r="AR6" s="246"/>
+      <c r="AS6" s="246"/>
+      <c r="AT6" s="246"/>
+      <c r="AU6" s="246"/>
+      <c r="AV6" s="246"/>
+      <c r="AW6" s="247"/>
+      <c r="AX6" s="245" t="s">
         <v>139</v>
       </c>
-      <c r="AY6" s="242"/>
-      <c r="AZ6" s="242"/>
-      <c r="BA6" s="242"/>
-      <c r="BB6" s="242"/>
-      <c r="BC6" s="242"/>
-      <c r="BD6" s="243"/>
+      <c r="AY6" s="246"/>
+      <c r="AZ6" s="246"/>
+      <c r="BA6" s="246"/>
+      <c r="BB6" s="246"/>
+      <c r="BC6" s="246"/>
+      <c r="BD6" s="247"/>
     </row>
     <row r="7" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="245"/>
-      <c r="B7" s="247"/>
-      <c r="C7" s="247"/>
-      <c r="D7" s="247"/>
+      <c r="A7" s="249"/>
+      <c r="B7" s="251"/>
+      <c r="C7" s="251"/>
+      <c r="D7" s="251"/>
       <c r="E7" s="154" t="s">
         <v>158</v>
       </c>
       <c r="F7" s="154" t="s">
         <v>309</v>
       </c>
-      <c r="G7" s="252"/>
+      <c r="G7" s="256"/>
       <c r="H7" s="155" t="s">
         <v>297</v>
       </c>
@@ -5128,7 +5087,7 @@
       <c r="BD9" s="89"/>
     </row>
     <row r="10" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="248" t="s">
+      <c r="A10" s="252" t="s">
         <v>311</v>
       </c>
       <c r="B10" s="135"/>
@@ -5196,7 +5155,7 @@
       <c r="BD10" s="89"/>
     </row>
     <row r="11" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="249"/>
+      <c r="A11" s="253"/>
       <c r="B11" s="135"/>
       <c r="C11" s="90" t="s">
         <v>291</v>
@@ -5262,7 +5221,7 @@
       <c r="BD11" s="89"/>
     </row>
     <row r="12" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="250"/>
+      <c r="A12" s="254"/>
       <c r="B12" s="135"/>
       <c r="C12" s="90" t="s">
         <v>89</v>
@@ -5452,7 +5411,7 @@
       <c r="BD14" s="89"/>
     </row>
     <row r="15" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="248" t="s">
+      <c r="A15" s="252" t="s">
         <v>312</v>
       </c>
       <c r="B15" s="135"/>
@@ -5522,7 +5481,7 @@
       <c r="BD15" s="89"/>
     </row>
     <row r="16" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="249"/>
+      <c r="A16" s="253"/>
       <c r="B16" s="135"/>
       <c r="C16" s="95" t="s">
         <v>104</v>
@@ -5590,7 +5549,7 @@
       <c r="BD16" s="89"/>
     </row>
     <row r="17" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="249"/>
+      <c r="A17" s="253"/>
       <c r="B17" s="135"/>
       <c r="C17" s="95" t="s">
         <v>105</v>
@@ -5658,7 +5617,7 @@
       <c r="BD17" s="89"/>
     </row>
     <row r="18" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="249"/>
+      <c r="A18" s="253"/>
       <c r="B18" s="135"/>
       <c r="C18" s="95" t="s">
         <v>106</v>
@@ -5726,7 +5685,7 @@
       <c r="BD18" s="89"/>
     </row>
     <row r="19" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="249"/>
+      <c r="A19" s="253"/>
       <c r="B19" s="135"/>
       <c r="C19" s="95" t="s">
         <v>99</v>
@@ -5794,7 +5753,7 @@
       <c r="BD19" s="89"/>
     </row>
     <row r="20" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="249"/>
+      <c r="A20" s="253"/>
       <c r="B20" s="135"/>
       <c r="C20" s="95" t="s">
         <v>107</v>
@@ -5862,7 +5821,7 @@
       <c r="BD20" s="89"/>
     </row>
     <row r="21" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="249"/>
+      <c r="A21" s="253"/>
       <c r="B21" s="135"/>
       <c r="C21" s="95" t="s">
         <v>108</v>
@@ -5930,7 +5889,7 @@
       <c r="BD21" s="89"/>
     </row>
     <row r="22" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="249"/>
+      <c r="A22" s="253"/>
       <c r="B22" s="135"/>
       <c r="C22" s="95" t="s">
         <v>109</v>
@@ -5998,7 +5957,7 @@
       <c r="BD22" s="89"/>
     </row>
     <row r="23" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="249"/>
+      <c r="A23" s="253"/>
       <c r="B23" s="135"/>
       <c r="C23" s="95" t="s">
         <v>110</v>
@@ -6066,7 +6025,7 @@
       <c r="BD23" s="89"/>
     </row>
     <row r="24" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="249"/>
+      <c r="A24" s="253"/>
       <c r="B24" s="135"/>
       <c r="C24" s="95" t="s">
         <v>111</v>
@@ -6134,7 +6093,7 @@
       <c r="BD24" s="89"/>
     </row>
     <row r="25" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="249"/>
+      <c r="A25" s="253"/>
       <c r="B25" s="135"/>
       <c r="C25" s="95" t="s">
         <v>112</v>
@@ -6202,7 +6161,7 @@
       <c r="BD25" s="89"/>
     </row>
     <row r="26" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="249"/>
+      <c r="A26" s="253"/>
       <c r="B26" s="135"/>
       <c r="C26" s="95" t="s">
         <v>113</v>
@@ -6270,7 +6229,7 @@
       <c r="BD26" s="89"/>
     </row>
     <row r="27" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="249"/>
+      <c r="A27" s="253"/>
       <c r="B27" s="135"/>
       <c r="C27" s="95" t="s">
         <v>114</v>
@@ -6338,7 +6297,7 @@
       <c r="BD27" s="89"/>
     </row>
     <row r="28" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="249"/>
+      <c r="A28" s="253"/>
       <c r="B28" s="135"/>
       <c r="C28" s="95" t="s">
         <v>115</v>
@@ -6406,7 +6365,7 @@
       <c r="BD28" s="89"/>
     </row>
     <row r="29" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="249"/>
+      <c r="A29" s="253"/>
       <c r="B29" s="135"/>
       <c r="C29" s="95" t="s">
         <v>116</v>
@@ -6474,7 +6433,7 @@
       <c r="BD29" s="89"/>
     </row>
     <row r="30" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="250"/>
+      <c r="A30" s="254"/>
       <c r="B30" s="135"/>
       <c r="C30" s="95" t="s">
         <v>117</v>
@@ -6604,7 +6563,7 @@
       <c r="BD31" s="89"/>
     </row>
     <row r="32" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="248" t="s">
+      <c r="A32" s="252" t="s">
         <v>313</v>
       </c>
       <c r="B32" s="135"/>
@@ -6672,7 +6631,7 @@
       <c r="BD32" s="89"/>
     </row>
     <row r="33" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="249"/>
+      <c r="A33" s="253"/>
       <c r="B33" s="135"/>
       <c r="C33" s="95" t="s">
         <v>105</v>
@@ -6738,7 +6697,7 @@
       <c r="BD33" s="89"/>
     </row>
     <row r="34" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="249"/>
+      <c r="A34" s="253"/>
       <c r="B34" s="135"/>
       <c r="C34" s="95" t="s">
         <v>108</v>
@@ -6804,7 +6763,7 @@
       <c r="BD34" s="89"/>
     </row>
     <row r="35" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="250"/>
+      <c r="A35" s="254"/>
       <c r="B35" s="135"/>
       <c r="C35" s="95" t="s">
         <v>91</v>
@@ -6932,7 +6891,7 @@
       <c r="BD36" s="89"/>
     </row>
     <row r="37" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="248" t="s">
+      <c r="A37" s="252" t="s">
         <v>314</v>
       </c>
       <c r="B37" s="136" t="s">
@@ -6996,7 +6955,7 @@
       <c r="BD37" s="89"/>
     </row>
     <row r="38" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="249"/>
+      <c r="A38" s="253"/>
       <c r="B38" s="137" t="s">
         <v>164</v>
       </c>
@@ -7064,7 +7023,7 @@
       <c r="BD38" s="89"/>
     </row>
     <row r="39" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="249"/>
+      <c r="A39" s="253"/>
       <c r="B39" s="137" t="s">
         <v>165</v>
       </c>
@@ -7132,7 +7091,7 @@
       <c r="BD39" s="89"/>
     </row>
     <row r="40" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="249"/>
+      <c r="A40" s="253"/>
       <c r="B40" s="136" t="s">
         <v>225</v>
       </c>
@@ -7194,7 +7153,7 @@
       <c r="BD40" s="89"/>
     </row>
     <row r="41" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="249"/>
+      <c r="A41" s="253"/>
       <c r="B41" s="137" t="s">
         <v>226</v>
       </c>
@@ -7262,7 +7221,7 @@
       <c r="BD41" s="89"/>
     </row>
     <row r="42" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="249"/>
+      <c r="A42" s="253"/>
       <c r="B42" s="136" t="s">
         <v>227</v>
       </c>
@@ -7324,7 +7283,7 @@
       <c r="BD42" s="89"/>
     </row>
     <row r="43" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="249"/>
+      <c r="A43" s="253"/>
       <c r="B43" s="137" t="s">
         <v>228</v>
       </c>
@@ -7388,7 +7347,7 @@
       <c r="BD43" s="89"/>
     </row>
     <row r="44" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="249"/>
+      <c r="A44" s="253"/>
       <c r="B44" s="135"/>
       <c r="C44" s="90" t="s">
         <v>174</v>
@@ -7454,7 +7413,7 @@
       <c r="BD44" s="89"/>
     </row>
     <row r="45" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="249"/>
+      <c r="A45" s="253"/>
       <c r="B45" s="135"/>
       <c r="C45" s="90" t="s">
         <v>173</v>
@@ -7520,7 +7479,7 @@
       <c r="BD45" s="89"/>
     </row>
     <row r="46" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="249"/>
+      <c r="A46" s="253"/>
       <c r="B46" s="136" t="s">
         <v>229</v>
       </c>
@@ -7582,7 +7541,7 @@
       <c r="BD46" s="89"/>
     </row>
     <row r="47" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="249"/>
+      <c r="A47" s="253"/>
       <c r="B47" s="137" t="s">
         <v>230</v>
       </c>
@@ -7650,7 +7609,7 @@
       <c r="BD47" s="89"/>
     </row>
     <row r="48" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="249"/>
+      <c r="A48" s="253"/>
       <c r="B48" s="137" t="s">
         <v>231</v>
       </c>
@@ -7718,7 +7677,7 @@
       <c r="BD48" s="89"/>
     </row>
     <row r="49" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="249"/>
+      <c r="A49" s="253"/>
       <c r="B49" s="137" t="s">
         <v>232</v>
       </c>
@@ -7786,7 +7745,7 @@
       <c r="BD49" s="89"/>
     </row>
     <row r="50" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="249"/>
+      <c r="A50" s="253"/>
       <c r="B50" s="137" t="s">
         <v>233</v>
       </c>
@@ -7854,7 +7813,7 @@
       <c r="BD50" s="89"/>
     </row>
     <row r="51" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="249"/>
+      <c r="A51" s="253"/>
       <c r="B51" s="136" t="s">
         <v>234</v>
       </c>
@@ -7916,7 +7875,7 @@
       <c r="BD51" s="89"/>
     </row>
     <row r="52" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="249"/>
+      <c r="A52" s="253"/>
       <c r="B52" s="137" t="s">
         <v>235</v>
       </c>
@@ -7984,7 +7943,7 @@
       <c r="BD52" s="89"/>
     </row>
     <row r="53" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="249"/>
+      <c r="A53" s="253"/>
       <c r="B53" s="137" t="s">
         <v>236</v>
       </c>
@@ -8052,7 +8011,7 @@
       <c r="BD53" s="89"/>
     </row>
     <row r="54" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="249"/>
+      <c r="A54" s="253"/>
       <c r="B54" s="136" t="s">
         <v>237</v>
       </c>
@@ -8114,7 +8073,7 @@
       <c r="BD54" s="89"/>
     </row>
     <row r="55" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="249"/>
+      <c r="A55" s="253"/>
       <c r="B55" s="137" t="s">
         <v>238</v>
       </c>
@@ -8180,7 +8139,7 @@
       <c r="BD55" s="89"/>
     </row>
     <row r="56" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="249"/>
+      <c r="A56" s="253"/>
       <c r="B56" s="135"/>
       <c r="C56" s="90" t="s">
         <v>183</v>
@@ -8248,7 +8207,7 @@
       <c r="BD56" s="89"/>
     </row>
     <row r="57" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="249"/>
+      <c r="A57" s="253"/>
       <c r="B57" s="135"/>
       <c r="C57" s="90" t="s">
         <v>182</v>
@@ -8316,7 +8275,7 @@
       <c r="BD57" s="89"/>
     </row>
     <row r="58" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="249"/>
+      <c r="A58" s="253"/>
       <c r="B58" s="137" t="s">
         <v>239</v>
       </c>
@@ -8382,7 +8341,7 @@
       <c r="BD58" s="89"/>
     </row>
     <row r="59" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="249"/>
+      <c r="A59" s="253"/>
       <c r="B59" s="135"/>
       <c r="C59" s="90" t="s">
         <v>282</v>
@@ -8450,7 +8409,7 @@
       <c r="BD59" s="89"/>
     </row>
     <row r="60" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="249"/>
+      <c r="A60" s="253"/>
       <c r="B60" s="135"/>
       <c r="C60" s="90" t="s">
         <v>283</v>
@@ -8518,7 +8477,7 @@
       <c r="BD60" s="89"/>
     </row>
     <row r="61" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="249"/>
+      <c r="A61" s="253"/>
       <c r="B61" s="136" t="s">
         <v>240</v>
       </c>
@@ -8580,7 +8539,7 @@
       <c r="BD61" s="89"/>
     </row>
     <row r="62" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="249"/>
+      <c r="A62" s="253"/>
       <c r="B62" s="137" t="s">
         <v>241</v>
       </c>
@@ -8648,7 +8607,7 @@
       <c r="BD62" s="89"/>
     </row>
     <row r="63" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="249"/>
+      <c r="A63" s="253"/>
       <c r="B63" s="137" t="s">
         <v>242</v>
       </c>
@@ -8716,7 +8675,7 @@
       <c r="BD63" s="89"/>
     </row>
     <row r="64" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="249"/>
+      <c r="A64" s="253"/>
       <c r="B64" s="136" t="s">
         <v>243</v>
       </c>
@@ -8778,7 +8737,7 @@
       <c r="BD64" s="89"/>
     </row>
     <row r="65" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="249"/>
+      <c r="A65" s="253"/>
       <c r="B65" s="137" t="s">
         <v>244</v>
       </c>
@@ -8846,7 +8805,7 @@
       <c r="BD65" s="89"/>
     </row>
     <row r="66" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="249"/>
+      <c r="A66" s="253"/>
       <c r="B66" s="136" t="s">
         <v>247</v>
       </c>
@@ -8908,7 +8867,7 @@
       <c r="BD66" s="89"/>
     </row>
     <row r="67" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="249"/>
+      <c r="A67" s="253"/>
       <c r="B67" s="137" t="s">
         <v>248</v>
       </c>
@@ -8976,7 +8935,7 @@
       <c r="BD67" s="89"/>
     </row>
     <row r="68" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="249"/>
+      <c r="A68" s="253"/>
       <c r="B68" s="136" t="s">
         <v>251</v>
       </c>
@@ -9038,7 +8997,7 @@
       <c r="BD68" s="89"/>
     </row>
     <row r="69" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="249"/>
+      <c r="A69" s="253"/>
       <c r="B69" s="137" t="s">
         <v>252</v>
       </c>
@@ -9106,7 +9065,7 @@
       <c r="BD69" s="89"/>
     </row>
     <row r="70" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="249"/>
+      <c r="A70" s="253"/>
       <c r="B70" s="137" t="s">
         <v>253</v>
       </c>
@@ -9174,7 +9133,7 @@
       <c r="BD70" s="89"/>
     </row>
     <row r="71" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="249"/>
+      <c r="A71" s="253"/>
       <c r="B71" s="136" t="s">
         <v>254</v>
       </c>
@@ -9236,7 +9195,7 @@
       <c r="BD71" s="89"/>
     </row>
     <row r="72" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="249"/>
+      <c r="A72" s="253"/>
       <c r="B72" s="137" t="s">
         <v>255</v>
       </c>
@@ -9304,7 +9263,7 @@
       <c r="BD72" s="89"/>
     </row>
     <row r="73" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="249"/>
+      <c r="A73" s="253"/>
       <c r="B73" s="136" t="s">
         <v>256</v>
       </c>
@@ -9366,7 +9325,7 @@
       <c r="BD73" s="89"/>
     </row>
     <row r="74" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="250"/>
+      <c r="A74" s="254"/>
       <c r="B74" s="137" t="s">
         <v>257</v>
       </c>
@@ -9558,7 +9517,7 @@
       <c r="BD76" s="89"/>
     </row>
     <row r="77" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="248" t="s">
+      <c r="A77" s="252" t="s">
         <v>162</v>
       </c>
       <c r="B77" s="135"/>
@@ -9626,7 +9585,7 @@
       <c r="BD77" s="89"/>
     </row>
     <row r="78" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="250"/>
+      <c r="A78" s="254"/>
       <c r="B78" s="135"/>
       <c r="C78" s="90" t="s">
         <v>95</v>
@@ -9754,7 +9713,7 @@
       <c r="BD79" s="89"/>
     </row>
     <row r="80" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="248" t="s">
+      <c r="A80" s="252" t="s">
         <v>162</v>
       </c>
       <c r="B80" s="135"/>
@@ -9822,7 +9781,7 @@
       <c r="BD80" s="89"/>
     </row>
     <row r="81" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="250"/>
+      <c r="A81" s="254"/>
       <c r="B81" s="135"/>
       <c r="C81" s="90" t="s">
         <v>93</v>
@@ -9950,7 +9909,7 @@
       <c r="BD82" s="89"/>
     </row>
     <row r="83" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="248" t="s">
+      <c r="A83" s="252" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="135"/>
@@ -10018,7 +9977,7 @@
       <c r="BD83" s="89"/>
     </row>
     <row r="84" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="250"/>
+      <c r="A84" s="254"/>
       <c r="B84" s="135"/>
       <c r="C84" s="90" t="s">
         <v>134</v>
@@ -10208,7 +10167,7 @@
       <c r="BD86" s="89"/>
     </row>
     <row r="87" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="248" t="s">
+      <c r="A87" s="252" t="s">
         <v>316</v>
       </c>
       <c r="B87" s="135"/>
@@ -10276,7 +10235,7 @@
       <c r="BD87" s="89"/>
     </row>
     <row r="88" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="249"/>
+      <c r="A88" s="253"/>
       <c r="B88" s="135"/>
       <c r="C88" s="95" t="s">
         <v>119</v>
@@ -10342,7 +10301,7 @@
       <c r="BD88" s="89"/>
     </row>
     <row r="89" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="249"/>
+      <c r="A89" s="253"/>
       <c r="B89" s="135"/>
       <c r="C89" s="95" t="s">
         <v>120</v>
@@ -10408,7 +10367,7 @@
       <c r="BD89" s="89"/>
     </row>
     <row r="90" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="249"/>
+      <c r="A90" s="253"/>
       <c r="B90" s="135"/>
       <c r="C90" s="95" t="s">
         <v>121</v>
@@ -10474,7 +10433,7 @@
       <c r="BD90" s="89"/>
     </row>
     <row r="91" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="249"/>
+      <c r="A91" s="253"/>
       <c r="B91" s="135"/>
       <c r="C91" s="95" t="s">
         <v>122</v>
@@ -10540,7 +10499,7 @@
       <c r="BD91" s="89"/>
     </row>
     <row r="92" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="249"/>
+      <c r="A92" s="253"/>
       <c r="B92" s="135"/>
       <c r="C92" s="95" t="s">
         <v>123</v>
@@ -10606,7 +10565,7 @@
       <c r="BD92" s="89"/>
     </row>
     <row r="93" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="249"/>
+      <c r="A93" s="253"/>
       <c r="B93" s="135"/>
       <c r="C93" s="95" t="s">
         <v>124</v>
@@ -10672,7 +10631,7 @@
       <c r="BD93" s="89"/>
     </row>
     <row r="94" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="249"/>
+      <c r="A94" s="253"/>
       <c r="B94" s="135"/>
       <c r="C94" s="95" t="s">
         <v>125</v>
@@ -10738,7 +10697,7 @@
       <c r="BD94" s="89"/>
     </row>
     <row r="95" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="249"/>
+      <c r="A95" s="253"/>
       <c r="B95" s="135"/>
       <c r="C95" s="95" t="s">
         <v>126</v>
@@ -10804,7 +10763,7 @@
       <c r="BD95" s="89"/>
     </row>
     <row r="96" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="249"/>
+      <c r="A96" s="253"/>
       <c r="B96" s="135"/>
       <c r="C96" s="95" t="s">
         <v>127</v>
@@ -10870,7 +10829,7 @@
       <c r="BD96" s="89"/>
     </row>
     <row r="97" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="249"/>
+      <c r="A97" s="253"/>
       <c r="B97" s="135"/>
       <c r="C97" s="95" t="s">
         <v>128</v>
@@ -10936,7 +10895,7 @@
       <c r="BD97" s="89"/>
     </row>
     <row r="98" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="249"/>
+      <c r="A98" s="253"/>
       <c r="B98" s="135"/>
       <c r="C98" s="95" t="s">
         <v>129</v>
@@ -11002,7 +10961,7 @@
       <c r="BD98" s="89"/>
     </row>
     <row r="99" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="249"/>
+      <c r="A99" s="253"/>
       <c r="B99" s="135"/>
       <c r="C99" s="95" t="s">
         <v>130</v>
@@ -11068,7 +11027,7 @@
       <c r="BD99" s="89"/>
     </row>
     <row r="100" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="249"/>
+      <c r="A100" s="253"/>
       <c r="B100" s="135"/>
       <c r="C100" s="95" t="s">
         <v>131</v>
@@ -11134,7 +11093,7 @@
       <c r="BD100" s="89"/>
     </row>
     <row r="101" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="249"/>
+      <c r="A101" s="253"/>
       <c r="B101" s="135"/>
       <c r="C101" s="95" t="s">
         <v>132</v>
@@ -11200,7 +11159,7 @@
       <c r="BD101" s="89"/>
     </row>
     <row r="102" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="250"/>
+      <c r="A102" s="254"/>
       <c r="B102" s="135"/>
       <c r="C102" s="95" t="s">
         <v>133</v>
@@ -11328,7 +11287,7 @@
       <c r="BD103" s="89"/>
     </row>
     <row r="104" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="248" t="s">
+      <c r="A104" s="252" t="s">
         <v>315</v>
       </c>
       <c r="B104" s="136" t="s">
@@ -11392,7 +11351,7 @@
       <c r="BD104" s="89"/>
     </row>
     <row r="105" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="249"/>
+      <c r="A105" s="253"/>
       <c r="B105" s="137">
         <v>3.0101010000000001</v>
       </c>
@@ -11460,7 +11419,7 @@
       <c r="BD105" s="89"/>
     </row>
     <row r="106" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="249"/>
+      <c r="A106" s="253"/>
       <c r="B106" s="136" t="s">
         <v>224</v>
       </c>
@@ -11522,7 +11481,7 @@
       <c r="BD106" s="89"/>
     </row>
     <row r="107" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="249"/>
+      <c r="A107" s="253"/>
       <c r="B107" s="137" t="s">
         <v>164</v>
       </c>
@@ -11590,7 +11549,7 @@
       <c r="BD107" s="89"/>
     </row>
     <row r="108" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="249"/>
+      <c r="A108" s="253"/>
       <c r="B108" s="137" t="s">
         <v>165</v>
       </c>
@@ -11658,7 +11617,7 @@
       <c r="BD108" s="89"/>
     </row>
     <row r="109" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="249"/>
+      <c r="A109" s="253"/>
       <c r="B109" s="136" t="s">
         <v>225</v>
       </c>
@@ -11720,7 +11679,7 @@
       <c r="BD109" s="89"/>
     </row>
     <row r="110" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="249"/>
+      <c r="A110" s="253"/>
       <c r="B110" s="137" t="s">
         <v>226</v>
       </c>
@@ -11788,7 +11747,7 @@
       <c r="BD110" s="89"/>
     </row>
     <row r="111" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="249"/>
+      <c r="A111" s="253"/>
       <c r="B111" s="136" t="s">
         <v>227</v>
       </c>
@@ -11850,7 +11809,7 @@
       <c r="BD111" s="89"/>
     </row>
     <row r="112" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="249"/>
+      <c r="A112" s="253"/>
       <c r="B112" s="137" t="s">
         <v>228</v>
       </c>
@@ -11918,7 +11877,7 @@
       <c r="BD112" s="89"/>
     </row>
     <row r="113" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="249"/>
+      <c r="A113" s="253"/>
       <c r="B113" s="135"/>
       <c r="C113" s="90" t="s">
         <v>174</v>
@@ -11984,7 +11943,7 @@
       <c r="BD113" s="89"/>
     </row>
     <row r="114" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="249"/>
+      <c r="A114" s="253"/>
       <c r="B114" s="135"/>
       <c r="C114" s="90" t="s">
         <v>173</v>
@@ -12050,7 +12009,7 @@
       <c r="BD114" s="89"/>
     </row>
     <row r="115" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="249"/>
+      <c r="A115" s="253"/>
       <c r="B115" s="136" t="s">
         <v>229</v>
       </c>
@@ -12112,7 +12071,7 @@
       <c r="BD115" s="89"/>
     </row>
     <row r="116" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="249"/>
+      <c r="A116" s="253"/>
       <c r="B116" s="137" t="s">
         <v>230</v>
       </c>
@@ -12180,7 +12139,7 @@
       <c r="BD116" s="89"/>
     </row>
     <row r="117" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="249"/>
+      <c r="A117" s="253"/>
       <c r="B117" s="137" t="s">
         <v>231</v>
       </c>
@@ -12248,7 +12207,7 @@
       <c r="BD117" s="89"/>
     </row>
     <row r="118" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="249"/>
+      <c r="A118" s="253"/>
       <c r="B118" s="137" t="s">
         <v>232</v>
       </c>
@@ -12316,7 +12275,7 @@
       <c r="BD118" s="89"/>
     </row>
     <row r="119" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="249"/>
+      <c r="A119" s="253"/>
       <c r="B119" s="137" t="s">
         <v>233</v>
       </c>
@@ -12384,7 +12343,7 @@
       <c r="BD119" s="89"/>
     </row>
     <row r="120" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="249"/>
+      <c r="A120" s="253"/>
       <c r="B120" s="136" t="s">
         <v>234</v>
       </c>
@@ -12446,7 +12405,7 @@
       <c r="BD120" s="89"/>
     </row>
     <row r="121" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="249"/>
+      <c r="A121" s="253"/>
       <c r="B121" s="137" t="s">
         <v>235</v>
       </c>
@@ -12514,7 +12473,7 @@
       <c r="BD121" s="89"/>
     </row>
     <row r="122" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="249"/>
+      <c r="A122" s="253"/>
       <c r="B122" s="137" t="s">
         <v>236</v>
       </c>
@@ -12582,7 +12541,7 @@
       <c r="BD122" s="89"/>
     </row>
     <row r="123" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="249"/>
+      <c r="A123" s="253"/>
       <c r="B123" s="136" t="s">
         <v>237</v>
       </c>
@@ -12644,7 +12603,7 @@
       <c r="BD123" s="89"/>
     </row>
     <row r="124" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="249"/>
+      <c r="A124" s="253"/>
       <c r="B124" s="137" t="s">
         <v>238</v>
       </c>
@@ -12708,7 +12667,7 @@
       <c r="BD124" s="89"/>
     </row>
     <row r="125" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="249"/>
+      <c r="A125" s="253"/>
       <c r="B125" s="135"/>
       <c r="C125" s="90" t="s">
         <v>183</v>
@@ -12774,7 +12733,7 @@
       <c r="BD125" s="89"/>
     </row>
     <row r="126" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="249"/>
+      <c r="A126" s="253"/>
       <c r="B126" s="135"/>
       <c r="C126" s="90" t="s">
         <v>182</v>
@@ -12840,7 +12799,7 @@
       <c r="BD126" s="89"/>
     </row>
     <row r="127" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="249"/>
+      <c r="A127" s="253"/>
       <c r="B127" s="137" t="s">
         <v>239</v>
       </c>
@@ -12904,7 +12863,7 @@
       <c r="BD127" s="89"/>
     </row>
     <row r="128" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="249"/>
+      <c r="A128" s="253"/>
       <c r="B128" s="135"/>
       <c r="C128" s="90" t="s">
         <v>282</v>
@@ -12970,7 +12929,7 @@
       <c r="BD128" s="89"/>
     </row>
     <row r="129" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="249"/>
+      <c r="A129" s="253"/>
       <c r="B129" s="135"/>
       <c r="C129" s="90" t="s">
         <v>283</v>
@@ -13036,7 +12995,7 @@
       <c r="BD129" s="89"/>
     </row>
     <row r="130" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="249"/>
+      <c r="A130" s="253"/>
       <c r="B130" s="136" t="s">
         <v>240</v>
       </c>
@@ -13098,7 +13057,7 @@
       <c r="BD130" s="89"/>
     </row>
     <row r="131" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="249"/>
+      <c r="A131" s="253"/>
       <c r="B131" s="137" t="s">
         <v>241</v>
       </c>
@@ -13166,7 +13125,7 @@
       <c r="BD131" s="89"/>
     </row>
     <row r="132" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="249"/>
+      <c r="A132" s="253"/>
       <c r="B132" s="137" t="s">
         <v>242</v>
       </c>
@@ -13234,7 +13193,7 @@
       <c r="BD132" s="89"/>
     </row>
     <row r="133" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="249"/>
+      <c r="A133" s="253"/>
       <c r="B133" s="136" t="s">
         <v>243</v>
       </c>
@@ -13296,7 +13255,7 @@
       <c r="BD133" s="89"/>
     </row>
     <row r="134" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="249"/>
+      <c r="A134" s="253"/>
       <c r="B134" s="137" t="s">
         <v>244</v>
       </c>
@@ -13364,7 +13323,7 @@
       <c r="BD134" s="89"/>
     </row>
     <row r="135" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="249"/>
+      <c r="A135" s="253"/>
       <c r="B135" s="136" t="s">
         <v>247</v>
       </c>
@@ -13426,7 +13385,7 @@
       <c r="BD135" s="89"/>
     </row>
     <row r="136" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="249"/>
+      <c r="A136" s="253"/>
       <c r="B136" s="137" t="s">
         <v>248</v>
       </c>
@@ -13494,7 +13453,7 @@
       <c r="BD136" s="89"/>
     </row>
     <row r="137" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="249"/>
+      <c r="A137" s="253"/>
       <c r="B137" s="136" t="s">
         <v>249</v>
       </c>
@@ -13556,7 +13515,7 @@
       <c r="BD137" s="89"/>
     </row>
     <row r="138" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="249"/>
+      <c r="A138" s="253"/>
       <c r="B138" s="137" t="s">
         <v>250</v>
       </c>
@@ -13624,7 +13583,7 @@
       <c r="BD138" s="89"/>
     </row>
     <row r="139" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="249"/>
+      <c r="A139" s="253"/>
       <c r="B139" s="136" t="s">
         <v>251</v>
       </c>
@@ -13686,7 +13645,7 @@
       <c r="BD139" s="89"/>
     </row>
     <row r="140" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="249"/>
+      <c r="A140" s="253"/>
       <c r="B140" s="137" t="s">
         <v>252</v>
       </c>
@@ -13754,7 +13713,7 @@
       <c r="BD140" s="89"/>
     </row>
     <row r="141" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="249"/>
+      <c r="A141" s="253"/>
       <c r="B141" s="137" t="s">
         <v>253</v>
       </c>
@@ -13822,7 +13781,7 @@
       <c r="BD141" s="89"/>
     </row>
     <row r="142" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="249"/>
+      <c r="A142" s="253"/>
       <c r="B142" s="136" t="s">
         <v>254</v>
       </c>
@@ -13884,7 +13843,7 @@
       <c r="BD142" s="89"/>
     </row>
     <row r="143" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="249"/>
+      <c r="A143" s="253"/>
       <c r="B143" s="137" t="s">
         <v>255</v>
       </c>
@@ -13952,7 +13911,7 @@
       <c r="BD143" s="89"/>
     </row>
     <row r="144" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="249"/>
+      <c r="A144" s="253"/>
       <c r="B144" s="136" t="s">
         <v>256</v>
       </c>
@@ -14014,7 +13973,7 @@
       <c r="BD144" s="89"/>
     </row>
     <row r="145" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="249"/>
+      <c r="A145" s="253"/>
       <c r="B145" s="137" t="s">
         <v>257</v>
       </c>
@@ -14082,7 +14041,7 @@
       <c r="BD145" s="89"/>
     </row>
     <row r="146" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="249"/>
+      <c r="A146" s="253"/>
       <c r="B146" s="136" t="s">
         <v>258</v>
       </c>
@@ -14144,7 +14103,7 @@
       <c r="BD146" s="89"/>
     </row>
     <row r="147" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="249"/>
+      <c r="A147" s="253"/>
       <c r="B147" s="137" t="s">
         <v>259</v>
       </c>
@@ -14212,7 +14171,7 @@
       <c r="BD147" s="89"/>
     </row>
     <row r="148" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="249"/>
+      <c r="A148" s="253"/>
       <c r="B148" s="136" t="s">
         <v>260</v>
       </c>
@@ -14274,7 +14233,7 @@
       <c r="BD148" s="89"/>
     </row>
     <row r="149" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="249"/>
+      <c r="A149" s="253"/>
       <c r="B149" s="137" t="s">
         <v>261</v>
       </c>
@@ -14342,7 +14301,7 @@
       <c r="BD149" s="89"/>
     </row>
     <row r="150" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="249"/>
+      <c r="A150" s="253"/>
       <c r="B150" s="137" t="s">
         <v>262</v>
       </c>
@@ -14410,7 +14369,7 @@
       <c r="BD150" s="89"/>
     </row>
     <row r="151" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="249"/>
+      <c r="A151" s="253"/>
       <c r="B151" s="137" t="s">
         <v>263</v>
       </c>
@@ -14478,7 +14437,7 @@
       <c r="BD151" s="89"/>
     </row>
     <row r="152" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="249"/>
+      <c r="A152" s="253"/>
       <c r="B152" s="137" t="s">
         <v>264</v>
       </c>
@@ -14546,7 +14505,7 @@
       <c r="BD152" s="89"/>
     </row>
     <row r="153" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="249"/>
+      <c r="A153" s="253"/>
       <c r="B153" s="136" t="s">
         <v>265</v>
       </c>
@@ -14608,7 +14567,7 @@
       <c r="BD153" s="89"/>
     </row>
     <row r="154" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="249"/>
+      <c r="A154" s="253"/>
       <c r="B154" s="137" t="s">
         <v>266</v>
       </c>
@@ -14676,7 +14635,7 @@
       <c r="BD154" s="89"/>
     </row>
     <row r="155" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="249"/>
+      <c r="A155" s="253"/>
       <c r="B155" s="137" t="s">
         <v>267</v>
       </c>
@@ -14744,7 +14703,7 @@
       <c r="BD155" s="89"/>
     </row>
     <row r="156" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="249"/>
+      <c r="A156" s="253"/>
       <c r="B156" s="136" t="s">
         <v>268</v>
       </c>
@@ -14806,7 +14765,7 @@
       <c r="BD156" s="89"/>
     </row>
     <row r="157" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="249"/>
+      <c r="A157" s="253"/>
       <c r="B157" s="137" t="s">
         <v>269</v>
       </c>
@@ -14874,7 +14833,7 @@
       <c r="BD157" s="89"/>
     </row>
     <row r="158" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="249"/>
+      <c r="A158" s="253"/>
       <c r="B158" s="137" t="s">
         <v>270</v>
       </c>
@@ -14942,7 +14901,7 @@
       <c r="BD158" s="89"/>
     </row>
     <row r="159" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="249"/>
+      <c r="A159" s="253"/>
       <c r="B159" s="137" t="s">
         <v>271</v>
       </c>
@@ -15010,7 +14969,7 @@
       <c r="BD159" s="89"/>
     </row>
     <row r="160" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="249"/>
+      <c r="A160" s="253"/>
       <c r="B160" s="137" t="s">
         <v>272</v>
       </c>
@@ -15078,7 +15037,7 @@
       <c r="BD160" s="89"/>
     </row>
     <row r="161" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="249"/>
+      <c r="A161" s="253"/>
       <c r="B161" s="136" t="s">
         <v>273</v>
       </c>
@@ -15140,7 +15099,7 @@
       <c r="BD161" s="89"/>
     </row>
     <row r="162" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="249"/>
+      <c r="A162" s="253"/>
       <c r="B162" s="137" t="s">
         <v>274</v>
       </c>
@@ -15208,7 +15167,7 @@
       <c r="BD162" s="89"/>
     </row>
     <row r="163" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="249"/>
+      <c r="A163" s="253"/>
       <c r="B163" s="137" t="s">
         <v>275</v>
       </c>
@@ -15276,7 +15235,7 @@
       <c r="BD163" s="89"/>
     </row>
     <row r="164" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="249"/>
+      <c r="A164" s="253"/>
       <c r="B164" s="136" t="s">
         <v>276</v>
       </c>
@@ -15338,7 +15297,7 @@
       <c r="BD164" s="89"/>
     </row>
     <row r="165" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="249"/>
+      <c r="A165" s="253"/>
       <c r="B165" s="137" t="s">
         <v>277</v>
       </c>
@@ -15406,7 +15365,7 @@
       <c r="BD165" s="89"/>
     </row>
     <row r="166" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="249"/>
+      <c r="A166" s="253"/>
       <c r="B166" s="137" t="s">
         <v>278</v>
       </c>
@@ -15474,7 +15433,7 @@
       <c r="BD166" s="89"/>
     </row>
     <row r="167" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="249"/>
+      <c r="A167" s="253"/>
       <c r="B167" s="136" t="s">
         <v>279</v>
       </c>
@@ -15536,7 +15495,7 @@
       <c r="BD167" s="89"/>
     </row>
     <row r="168" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="255"/>
+      <c r="A168" s="259"/>
       <c r="B168" s="138" t="s">
         <v>280</v>
       </c>
@@ -15676,74 +15635,74 @@
         <f>SUM(K170:BD170)</f>
         <v>3500</v>
       </c>
-      <c r="E170" s="270" t="s">
+      <c r="E170" s="274" t="s">
         <v>321</v>
       </c>
-      <c r="F170" s="270"/>
-      <c r="G170" s="270"/>
-      <c r="H170" s="262"/>
-      <c r="I170" s="260"/>
-      <c r="J170" s="260"/>
-      <c r="K170" s="260">
+      <c r="F170" s="274"/>
+      <c r="G170" s="274"/>
+      <c r="H170" s="266"/>
+      <c r="I170" s="264"/>
+      <c r="J170" s="264"/>
+      <c r="K170" s="264">
         <v>500</v>
       </c>
-      <c r="L170" s="260"/>
-      <c r="M170" s="260"/>
-      <c r="N170" s="261"/>
-      <c r="O170" s="262"/>
-      <c r="P170" s="260"/>
-      <c r="Q170" s="260"/>
-      <c r="R170" s="260">
+      <c r="L170" s="264"/>
+      <c r="M170" s="264"/>
+      <c r="N170" s="265"/>
+      <c r="O170" s="266"/>
+      <c r="P170" s="264"/>
+      <c r="Q170" s="264"/>
+      <c r="R170" s="264">
         <v>500</v>
       </c>
-      <c r="S170" s="260"/>
-      <c r="T170" s="260"/>
-      <c r="U170" s="261"/>
-      <c r="V170" s="262"/>
-      <c r="W170" s="260"/>
-      <c r="X170" s="260"/>
-      <c r="Y170" s="260">
+      <c r="S170" s="264"/>
+      <c r="T170" s="264"/>
+      <c r="U170" s="265"/>
+      <c r="V170" s="266"/>
+      <c r="W170" s="264"/>
+      <c r="X170" s="264"/>
+      <c r="Y170" s="264">
         <v>500</v>
       </c>
-      <c r="Z170" s="260"/>
-      <c r="AA170" s="260"/>
-      <c r="AB170" s="261"/>
-      <c r="AC170" s="262"/>
-      <c r="AD170" s="260"/>
-      <c r="AE170" s="260"/>
-      <c r="AF170" s="260">
+      <c r="Z170" s="264"/>
+      <c r="AA170" s="264"/>
+      <c r="AB170" s="265"/>
+      <c r="AC170" s="266"/>
+      <c r="AD170" s="264"/>
+      <c r="AE170" s="264"/>
+      <c r="AF170" s="264">
         <v>500</v>
       </c>
-      <c r="AG170" s="260"/>
-      <c r="AH170" s="260"/>
-      <c r="AI170" s="261"/>
-      <c r="AJ170" s="262"/>
-      <c r="AK170" s="260"/>
-      <c r="AL170" s="260"/>
-      <c r="AM170" s="260">
+      <c r="AG170" s="264"/>
+      <c r="AH170" s="264"/>
+      <c r="AI170" s="265"/>
+      <c r="AJ170" s="266"/>
+      <c r="AK170" s="264"/>
+      <c r="AL170" s="264"/>
+      <c r="AM170" s="264">
         <v>500</v>
       </c>
-      <c r="AN170" s="260"/>
-      <c r="AO170" s="260"/>
-      <c r="AP170" s="261"/>
-      <c r="AQ170" s="262"/>
-      <c r="AR170" s="260"/>
-      <c r="AS170" s="260"/>
-      <c r="AT170" s="260">
+      <c r="AN170" s="264"/>
+      <c r="AO170" s="264"/>
+      <c r="AP170" s="265"/>
+      <c r="AQ170" s="266"/>
+      <c r="AR170" s="264"/>
+      <c r="AS170" s="264"/>
+      <c r="AT170" s="264">
         <v>500</v>
       </c>
-      <c r="AU170" s="260"/>
-      <c r="AV170" s="260"/>
-      <c r="AW170" s="261"/>
-      <c r="AX170" s="262"/>
-      <c r="AY170" s="260"/>
-      <c r="AZ170" s="260"/>
-      <c r="BA170" s="260">
+      <c r="AU170" s="264"/>
+      <c r="AV170" s="264"/>
+      <c r="AW170" s="265"/>
+      <c r="AX170" s="266"/>
+      <c r="AY170" s="264"/>
+      <c r="AZ170" s="264"/>
+      <c r="BA170" s="264">
         <v>500</v>
       </c>
-      <c r="BB170" s="260"/>
-      <c r="BC170" s="260"/>
-      <c r="BD170" s="261"/>
+      <c r="BB170" s="264"/>
+      <c r="BC170" s="264"/>
+      <c r="BD170" s="265"/>
     </row>
     <row r="171" spans="1:56" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A171" s="150"/>
@@ -15755,74 +15714,74 @@
         <f>SUM(K171:BD171)</f>
         <v>4410</v>
       </c>
-      <c r="E171" s="270" t="s">
+      <c r="E171" s="274" t="s">
         <v>320</v>
       </c>
-      <c r="F171" s="270"/>
-      <c r="G171" s="270"/>
-      <c r="H171" s="262"/>
-      <c r="I171" s="260"/>
-      <c r="J171" s="260"/>
-      <c r="K171" s="260">
+      <c r="F171" s="274"/>
+      <c r="G171" s="274"/>
+      <c r="H171" s="266"/>
+      <c r="I171" s="264"/>
+      <c r="J171" s="264"/>
+      <c r="K171" s="264">
         <v>630</v>
       </c>
-      <c r="L171" s="260"/>
-      <c r="M171" s="260"/>
-      <c r="N171" s="261"/>
-      <c r="O171" s="262"/>
-      <c r="P171" s="260"/>
-      <c r="Q171" s="260"/>
-      <c r="R171" s="260">
+      <c r="L171" s="264"/>
+      <c r="M171" s="264"/>
+      <c r="N171" s="265"/>
+      <c r="O171" s="266"/>
+      <c r="P171" s="264"/>
+      <c r="Q171" s="264"/>
+      <c r="R171" s="264">
         <v>630</v>
       </c>
-      <c r="S171" s="260"/>
-      <c r="T171" s="260"/>
-      <c r="U171" s="261"/>
-      <c r="V171" s="262"/>
-      <c r="W171" s="260"/>
-      <c r="X171" s="260"/>
-      <c r="Y171" s="260">
+      <c r="S171" s="264"/>
+      <c r="T171" s="264"/>
+      <c r="U171" s="265"/>
+      <c r="V171" s="266"/>
+      <c r="W171" s="264"/>
+      <c r="X171" s="264"/>
+      <c r="Y171" s="264">
         <v>630</v>
       </c>
-      <c r="Z171" s="260"/>
-      <c r="AA171" s="260"/>
-      <c r="AB171" s="261"/>
-      <c r="AC171" s="262"/>
-      <c r="AD171" s="260"/>
-      <c r="AE171" s="260"/>
-      <c r="AF171" s="260">
+      <c r="Z171" s="264"/>
+      <c r="AA171" s="264"/>
+      <c r="AB171" s="265"/>
+      <c r="AC171" s="266"/>
+      <c r="AD171" s="264"/>
+      <c r="AE171" s="264"/>
+      <c r="AF171" s="264">
         <v>630</v>
       </c>
-      <c r="AG171" s="260"/>
-      <c r="AH171" s="260"/>
-      <c r="AI171" s="261"/>
-      <c r="AJ171" s="262"/>
-      <c r="AK171" s="260"/>
-      <c r="AL171" s="260"/>
-      <c r="AM171" s="260">
+      <c r="AG171" s="264"/>
+      <c r="AH171" s="264"/>
+      <c r="AI171" s="265"/>
+      <c r="AJ171" s="266"/>
+      <c r="AK171" s="264"/>
+      <c r="AL171" s="264"/>
+      <c r="AM171" s="264">
         <v>630</v>
       </c>
-      <c r="AN171" s="260"/>
-      <c r="AO171" s="260"/>
-      <c r="AP171" s="261"/>
-      <c r="AQ171" s="262"/>
-      <c r="AR171" s="260"/>
-      <c r="AS171" s="260"/>
-      <c r="AT171" s="260">
+      <c r="AN171" s="264"/>
+      <c r="AO171" s="264"/>
+      <c r="AP171" s="265"/>
+      <c r="AQ171" s="266"/>
+      <c r="AR171" s="264"/>
+      <c r="AS171" s="264"/>
+      <c r="AT171" s="264">
         <v>630</v>
       </c>
-      <c r="AU171" s="260"/>
-      <c r="AV171" s="260"/>
-      <c r="AW171" s="261"/>
-      <c r="AX171" s="262"/>
-      <c r="AY171" s="260"/>
-      <c r="AZ171" s="260"/>
-      <c r="BA171" s="260">
+      <c r="AU171" s="264"/>
+      <c r="AV171" s="264"/>
+      <c r="AW171" s="265"/>
+      <c r="AX171" s="266"/>
+      <c r="AY171" s="264"/>
+      <c r="AZ171" s="264"/>
+      <c r="BA171" s="264">
         <v>630</v>
       </c>
-      <c r="BB171" s="260"/>
-      <c r="BC171" s="260"/>
-      <c r="BD171" s="261"/>
+      <c r="BB171" s="264"/>
+      <c r="BC171" s="264"/>
+      <c r="BD171" s="265"/>
     </row>
     <row r="172" spans="1:56" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="152"/>
@@ -15834,74 +15793,74 @@
         <f>+D169+D171</f>
         <v>9910</v>
       </c>
-      <c r="E172" s="263" t="s">
+      <c r="E172" s="267" t="s">
         <v>304</v>
       </c>
-      <c r="F172" s="263"/>
-      <c r="G172" s="263"/>
-      <c r="H172" s="258"/>
-      <c r="I172" s="259"/>
-      <c r="J172" s="259"/>
-      <c r="K172" s="256">
+      <c r="F172" s="267"/>
+      <c r="G172" s="267"/>
+      <c r="H172" s="262"/>
+      <c r="I172" s="263"/>
+      <c r="J172" s="263"/>
+      <c r="K172" s="260">
         <v>44607</v>
       </c>
-      <c r="L172" s="256"/>
-      <c r="M172" s="256"/>
-      <c r="N172" s="257"/>
-      <c r="O172" s="258"/>
-      <c r="P172" s="259"/>
-      <c r="Q172" s="259"/>
-      <c r="R172" s="256">
+      <c r="L172" s="260"/>
+      <c r="M172" s="260"/>
+      <c r="N172" s="261"/>
+      <c r="O172" s="262"/>
+      <c r="P172" s="263"/>
+      <c r="Q172" s="263"/>
+      <c r="R172" s="260">
         <v>44607</v>
       </c>
-      <c r="S172" s="256"/>
-      <c r="T172" s="256"/>
-      <c r="U172" s="257"/>
-      <c r="V172" s="258"/>
-      <c r="W172" s="259"/>
-      <c r="X172" s="259"/>
-      <c r="Y172" s="256">
+      <c r="S172" s="260"/>
+      <c r="T172" s="260"/>
+      <c r="U172" s="261"/>
+      <c r="V172" s="262"/>
+      <c r="W172" s="263"/>
+      <c r="X172" s="263"/>
+      <c r="Y172" s="260">
         <v>44607</v>
       </c>
-      <c r="Z172" s="256"/>
-      <c r="AA172" s="256"/>
-      <c r="AB172" s="257"/>
-      <c r="AC172" s="258"/>
-      <c r="AD172" s="259"/>
-      <c r="AE172" s="259"/>
-      <c r="AF172" s="256">
+      <c r="Z172" s="260"/>
+      <c r="AA172" s="260"/>
+      <c r="AB172" s="261"/>
+      <c r="AC172" s="262"/>
+      <c r="AD172" s="263"/>
+      <c r="AE172" s="263"/>
+      <c r="AF172" s="260">
         <v>44607</v>
       </c>
-      <c r="AG172" s="256"/>
-      <c r="AH172" s="256"/>
-      <c r="AI172" s="257"/>
-      <c r="AJ172" s="258"/>
-      <c r="AK172" s="259"/>
-      <c r="AL172" s="259"/>
-      <c r="AM172" s="256">
+      <c r="AG172" s="260"/>
+      <c r="AH172" s="260"/>
+      <c r="AI172" s="261"/>
+      <c r="AJ172" s="262"/>
+      <c r="AK172" s="263"/>
+      <c r="AL172" s="263"/>
+      <c r="AM172" s="260">
         <v>44607</v>
       </c>
-      <c r="AN172" s="256"/>
-      <c r="AO172" s="256"/>
-      <c r="AP172" s="257"/>
-      <c r="AQ172" s="258"/>
-      <c r="AR172" s="259"/>
-      <c r="AS172" s="259"/>
-      <c r="AT172" s="256">
+      <c r="AN172" s="260"/>
+      <c r="AO172" s="260"/>
+      <c r="AP172" s="261"/>
+      <c r="AQ172" s="262"/>
+      <c r="AR172" s="263"/>
+      <c r="AS172" s="263"/>
+      <c r="AT172" s="260">
         <v>44607</v>
       </c>
-      <c r="AU172" s="256"/>
-      <c r="AV172" s="256"/>
-      <c r="AW172" s="257"/>
-      <c r="AX172" s="258"/>
-      <c r="AY172" s="259"/>
-      <c r="AZ172" s="259"/>
-      <c r="BA172" s="256">
+      <c r="AU172" s="260"/>
+      <c r="AV172" s="260"/>
+      <c r="AW172" s="261"/>
+      <c r="AX172" s="262"/>
+      <c r="AY172" s="263"/>
+      <c r="AZ172" s="263"/>
+      <c r="BA172" s="260">
         <v>44607</v>
       </c>
-      <c r="BB172" s="256"/>
-      <c r="BC172" s="256"/>
-      <c r="BD172" s="257"/>
+      <c r="BB172" s="260"/>
+      <c r="BC172" s="260"/>
+      <c r="BD172" s="261"/>
     </row>
     <row r="173" spans="1:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="163"/>
@@ -16132,8 +16091,8 @@
   </sheetPr>
   <dimension ref="B1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScale="129" zoomScaleNormal="129" zoomScaleSheetLayoutView="129" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="129" zoomScaleNormal="129" zoomScaleSheetLayoutView="129" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -16156,15 +16115,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="285" t="s">
-        <v>362</v>
-      </c>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="285"/>
-      <c r="H1" s="285"/>
-      <c r="I1" s="285"/>
+      <c r="C1" s="287" t="s">
+        <v>356</v>
+      </c>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
       <c r="J1" s="193"/>
       <c r="K1" s="193"/>
       <c r="L1" s="193"/>
@@ -16192,13 +16151,13 @@
     </row>
     <row r="2" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="193"/>
-      <c r="C2" s="285"/>
-      <c r="D2" s="285"/>
-      <c r="E2" s="285"/>
-      <c r="F2" s="285"/>
-      <c r="G2" s="285"/>
-      <c r="H2" s="285"/>
-      <c r="I2" s="285"/>
+      <c r="C2" s="287"/>
+      <c r="D2" s="287"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287"/>
+      <c r="H2" s="287"/>
+      <c r="I2" s="287"/>
       <c r="J2" s="193"/>
       <c r="K2" s="193"/>
       <c r="L2" s="193"/>
@@ -16225,11 +16184,11 @@
       <c r="AG2" s="182"/>
     </row>
     <row r="3" spans="2:33" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="215"/>
-      <c r="C3" s="215"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="215"/>
+      <c r="B3" s="207"/>
+      <c r="C3" s="207"/>
+      <c r="D3" s="207"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
       <c r="G3" s="192"/>
       <c r="H3" s="192"/>
       <c r="I3" s="193"/>
@@ -16262,14 +16221,14 @@
       <c r="C4" s="202" t="s">
         <v>337</v>
       </c>
-      <c r="D4" s="286" t="s">
+      <c r="D4" s="288" t="s">
         <v>338</v>
       </c>
-      <c r="E4" s="286"/>
-      <c r="F4" s="286"/>
-      <c r="G4" s="286"/>
-      <c r="H4" s="286"/>
-      <c r="I4" s="287"/>
+      <c r="E4" s="288"/>
+      <c r="F4" s="288"/>
+      <c r="G4" s="288"/>
+      <c r="H4" s="288"/>
+      <c r="I4" s="289"/>
       <c r="J4" s="193"/>
       <c r="K4" s="193"/>
       <c r="L4" s="193"/>
@@ -16297,9 +16256,11 @@
     </row>
     <row r="5" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="202" t="s">
-        <v>349</v>
-      </c>
-      <c r="D5" s="288"/>
+        <v>343</v>
+      </c>
+      <c r="D5" s="288" t="s">
+        <v>363</v>
+      </c>
       <c r="E5" s="288"/>
       <c r="F5" s="288"/>
       <c r="G5" s="288"/>
@@ -16366,16 +16327,16 @@
     </row>
     <row r="7" spans="2:33" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="200" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D7" s="290"/>
       <c r="E7" s="291"/>
-      <c r="F7" s="324"/>
-      <c r="G7" s="324"/>
+      <c r="F7" s="225"/>
+      <c r="G7" s="225"/>
       <c r="H7" s="188" t="s">
-        <v>363</v>
-      </c>
-      <c r="I7" s="338"/>
+        <v>357</v>
+      </c>
+      <c r="I7" s="232"/>
       <c r="J7" s="193"/>
       <c r="K7" s="193"/>
       <c r="L7" s="193"/>
@@ -16403,16 +16364,16 @@
     </row>
     <row r="8" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="200" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="D8" s="290"/>
       <c r="E8" s="291"/>
-      <c r="F8" s="324"/>
-      <c r="G8" s="324"/>
+      <c r="F8" s="225"/>
+      <c r="G8" s="225"/>
       <c r="H8" s="188" t="s">
-        <v>364</v>
-      </c>
-      <c r="I8" s="333"/>
+        <v>358</v>
+      </c>
+      <c r="I8" s="227"/>
       <c r="J8" s="193"/>
       <c r="K8" s="193"/>
       <c r="L8" s="193"/>
@@ -16440,15 +16401,15 @@
     </row>
     <row r="9" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="200" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D9" s="290"/>
       <c r="E9" s="291"/>
       <c r="F9" s="188"/>
       <c r="H9" s="183" t="s">
-        <v>365</v>
-      </c>
-      <c r="I9" s="334"/>
+        <v>359</v>
+      </c>
+      <c r="I9" s="228"/>
       <c r="L9" s="193"/>
       <c r="M9" s="193"/>
       <c r="N9" s="193"/>
@@ -16474,13 +16435,13 @@
     </row>
     <row r="10" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="190"/>
-      <c r="D10" s="234"/>
+      <c r="D10" s="224"/>
       <c r="E10" s="188"/>
       <c r="F10" s="188"/>
       <c r="H10" s="183" t="s">
-        <v>366</v>
-      </c>
-      <c r="I10" s="335"/>
+        <v>360</v>
+      </c>
+      <c r="I10" s="229"/>
       <c r="L10" s="193"/>
       <c r="M10" s="193"/>
       <c r="N10" s="193"/>
@@ -16506,18 +16467,18 @@
     </row>
     <row r="11" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="202" t="s">
-        <v>345</v>
-      </c>
-      <c r="D11" s="329" t="s">
-        <v>347</v>
-      </c>
-      <c r="E11" s="325"/>
-      <c r="F11" s="330"/>
-      <c r="G11" s="327"/>
-      <c r="H11" s="327" t="s">
-        <v>367</v>
-      </c>
-      <c r="I11" s="336"/>
+        <v>339</v>
+      </c>
+      <c r="D11" s="292" t="s">
+        <v>341</v>
+      </c>
+      <c r="E11" s="288"/>
+      <c r="F11" s="289"/>
+      <c r="G11" s="180"/>
+      <c r="H11" s="180" t="s">
+        <v>361</v>
+      </c>
+      <c r="I11" s="230"/>
       <c r="L11" s="193"/>
       <c r="M11" s="193"/>
       <c r="N11" s="193"/>
@@ -16539,18 +16500,18 @@
     </row>
     <row r="12" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="202" t="s">
-        <v>346</v>
-      </c>
-      <c r="D12" s="331" t="s">
-        <v>348</v>
-      </c>
-      <c r="E12" s="326"/>
-      <c r="F12" s="332"/>
-      <c r="G12" s="328"/>
-      <c r="H12" s="328" t="s">
-        <v>368</v>
-      </c>
-      <c r="I12" s="337"/>
+        <v>340</v>
+      </c>
+      <c r="D12" s="327" t="s">
+        <v>342</v>
+      </c>
+      <c r="E12" s="328"/>
+      <c r="F12" s="329"/>
+      <c r="G12" s="226"/>
+      <c r="H12" s="226" t="s">
+        <v>362</v>
+      </c>
+      <c r="I12" s="231"/>
       <c r="J12" s="193"/>
       <c r="K12" s="193"/>
       <c r="L12" s="193"/>
@@ -16601,14 +16562,14 @@
     </row>
     <row r="14" spans="2:33" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G14" s="180"/>
-      <c r="K14" s="212"/>
-      <c r="L14" s="212"/>
-      <c r="M14" s="212"/>
-      <c r="N14" s="212"/>
-      <c r="O14" s="212"/>
-      <c r="P14" s="212"/>
-      <c r="Q14" s="212"/>
-      <c r="R14" s="212"/>
+      <c r="K14" s="204"/>
+      <c r="L14" s="204"/>
+      <c r="M14" s="204"/>
+      <c r="N14" s="204"/>
+      <c r="O14" s="204"/>
+      <c r="P14" s="204"/>
+      <c r="Q14" s="204"/>
+      <c r="R14" s="204"/>
       <c r="S14" s="187"/>
       <c r="T14" s="187"/>
       <c r="U14" s="187"/>
@@ -16622,23 +16583,23 @@
       <c r="AC14" s="186"/>
     </row>
     <row r="15" spans="2:33" s="182" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="292" t="s">
+      <c r="B15" s="293" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="302" t="s">
-        <v>353</v>
-      </c>
-      <c r="D15" s="277" t="s">
+      <c r="C15" s="303" t="s">
+        <v>347</v>
+      </c>
+      <c r="D15" s="279" t="s">
         <v>301</v>
       </c>
-      <c r="E15" s="278"/>
-      <c r="F15" s="279"/>
-      <c r="G15" s="277" t="s">
-        <v>361</v>
-      </c>
-      <c r="H15" s="278"/>
-      <c r="I15" s="278"/>
-      <c r="J15" s="279"/>
+      <c r="E15" s="280"/>
+      <c r="F15" s="281"/>
+      <c r="G15" s="279" t="s">
+        <v>355</v>
+      </c>
+      <c r="H15" s="280"/>
+      <c r="I15" s="280"/>
+      <c r="J15" s="281"/>
       <c r="K15" s="189"/>
       <c r="L15" s="189"/>
       <c r="M15" s="189"/>
@@ -16664,15 +16625,15 @@
       <c r="AG15" s="183"/>
     </row>
     <row r="16" spans="2:33" s="182" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="293"/>
-      <c r="C16" s="303"/>
-      <c r="D16" s="280"/>
-      <c r="E16" s="281"/>
-      <c r="F16" s="282"/>
-      <c r="G16" s="280"/>
-      <c r="H16" s="281"/>
-      <c r="I16" s="281"/>
-      <c r="J16" s="282"/>
+      <c r="B16" s="294"/>
+      <c r="C16" s="304"/>
+      <c r="D16" s="282"/>
+      <c r="E16" s="283"/>
+      <c r="F16" s="284"/>
+      <c r="G16" s="282"/>
+      <c r="H16" s="283"/>
+      <c r="I16" s="283"/>
+      <c r="J16" s="284"/>
       <c r="K16" s="190"/>
       <c r="L16" s="190"/>
       <c r="M16" s="190"/>
@@ -16691,80 +16652,80 @@
       <c r="Z16" s="190"/>
       <c r="AA16" s="190"/>
       <c r="AB16" s="190"/>
-      <c r="AC16" s="211"/>
+      <c r="AC16" s="203"/>
       <c r="AD16" s="183"/>
       <c r="AE16" s="183"/>
       <c r="AF16" s="183"/>
       <c r="AG16" s="183"/>
     </row>
     <row r="17" spans="2:29" s="182" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="293"/>
-      <c r="C17" s="303"/>
-      <c r="D17" s="296" t="s">
+      <c r="B17" s="294"/>
+      <c r="C17" s="304"/>
+      <c r="D17" s="297" t="s">
+        <v>348</v>
+      </c>
+      <c r="E17" s="297" t="s">
+        <v>349</v>
+      </c>
+      <c r="F17" s="305" t="s">
+        <v>350</v>
+      </c>
+      <c r="G17" s="285" t="s">
+        <v>351</v>
+      </c>
+      <c r="H17" s="285" t="s">
+        <v>352</v>
+      </c>
+      <c r="I17" s="299" t="s">
+        <v>353</v>
+      </c>
+      <c r="J17" s="306" t="s">
         <v>354</v>
       </c>
-      <c r="E17" s="296" t="s">
-        <v>355</v>
-      </c>
-      <c r="F17" s="304" t="s">
-        <v>356</v>
-      </c>
-      <c r="G17" s="283" t="s">
-        <v>357</v>
-      </c>
-      <c r="H17" s="283" t="s">
-        <v>358</v>
-      </c>
-      <c r="I17" s="298" t="s">
-        <v>359</v>
-      </c>
-      <c r="J17" s="275" t="s">
-        <v>360</v>
-      </c>
     </row>
     <row r="18" spans="2:29" s="182" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="293"/>
-      <c r="C18" s="303"/>
-      <c r="D18" s="296"/>
-      <c r="E18" s="296"/>
-      <c r="F18" s="283"/>
-      <c r="G18" s="283"/>
-      <c r="H18" s="283"/>
-      <c r="I18" s="296"/>
-      <c r="J18" s="275"/>
+      <c r="B18" s="294"/>
+      <c r="C18" s="304"/>
+      <c r="D18" s="297"/>
+      <c r="E18" s="297"/>
+      <c r="F18" s="285"/>
+      <c r="G18" s="285"/>
+      <c r="H18" s="285"/>
+      <c r="I18" s="297"/>
+      <c r="J18" s="306"/>
     </row>
     <row r="19" spans="2:29" s="182" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="294"/>
-      <c r="C19" s="303"/>
-      <c r="D19" s="297"/>
-      <c r="E19" s="297"/>
-      <c r="F19" s="284"/>
-      <c r="G19" s="284"/>
-      <c r="H19" s="284"/>
-      <c r="I19" s="297"/>
-      <c r="J19" s="276"/>
+      <c r="B19" s="295"/>
+      <c r="C19" s="304"/>
+      <c r="D19" s="298"/>
+      <c r="E19" s="298"/>
+      <c r="F19" s="286"/>
+      <c r="G19" s="286"/>
+      <c r="H19" s="286"/>
+      <c r="I19" s="298"/>
+      <c r="J19" s="307"/>
     </row>
     <row r="20" spans="2:29" s="182" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B20" s="216"/>
-      <c r="C20" s="217"/>
-      <c r="D20" s="218"/>
-      <c r="E20" s="219"/>
-      <c r="F20" s="232"/>
-      <c r="G20" s="220"/>
-      <c r="H20" s="220"/>
-      <c r="I20" s="221"/>
-      <c r="J20" s="222"/>
+      <c r="B20" s="208"/>
+      <c r="C20" s="209"/>
+      <c r="D20" s="210"/>
+      <c r="E20" s="211"/>
+      <c r="F20" s="222"/>
+      <c r="G20" s="212"/>
+      <c r="H20" s="212"/>
+      <c r="I20" s="213"/>
+      <c r="J20" s="214"/>
     </row>
     <row r="21" spans="2:29" s="182" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="223"/>
-      <c r="C21" s="224"/>
-      <c r="D21" s="225"/>
-      <c r="E21" s="226"/>
-      <c r="F21" s="233"/>
-      <c r="G21" s="227"/>
-      <c r="H21" s="227"/>
-      <c r="I21" s="228"/>
-      <c r="J21" s="229"/>
+      <c r="B21" s="215"/>
+      <c r="C21" s="216"/>
+      <c r="D21" s="217"/>
+      <c r="E21" s="218"/>
+      <c r="F21" s="223"/>
+      <c r="G21" s="219"/>
+      <c r="H21" s="219"/>
+      <c r="I21" s="220"/>
+      <c r="J21" s="221"/>
     </row>
     <row r="22" spans="2:29" s="182" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="195"/>
@@ -16778,170 +16739,158 @@
     </row>
     <row r="23" spans="2:29" s="182" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="181"/>
-      <c r="C23" s="203" t="s">
-        <v>340</v>
-      </c>
-      <c r="D23" s="204"/>
-      <c r="E23" s="204"/>
-      <c r="F23" s="204"/>
-      <c r="G23" s="204"/>
-      <c r="H23" s="231"/>
-      <c r="I23" s="230"/>
-      <c r="J23" s="299"/>
-      <c r="K23" s="299"/>
-      <c r="L23" s="299"/>
-      <c r="M23" s="214"/>
-      <c r="N23" s="214"/>
-      <c r="O23" s="214"/>
+      <c r="C23" s="233"/>
+      <c r="D23" s="233"/>
+      <c r="E23" s="233"/>
+      <c r="F23" s="233"/>
+      <c r="G23" s="233"/>
+      <c r="H23" s="234"/>
+      <c r="I23" s="234"/>
+      <c r="J23" s="300"/>
+      <c r="K23" s="300"/>
+      <c r="L23" s="300"/>
+      <c r="M23" s="206"/>
+      <c r="N23" s="206"/>
+      <c r="O23" s="206"/>
       <c r="P23" s="191"/>
-      <c r="Q23" s="214"/>
-      <c r="R23" s="214"/>
-      <c r="S23" s="214"/>
-      <c r="T23" s="214"/>
-      <c r="U23" s="214"/>
-      <c r="V23" s="300"/>
-      <c r="W23" s="300"/>
-      <c r="X23" s="299"/>
-      <c r="Y23" s="299"/>
-      <c r="Z23" s="299"/>
-      <c r="AA23" s="299"/>
-      <c r="AB23" s="299"/>
-      <c r="AC23" s="212"/>
+      <c r="Q23" s="206"/>
+      <c r="R23" s="206"/>
+      <c r="S23" s="206"/>
+      <c r="T23" s="206"/>
+      <c r="U23" s="206"/>
+      <c r="V23" s="301"/>
+      <c r="W23" s="301"/>
+      <c r="X23" s="300"/>
+      <c r="Y23" s="300"/>
+      <c r="Z23" s="300"/>
+      <c r="AA23" s="300"/>
+      <c r="AB23" s="300"/>
+      <c r="AC23" s="204"/>
     </row>
     <row r="24" spans="2:29" s="182" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="181"/>
-      <c r="C24" s="205" t="s">
-        <v>343</v>
-      </c>
-      <c r="D24" s="206"/>
-      <c r="E24" s="206"/>
-      <c r="F24" s="206"/>
-      <c r="G24" s="206"/>
-      <c r="H24" s="231"/>
-      <c r="I24" s="230"/>
-      <c r="J24" s="212"/>
-      <c r="O24" s="214"/>
-      <c r="P24" s="214"/>
-      <c r="Q24" s="214"/>
-      <c r="R24" s="214"/>
-      <c r="S24" s="214"/>
-      <c r="T24" s="214"/>
-      <c r="U24" s="214"/>
-      <c r="V24" s="213"/>
-      <c r="W24" s="213"/>
-      <c r="X24" s="212"/>
-      <c r="Y24" s="212"/>
-      <c r="Z24" s="212"/>
-      <c r="AA24" s="212"/>
-      <c r="AB24" s="212"/>
-      <c r="AC24" s="212"/>
+      <c r="C24" s="235"/>
+      <c r="D24" s="235"/>
+      <c r="E24" s="235"/>
+      <c r="F24" s="235"/>
+      <c r="G24" s="235"/>
+      <c r="H24" s="234"/>
+      <c r="I24" s="234"/>
+      <c r="J24" s="204"/>
+      <c r="O24" s="206"/>
+      <c r="P24" s="206"/>
+      <c r="Q24" s="206"/>
+      <c r="R24" s="206"/>
+      <c r="S24" s="206"/>
+      <c r="T24" s="206"/>
+      <c r="U24" s="206"/>
+      <c r="V24" s="205"/>
+      <c r="W24" s="205"/>
+      <c r="X24" s="204"/>
+      <c r="Y24" s="204"/>
+      <c r="Z24" s="204"/>
+      <c r="AA24" s="204"/>
+      <c r="AB24" s="204"/>
+      <c r="AC24" s="204"/>
     </row>
     <row r="25" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="181"/>
-      <c r="C25" s="207" t="s">
-        <v>339</v>
-      </c>
-      <c r="D25" s="208"/>
-      <c r="E25" s="208"/>
-      <c r="F25" s="208"/>
-      <c r="G25" s="208"/>
-      <c r="H25" s="231"/>
-      <c r="I25" s="230"/>
-      <c r="J25" s="299"/>
-      <c r="K25" s="299"/>
-      <c r="L25" s="299"/>
-      <c r="M25" s="214"/>
-      <c r="N25" s="214"/>
-      <c r="O25" s="214"/>
-      <c r="P25" s="214"/>
-      <c r="Q25" s="214"/>
-      <c r="R25" s="214"/>
-      <c r="S25" s="214"/>
-      <c r="T25" s="214"/>
-      <c r="U25" s="214"/>
-      <c r="V25" s="214"/>
-      <c r="W25" s="301"/>
-      <c r="X25" s="301"/>
-      <c r="Y25" s="301"/>
-      <c r="Z25" s="214"/>
-      <c r="AA25" s="214"/>
-      <c r="AB25" s="214"/>
-      <c r="AC25" s="214"/>
+      <c r="C25" s="236"/>
+      <c r="D25" s="236"/>
+      <c r="E25" s="236"/>
+      <c r="F25" s="236"/>
+      <c r="G25" s="236"/>
+      <c r="H25" s="234"/>
+      <c r="I25" s="234"/>
+      <c r="J25" s="300"/>
+      <c r="K25" s="300"/>
+      <c r="L25" s="300"/>
+      <c r="M25" s="206"/>
+      <c r="N25" s="206"/>
+      <c r="O25" s="206"/>
+      <c r="P25" s="206"/>
+      <c r="Q25" s="206"/>
+      <c r="R25" s="206"/>
+      <c r="S25" s="206"/>
+      <c r="T25" s="206"/>
+      <c r="U25" s="206"/>
+      <c r="V25" s="206"/>
+      <c r="W25" s="302"/>
+      <c r="X25" s="302"/>
+      <c r="Y25" s="302"/>
+      <c r="Z25" s="206"/>
+      <c r="AA25" s="206"/>
+      <c r="AB25" s="206"/>
+      <c r="AC25" s="206"/>
     </row>
     <row r="26" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="181"/>
-      <c r="C26" s="207" t="s">
-        <v>341</v>
-      </c>
-      <c r="D26" s="208"/>
-      <c r="E26" s="208"/>
-      <c r="F26" s="208"/>
-      <c r="G26" s="208"/>
-      <c r="H26" s="231"/>
-      <c r="I26" s="230"/>
-      <c r="J26" s="214"/>
-      <c r="K26" s="214"/>
-      <c r="L26" s="214"/>
-      <c r="M26" s="214"/>
-      <c r="N26" s="214"/>
-      <c r="O26" s="214"/>
-      <c r="P26" s="214"/>
-      <c r="Q26" s="214"/>
-      <c r="R26" s="214"/>
-      <c r="S26" s="214"/>
-      <c r="T26" s="214"/>
-      <c r="U26" s="214"/>
-      <c r="V26" s="214"/>
-      <c r="W26" s="295"/>
-      <c r="X26" s="295"/>
-      <c r="Y26" s="295"/>
-      <c r="Z26" s="295"/>
-      <c r="AA26" s="295"/>
-      <c r="AB26" s="214"/>
-      <c r="AC26" s="214"/>
+      <c r="C26" s="236"/>
+      <c r="D26" s="236"/>
+      <c r="E26" s="236"/>
+      <c r="F26" s="236"/>
+      <c r="G26" s="236"/>
+      <c r="H26" s="234"/>
+      <c r="I26" s="234"/>
+      <c r="J26" s="206"/>
+      <c r="K26" s="206"/>
+      <c r="L26" s="206"/>
+      <c r="M26" s="206"/>
+      <c r="N26" s="206"/>
+      <c r="O26" s="206"/>
+      <c r="P26" s="206"/>
+      <c r="Q26" s="206"/>
+      <c r="R26" s="206"/>
+      <c r="S26" s="206"/>
+      <c r="T26" s="206"/>
+      <c r="U26" s="206"/>
+      <c r="V26" s="206"/>
+      <c r="W26" s="296"/>
+      <c r="X26" s="296"/>
+      <c r="Y26" s="296"/>
+      <c r="Z26" s="296"/>
+      <c r="AA26" s="296"/>
+      <c r="AB26" s="206"/>
+      <c r="AC26" s="206"/>
     </row>
     <row r="27" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="181"/>
-      <c r="C27" s="205" t="s">
-        <v>342</v>
-      </c>
-      <c r="D27" s="206"/>
-      <c r="E27" s="206"/>
-      <c r="F27" s="206"/>
-      <c r="G27" s="206"/>
-      <c r="H27" s="231"/>
-      <c r="I27" s="230"/>
-      <c r="J27" s="214"/>
-      <c r="K27" s="214"/>
-      <c r="L27" s="214"/>
-      <c r="M27" s="214"/>
-      <c r="N27" s="214"/>
-      <c r="O27" s="214"/>
-      <c r="P27" s="214"/>
-      <c r="Q27" s="214"/>
-      <c r="R27" s="214"/>
-      <c r="S27" s="214"/>
-      <c r="T27" s="214"/>
-      <c r="U27" s="214"/>
-      <c r="V27" s="214"/>
-      <c r="W27" s="214"/>
-      <c r="X27" s="214"/>
-      <c r="Y27" s="214"/>
-      <c r="Z27" s="214"/>
-      <c r="AA27" s="214"/>
-      <c r="AB27" s="214"/>
-      <c r="AC27" s="214"/>
+      <c r="C27" s="235"/>
+      <c r="D27" s="235"/>
+      <c r="E27" s="235"/>
+      <c r="F27" s="235"/>
+      <c r="G27" s="235"/>
+      <c r="H27" s="234"/>
+      <c r="I27" s="234"/>
+      <c r="J27" s="238"/>
+      <c r="K27" s="206"/>
+      <c r="L27" s="206"/>
+      <c r="M27" s="206"/>
+      <c r="N27" s="206"/>
+      <c r="O27" s="206"/>
+      <c r="P27" s="206"/>
+      <c r="Q27" s="206"/>
+      <c r="R27" s="206"/>
+      <c r="S27" s="206"/>
+      <c r="T27" s="206"/>
+      <c r="U27" s="206"/>
+      <c r="V27" s="206"/>
+      <c r="W27" s="206"/>
+      <c r="X27" s="206"/>
+      <c r="Y27" s="206"/>
+      <c r="Z27" s="206"/>
+      <c r="AA27" s="206"/>
+      <c r="AB27" s="206"/>
+      <c r="AC27" s="206"/>
     </row>
     <row r="28" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="209" t="s">
-        <v>344</v>
-      </c>
-      <c r="D28" s="210"/>
-      <c r="E28" s="210"/>
-      <c r="F28" s="210"/>
-      <c r="G28" s="210"/>
-      <c r="H28" s="231"/>
-      <c r="I28" s="230"/>
+      <c r="C28" s="237"/>
+      <c r="D28" s="237"/>
+      <c r="E28" s="237"/>
+      <c r="F28" s="237"/>
+      <c r="G28" s="237"/>
+      <c r="H28" s="234"/>
+      <c r="I28" s="234"/>
       <c r="J28" s="184"/>
       <c r="W28" s="185"/>
     </row>
@@ -16950,8 +16899,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="W26:AA26"/>
     <mergeCell ref="D17:D19"/>
@@ -16975,6 +16922,8 @@
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="P23">
@@ -16988,9 +16937,6 @@
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="82" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <rowBreaks count="1" manualBreakCount="1">
-    <brk id="24" max="10" man="1"/>
-  </rowBreaks>
 </worksheet>
 </file>
 
@@ -17018,72 +16964,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="306" t="s">
+      <c r="B2" s="309" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="307"/>
-      <c r="F2" s="307"/>
-      <c r="G2" s="307"/>
-      <c r="H2" s="307"/>
-      <c r="I2" s="307"/>
-      <c r="J2" s="307"/>
-      <c r="K2" s="307"/>
-      <c r="L2" s="307"/>
-      <c r="M2" s="308"/>
+      <c r="C2" s="310"/>
+      <c r="D2" s="310"/>
+      <c r="E2" s="310"/>
+      <c r="F2" s="310"/>
+      <c r="G2" s="310"/>
+      <c r="H2" s="310"/>
+      <c r="I2" s="310"/>
+      <c r="J2" s="310"/>
+      <c r="K2" s="310"/>
+      <c r="L2" s="310"/>
+      <c r="M2" s="311"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="309" t="s">
+      <c r="B3" s="312" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="311" t="s">
+      <c r="C3" s="314" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="311" t="s">
+      <c r="D3" s="314" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="313" t="s">
+      <c r="E3" s="316" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="315" t="s">
+      <c r="F3" s="318" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="316"/>
-      <c r="H3" s="316"/>
-      <c r="I3" s="316"/>
-      <c r="J3" s="316"/>
-      <c r="K3" s="316"/>
-      <c r="L3" s="316"/>
-      <c r="M3" s="317"/>
+      <c r="G3" s="319"/>
+      <c r="H3" s="319"/>
+      <c r="I3" s="319"/>
+      <c r="J3" s="319"/>
+      <c r="K3" s="319"/>
+      <c r="L3" s="319"/>
+      <c r="M3" s="320"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="310"/>
-      <c r="C4" s="312"/>
-      <c r="D4" s="312"/>
-      <c r="E4" s="314"/>
-      <c r="F4" s="318"/>
-      <c r="G4" s="319"/>
-      <c r="H4" s="319"/>
-      <c r="I4" s="319"/>
-      <c r="J4" s="319"/>
-      <c r="K4" s="319"/>
-      <c r="L4" s="319"/>
-      <c r="M4" s="320"/>
+      <c r="B4" s="313"/>
+      <c r="C4" s="315"/>
+      <c r="D4" s="315"/>
+      <c r="E4" s="317"/>
+      <c r="F4" s="321"/>
+      <c r="G4" s="322"/>
+      <c r="H4" s="322"/>
+      <c r="I4" s="322"/>
+      <c r="J4" s="322"/>
+      <c r="K4" s="322"/>
+      <c r="L4" s="322"/>
+      <c r="M4" s="323"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="305"/>
-      <c r="C5" s="305"/>
-      <c r="D5" s="305"/>
-      <c r="E5" s="305"/>
-      <c r="F5" s="305"/>
-      <c r="G5" s="305"/>
-      <c r="H5" s="305"/>
-      <c r="I5" s="305"/>
-      <c r="J5" s="305"/>
-      <c r="K5" s="305"/>
-      <c r="L5" s="305"/>
-      <c r="M5" s="305"/>
+      <c r="B5" s="308"/>
+      <c r="C5" s="308"/>
+      <c r="D5" s="308"/>
+      <c r="E5" s="308"/>
+      <c r="F5" s="308"/>
+      <c r="G5" s="308"/>
+      <c r="H5" s="308"/>
+      <c r="I5" s="308"/>
+      <c r="J5" s="308"/>
+      <c r="K5" s="308"/>
+      <c r="L5" s="308"/>
+      <c r="M5" s="308"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -17696,72 +17642,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="306" t="s">
+      <c r="B2" s="309" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="307"/>
-      <c r="F2" s="307"/>
-      <c r="G2" s="307"/>
-      <c r="H2" s="307"/>
-      <c r="I2" s="307"/>
-      <c r="J2" s="307"/>
-      <c r="K2" s="307"/>
-      <c r="L2" s="307"/>
-      <c r="M2" s="308"/>
+      <c r="C2" s="310"/>
+      <c r="D2" s="310"/>
+      <c r="E2" s="310"/>
+      <c r="F2" s="310"/>
+      <c r="G2" s="310"/>
+      <c r="H2" s="310"/>
+      <c r="I2" s="310"/>
+      <c r="J2" s="310"/>
+      <c r="K2" s="310"/>
+      <c r="L2" s="310"/>
+      <c r="M2" s="311"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="309" t="s">
+      <c r="B3" s="312" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="311" t="s">
+      <c r="C3" s="314" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="311" t="s">
+      <c r="D3" s="314" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="313" t="s">
+      <c r="E3" s="316" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="315" t="s">
+      <c r="F3" s="318" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="316"/>
-      <c r="H3" s="316"/>
-      <c r="I3" s="316"/>
-      <c r="J3" s="316"/>
-      <c r="K3" s="316"/>
-      <c r="L3" s="316"/>
-      <c r="M3" s="317"/>
+      <c r="G3" s="319"/>
+      <c r="H3" s="319"/>
+      <c r="I3" s="319"/>
+      <c r="J3" s="319"/>
+      <c r="K3" s="319"/>
+      <c r="L3" s="319"/>
+      <c r="M3" s="320"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="310"/>
-      <c r="C4" s="312"/>
-      <c r="D4" s="312"/>
-      <c r="E4" s="314"/>
-      <c r="F4" s="318"/>
-      <c r="G4" s="319"/>
-      <c r="H4" s="319"/>
-      <c r="I4" s="319"/>
-      <c r="J4" s="319"/>
-      <c r="K4" s="319"/>
-      <c r="L4" s="319"/>
-      <c r="M4" s="320"/>
+      <c r="B4" s="313"/>
+      <c r="C4" s="315"/>
+      <c r="D4" s="315"/>
+      <c r="E4" s="317"/>
+      <c r="F4" s="321"/>
+      <c r="G4" s="322"/>
+      <c r="H4" s="322"/>
+      <c r="I4" s="322"/>
+      <c r="J4" s="322"/>
+      <c r="K4" s="322"/>
+      <c r="L4" s="322"/>
+      <c r="M4" s="323"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="305"/>
-      <c r="C5" s="305"/>
-      <c r="D5" s="305"/>
-      <c r="E5" s="305"/>
-      <c r="F5" s="321"/>
-      <c r="G5" s="321"/>
-      <c r="H5" s="321"/>
-      <c r="I5" s="321"/>
-      <c r="J5" s="321"/>
-      <c r="K5" s="321"/>
-      <c r="L5" s="321"/>
-      <c r="M5" s="321"/>
+      <c r="B5" s="308"/>
+      <c r="C5" s="308"/>
+      <c r="D5" s="308"/>
+      <c r="E5" s="308"/>
+      <c r="F5" s="324"/>
+      <c r="G5" s="324"/>
+      <c r="H5" s="324"/>
+      <c r="I5" s="324"/>
+      <c r="J5" s="324"/>
+      <c r="K5" s="324"/>
+      <c r="L5" s="324"/>
+      <c r="M5" s="324"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -18362,72 +18308,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="306" t="s">
+      <c r="B2" s="309" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="307"/>
-      <c r="D2" s="307"/>
-      <c r="E2" s="307"/>
-      <c r="F2" s="307"/>
-      <c r="G2" s="307"/>
-      <c r="H2" s="307"/>
-      <c r="I2" s="307"/>
-      <c r="J2" s="307"/>
-      <c r="K2" s="307"/>
-      <c r="L2" s="307"/>
-      <c r="M2" s="308"/>
+      <c r="C2" s="310"/>
+      <c r="D2" s="310"/>
+      <c r="E2" s="310"/>
+      <c r="F2" s="310"/>
+      <c r="G2" s="310"/>
+      <c r="H2" s="310"/>
+      <c r="I2" s="310"/>
+      <c r="J2" s="310"/>
+      <c r="K2" s="310"/>
+      <c r="L2" s="310"/>
+      <c r="M2" s="311"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="309" t="s">
+      <c r="B3" s="312" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="311" t="s">
+      <c r="C3" s="314" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="311" t="s">
+      <c r="D3" s="314" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="313" t="s">
+      <c r="E3" s="316" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="315" t="s">
+      <c r="F3" s="318" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="316"/>
-      <c r="H3" s="316"/>
-      <c r="I3" s="316"/>
-      <c r="J3" s="316"/>
-      <c r="K3" s="316"/>
-      <c r="L3" s="316"/>
-      <c r="M3" s="317"/>
+      <c r="G3" s="319"/>
+      <c r="H3" s="319"/>
+      <c r="I3" s="319"/>
+      <c r="J3" s="319"/>
+      <c r="K3" s="319"/>
+      <c r="L3" s="319"/>
+      <c r="M3" s="320"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="310"/>
-      <c r="C4" s="312"/>
-      <c r="D4" s="312"/>
-      <c r="E4" s="314"/>
-      <c r="F4" s="318"/>
-      <c r="G4" s="319"/>
-      <c r="H4" s="319"/>
-      <c r="I4" s="319"/>
-      <c r="J4" s="319"/>
-      <c r="K4" s="319"/>
-      <c r="L4" s="319"/>
-      <c r="M4" s="320"/>
+      <c r="B4" s="313"/>
+      <c r="C4" s="315"/>
+      <c r="D4" s="315"/>
+      <c r="E4" s="317"/>
+      <c r="F4" s="321"/>
+      <c r="G4" s="322"/>
+      <c r="H4" s="322"/>
+      <c r="I4" s="322"/>
+      <c r="J4" s="322"/>
+      <c r="K4" s="322"/>
+      <c r="L4" s="322"/>
+      <c r="M4" s="323"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="322"/>
-      <c r="C5" s="305"/>
-      <c r="D5" s="305"/>
-      <c r="E5" s="305"/>
-      <c r="F5" s="305"/>
-      <c r="G5" s="305"/>
-      <c r="H5" s="305"/>
-      <c r="I5" s="305"/>
-      <c r="J5" s="305"/>
-      <c r="K5" s="305"/>
-      <c r="L5" s="305"/>
-      <c r="M5" s="323"/>
+      <c r="B5" s="325"/>
+      <c r="C5" s="308"/>
+      <c r="D5" s="308"/>
+      <c r="E5" s="308"/>
+      <c r="F5" s="308"/>
+      <c r="G5" s="308"/>
+      <c r="H5" s="308"/>
+      <c r="I5" s="308"/>
+      <c r="J5" s="308"/>
+      <c r="K5" s="308"/>
+      <c r="L5" s="308"/>
+      <c r="M5" s="326"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">

</xml_diff>

<commit_message>
config generate report for Nivel and modified styles
</commit_message>
<xml_diff>
--- a/public/templates/report_template_project.xlsx
+++ b/public/templates/report_template_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcastillo\Documents\QuisVar\quisvar_proyect_ft\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyecto_quisvar\quisvar_proyect_ft\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCA908E-26C9-45BC-9694-B2D1D080E3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDA1AD1-BC86-4884-BA71-8D0CF9C80C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="482" firstSheet="1" activeTab="1" xr2:uid="{F98A2DB2-54A5-485C-A701-CE43CF6B2BAF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="482" firstSheet="1" activeTab="1" xr2:uid="{F98A2DB2-54A5-485C-A701-CE43CF6B2BAF}"/>
   </bookViews>
   <sheets>
     <sheet name="LIQUIDACION" sheetId="9" state="hidden" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="358">
   <si>
     <t>ITEM</t>
   </si>
@@ -1590,18 +1590,9 @@
     <t xml:space="preserve">Saldo ha recibir </t>
   </si>
   <si>
-    <t>CC  COORDINADOR GENERAL DE PROYECTOS</t>
-  </si>
-  <si>
     <t>ING JUAN GONZALO QUISPE CONDORI</t>
   </si>
   <si>
-    <t>FECHA DE INICIO</t>
-  </si>
-  <si>
-    <t>FECHA FINAL</t>
-  </si>
-  <si>
     <t>28 DE MARZO DEL 2023</t>
   </si>
   <si>
@@ -1632,43 +1623,34 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Sin Asignar</t>
-  </si>
-  <si>
-    <t>En proceso</t>
-  </si>
-  <si>
-    <t>Terminadas</t>
-  </si>
-  <si>
-    <t>Liquidados</t>
-  </si>
-  <si>
-    <t>Estado de las Tareas</t>
-  </si>
-  <si>
     <t>INFORME PARCIAL DEL PROYECTO</t>
   </si>
   <si>
-    <t>Proyecto</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Nivel1</t>
-  </si>
-  <si>
-    <t>Nivel2</t>
-  </si>
-  <si>
-    <t>Nivel3</t>
-  </si>
-  <si>
-    <t>Nivel4</t>
-  </si>
-  <si>
     <t>sadsa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC  COORDINADOR GENERAL </t>
+  </si>
+  <si>
+    <t>FECHA DE INICIO DEL PROYECTO</t>
+  </si>
+  <si>
+    <t>FECHA FINAL DEL PROYECTO</t>
+  </si>
+  <si>
+    <t>Porcentaje</t>
+  </si>
+  <si>
+    <t>Total de dias</t>
+  </si>
+  <si>
+    <t>total de tareas</t>
+  </si>
+  <si>
+    <t>Nivel</t>
+  </si>
+  <si>
+    <t>Mas informacion</t>
   </si>
 </sst>
 </file>
@@ -1676,13 +1658,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="00.00.00.00"/>
-    <numFmt numFmtId="166" formatCode="00.00.00"/>
-    <numFmt numFmtId="167" formatCode="&quot;S/&quot;#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="169" formatCode="&quot;S/&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="00.00.00.00"/>
+    <numFmt numFmtId="167" formatCode="00.00.00"/>
+    <numFmt numFmtId="168" formatCode="&quot;S/&quot;#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="170" formatCode="&quot;S/&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="38" x14ac:knownFonts="1">
     <font>
@@ -1940,7 +1922,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2001,42 +1983,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF666F88"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF788199"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF8990A2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA3A8B7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB5BAC9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9E1F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="85">
     <border>
@@ -3107,13 +3053,13 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="169" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="330">
+  <cellXfs count="324">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3148,10 +3094,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3419,19 +3365,25 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3440,13 +3392,7 @@
     <xf numFmtId="166" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3526,7 +3472,7 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3544,7 +3490,7 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="9" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3559,13 +3505,13 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="9" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="17" fillId="9" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3586,7 +3532,7 @@
     <xf numFmtId="0" fontId="34" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="27" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="27" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3601,7 +3547,7 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3619,7 +3565,7 @@
     <xf numFmtId="0" fontId="28" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="31" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3658,7 +3604,7 @@
     <xf numFmtId="0" fontId="28" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="9" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="31" fillId="9" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3679,7 +3625,7 @@
     <xf numFmtId="0" fontId="28" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="9" borderId="63" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="31" fillId="9" borderId="63" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3707,26 +3653,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="33" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="33" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3816,13 +3746,13 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="9" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="9" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3861,6 +3791,84 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="10" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3879,75 +3887,6 @@
     <xf numFmtId="0" fontId="23" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4004,15 +3943,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -4381,174 +4311,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="273" t="s">
+      <c r="A1" s="267" t="s">
         <v>325</v>
       </c>
-      <c r="B1" s="272"/>
-      <c r="C1" s="272"/>
-      <c r="D1" s="272"/>
-      <c r="E1" s="272"/>
-      <c r="F1" s="272"/>
-      <c r="G1" s="272"/>
-      <c r="H1" s="272"/>
-      <c r="I1" s="272"/>
-      <c r="J1" s="272"/>
-      <c r="K1" s="272"/>
-      <c r="L1" s="272"/>
-      <c r="M1" s="272"/>
-      <c r="N1" s="272"/>
-      <c r="O1" s="271" t="s">
+      <c r="B1" s="266"/>
+      <c r="C1" s="266"/>
+      <c r="D1" s="266"/>
+      <c r="E1" s="266"/>
+      <c r="F1" s="266"/>
+      <c r="G1" s="266"/>
+      <c r="H1" s="266"/>
+      <c r="I1" s="266"/>
+      <c r="J1" s="266"/>
+      <c r="K1" s="266"/>
+      <c r="L1" s="266"/>
+      <c r="M1" s="266"/>
+      <c r="N1" s="266"/>
+      <c r="O1" s="265" t="s">
         <v>323</v>
       </c>
-      <c r="P1" s="271"/>
-      <c r="Q1" s="271"/>
-      <c r="R1" s="271"/>
-      <c r="S1" s="271"/>
-      <c r="T1" s="271"/>
-      <c r="U1" s="271"/>
-      <c r="V1" s="271"/>
-      <c r="W1" s="271"/>
-      <c r="X1" s="271"/>
-      <c r="Y1" s="271"/>
-      <c r="Z1" s="271"/>
-      <c r="AA1" s="271"/>
-      <c r="AB1" s="271"/>
-      <c r="AC1" s="271"/>
-      <c r="AD1" s="271"/>
-      <c r="AE1" s="271"/>
-      <c r="AF1" s="271"/>
-      <c r="AG1" s="271"/>
-      <c r="AH1" s="272" t="s">
+      <c r="P1" s="265"/>
+      <c r="Q1" s="265"/>
+      <c r="R1" s="265"/>
+      <c r="S1" s="265"/>
+      <c r="T1" s="265"/>
+      <c r="U1" s="265"/>
+      <c r="V1" s="265"/>
+      <c r="W1" s="265"/>
+      <c r="X1" s="265"/>
+      <c r="Y1" s="265"/>
+      <c r="Z1" s="265"/>
+      <c r="AA1" s="265"/>
+      <c r="AB1" s="265"/>
+      <c r="AC1" s="265"/>
+      <c r="AD1" s="265"/>
+      <c r="AE1" s="265"/>
+      <c r="AF1" s="265"/>
+      <c r="AG1" s="265"/>
+      <c r="AH1" s="266" t="s">
         <v>317</v>
       </c>
-      <c r="AI1" s="272"/>
-      <c r="AJ1" s="272"/>
-      <c r="AK1" s="272"/>
-      <c r="AL1" s="269" t="s">
+      <c r="AI1" s="266"/>
+      <c r="AJ1" s="266"/>
+      <c r="AK1" s="266"/>
+      <c r="AL1" s="263" t="s">
         <v>324</v>
       </c>
-      <c r="AM1" s="269"/>
-      <c r="AN1" s="269"/>
-      <c r="AO1" s="269"/>
-      <c r="AP1" s="269"/>
-      <c r="AQ1" s="269"/>
-      <c r="AR1" s="269"/>
-      <c r="AS1" s="269"/>
-      <c r="AT1" s="269"/>
-      <c r="AU1" s="269"/>
-      <c r="AV1" s="269"/>
-      <c r="AW1" s="269"/>
-      <c r="AX1" s="269"/>
-      <c r="AY1" s="269"/>
-      <c r="AZ1" s="269"/>
-      <c r="BA1" s="269"/>
-      <c r="BB1" s="269"/>
-      <c r="BC1" s="269"/>
-      <c r="BD1" s="270"/>
+      <c r="AM1" s="263"/>
+      <c r="AN1" s="263"/>
+      <c r="AO1" s="263"/>
+      <c r="AP1" s="263"/>
+      <c r="AQ1" s="263"/>
+      <c r="AR1" s="263"/>
+      <c r="AS1" s="263"/>
+      <c r="AT1" s="263"/>
+      <c r="AU1" s="263"/>
+      <c r="AV1" s="263"/>
+      <c r="AW1" s="263"/>
+      <c r="AX1" s="263"/>
+      <c r="AY1" s="263"/>
+      <c r="AZ1" s="263"/>
+      <c r="BA1" s="263"/>
+      <c r="BB1" s="263"/>
+      <c r="BC1" s="263"/>
+      <c r="BD1" s="264"/>
     </row>
     <row r="2" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="239" t="s">
+      <c r="A2" s="233" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="240"/>
+      <c r="B2" s="234"/>
       <c r="C2" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D2" s="243" t="s">
+      <c r="D2" s="237" t="s">
         <v>327</v>
       </c>
-      <c r="E2" s="243"/>
-      <c r="F2" s="275" t="s">
+      <c r="E2" s="237"/>
+      <c r="F2" s="269" t="s">
         <v>326</v>
       </c>
-      <c r="G2" s="275"/>
-      <c r="H2" s="275"/>
-      <c r="I2" s="275"/>
-      <c r="J2" s="275"/>
-      <c r="K2" s="275"/>
-      <c r="L2" s="275"/>
-      <c r="M2" s="275"/>
-      <c r="N2" s="275"/>
-      <c r="O2" s="275"/>
-      <c r="P2" s="275"/>
-      <c r="Q2" s="275"/>
-      <c r="R2" s="275"/>
-      <c r="S2" s="275"/>
-      <c r="T2" s="275"/>
-      <c r="U2" s="275"/>
-      <c r="V2" s="275"/>
-      <c r="W2" s="275"/>
-      <c r="X2" s="275"/>
-      <c r="Y2" s="275"/>
-      <c r="Z2" s="275"/>
-      <c r="AA2" s="275"/>
-      <c r="AB2" s="275"/>
-      <c r="AC2" s="275"/>
-      <c r="AD2" s="275"/>
-      <c r="AE2" s="275"/>
-      <c r="AF2" s="275"/>
-      <c r="AG2" s="275"/>
-      <c r="AH2" s="275"/>
-      <c r="AI2" s="275"/>
-      <c r="AJ2" s="275"/>
-      <c r="AK2" s="275"/>
-      <c r="AL2" s="275"/>
-      <c r="AM2" s="275"/>
-      <c r="AN2" s="275"/>
-      <c r="AO2" s="275"/>
-      <c r="AP2" s="275"/>
-      <c r="AQ2" s="275"/>
-      <c r="AR2" s="275"/>
-      <c r="AS2" s="275"/>
-      <c r="AT2" s="275"/>
-      <c r="AU2" s="275"/>
-      <c r="AV2" s="275"/>
-      <c r="AW2" s="275"/>
-      <c r="AX2" s="275"/>
-      <c r="AY2" s="275"/>
-      <c r="AZ2" s="275"/>
-      <c r="BA2" s="275"/>
-      <c r="BB2" s="275"/>
-      <c r="BC2" s="275"/>
-      <c r="BD2" s="276"/>
+      <c r="G2" s="269"/>
+      <c r="H2" s="269"/>
+      <c r="I2" s="269"/>
+      <c r="J2" s="269"/>
+      <c r="K2" s="269"/>
+      <c r="L2" s="269"/>
+      <c r="M2" s="269"/>
+      <c r="N2" s="269"/>
+      <c r="O2" s="269"/>
+      <c r="P2" s="269"/>
+      <c r="Q2" s="269"/>
+      <c r="R2" s="269"/>
+      <c r="S2" s="269"/>
+      <c r="T2" s="269"/>
+      <c r="U2" s="269"/>
+      <c r="V2" s="269"/>
+      <c r="W2" s="269"/>
+      <c r="X2" s="269"/>
+      <c r="Y2" s="269"/>
+      <c r="Z2" s="269"/>
+      <c r="AA2" s="269"/>
+      <c r="AB2" s="269"/>
+      <c r="AC2" s="269"/>
+      <c r="AD2" s="269"/>
+      <c r="AE2" s="269"/>
+      <c r="AF2" s="269"/>
+      <c r="AG2" s="269"/>
+      <c r="AH2" s="269"/>
+      <c r="AI2" s="269"/>
+      <c r="AJ2" s="269"/>
+      <c r="AK2" s="269"/>
+      <c r="AL2" s="269"/>
+      <c r="AM2" s="269"/>
+      <c r="AN2" s="269"/>
+      <c r="AO2" s="269"/>
+      <c r="AP2" s="269"/>
+      <c r="AQ2" s="269"/>
+      <c r="AR2" s="269"/>
+      <c r="AS2" s="269"/>
+      <c r="AT2" s="269"/>
+      <c r="AU2" s="269"/>
+      <c r="AV2" s="269"/>
+      <c r="AW2" s="269"/>
+      <c r="AX2" s="269"/>
+      <c r="AY2" s="269"/>
+      <c r="AZ2" s="269"/>
+      <c r="BA2" s="269"/>
+      <c r="BB2" s="269"/>
+      <c r="BC2" s="269"/>
+      <c r="BD2" s="270"/>
     </row>
     <row r="3" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="239" t="s">
+      <c r="A3" s="233" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="240"/>
+      <c r="B3" s="234"/>
       <c r="C3" s="141" t="s">
         <v>286</v>
       </c>
-      <c r="D3" s="268" t="s">
+      <c r="D3" s="262" t="s">
         <v>328</v>
       </c>
-      <c r="E3" s="268"/>
+      <c r="E3" s="262"/>
       <c r="F3" s="145">
         <v>75263586</v>
       </c>
       <c r="G3" s="145"/>
       <c r="H3" s="145"/>
-      <c r="I3" s="268" t="s">
+      <c r="I3" s="262" t="s">
         <v>332</v>
       </c>
-      <c r="J3" s="268"/>
-      <c r="K3" s="268"/>
-      <c r="L3" s="268"/>
-      <c r="M3" s="268"/>
-      <c r="N3" s="268"/>
-      <c r="O3" s="268"/>
-      <c r="P3" s="268"/>
-      <c r="Q3" s="268"/>
-      <c r="R3" s="278" t="s">
+      <c r="J3" s="262"/>
+      <c r="K3" s="262"/>
+      <c r="L3" s="262"/>
+      <c r="M3" s="262"/>
+      <c r="N3" s="262"/>
+      <c r="O3" s="262"/>
+      <c r="P3" s="262"/>
+      <c r="Q3" s="262"/>
+      <c r="R3" s="272" t="s">
         <v>334</v>
       </c>
-      <c r="S3" s="278"/>
-      <c r="T3" s="278"/>
-      <c r="U3" s="278"/>
-      <c r="V3" s="278"/>
-      <c r="W3" s="278"/>
-      <c r="X3" s="278"/>
+      <c r="S3" s="272"/>
+      <c r="T3" s="272"/>
+      <c r="U3" s="272"/>
+      <c r="V3" s="272"/>
+      <c r="W3" s="272"/>
+      <c r="X3" s="272"/>
       <c r="Y3" s="143"/>
       <c r="Z3" s="143"/>
       <c r="AA3" s="143"/>
@@ -4583,42 +4513,42 @@
       <c r="BD3" s="139"/>
     </row>
     <row r="4" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="239" t="s">
+      <c r="A4" s="233" t="s">
         <v>296</v>
       </c>
-      <c r="B4" s="240"/>
+      <c r="B4" s="234"/>
       <c r="C4" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D4" s="268" t="s">
+      <c r="D4" s="262" t="s">
         <v>329</v>
       </c>
-      <c r="E4" s="268"/>
+      <c r="E4" s="262"/>
       <c r="F4" s="145">
         <v>99826036</v>
       </c>
       <c r="G4" s="145"/>
       <c r="H4" s="145"/>
-      <c r="I4" s="268" t="s">
+      <c r="I4" s="262" t="s">
         <v>333</v>
       </c>
-      <c r="J4" s="268"/>
-      <c r="K4" s="268"/>
-      <c r="L4" s="268"/>
-      <c r="M4" s="268"/>
-      <c r="N4" s="268"/>
-      <c r="O4" s="268"/>
-      <c r="P4" s="268"/>
-      <c r="Q4" s="268"/>
-      <c r="R4" s="278" t="s">
+      <c r="J4" s="262"/>
+      <c r="K4" s="262"/>
+      <c r="L4" s="262"/>
+      <c r="M4" s="262"/>
+      <c r="N4" s="262"/>
+      <c r="O4" s="262"/>
+      <c r="P4" s="262"/>
+      <c r="Q4" s="262"/>
+      <c r="R4" s="272" t="s">
         <v>335</v>
       </c>
-      <c r="S4" s="278"/>
-      <c r="T4" s="278"/>
-      <c r="U4" s="278"/>
-      <c r="V4" s="278"/>
-      <c r="W4" s="278"/>
-      <c r="X4" s="278"/>
+      <c r="S4" s="272"/>
+      <c r="T4" s="272"/>
+      <c r="U4" s="272"/>
+      <c r="V4" s="272"/>
+      <c r="W4" s="272"/>
+      <c r="X4" s="272"/>
       <c r="Y4" s="143"/>
       <c r="Z4" s="143"/>
       <c r="AA4" s="143"/>
@@ -4653,35 +4583,35 @@
       <c r="BD4" s="139"/>
     </row>
     <row r="5" spans="1:56" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="241" t="s">
+      <c r="A5" s="235" t="s">
         <v>302</v>
       </c>
-      <c r="B5" s="242"/>
+      <c r="B5" s="236"/>
       <c r="C5" s="142" t="s">
         <v>288</v>
       </c>
-      <c r="D5" s="244" t="s">
+      <c r="D5" s="238" t="s">
         <v>330</v>
       </c>
-      <c r="E5" s="244"/>
-      <c r="F5" s="277" t="s">
+      <c r="E5" s="238"/>
+      <c r="F5" s="271" t="s">
         <v>331</v>
       </c>
-      <c r="G5" s="277"/>
-      <c r="H5" s="277"/>
-      <c r="I5" s="277"/>
-      <c r="J5" s="277"/>
-      <c r="K5" s="277"/>
-      <c r="L5" s="277"/>
-      <c r="M5" s="277"/>
-      <c r="N5" s="277"/>
-      <c r="O5" s="277"/>
-      <c r="P5" s="277"/>
-      <c r="Q5" s="277"/>
-      <c r="R5" s="277"/>
-      <c r="S5" s="277"/>
-      <c r="T5" s="277"/>
-      <c r="U5" s="277"/>
+      <c r="G5" s="271"/>
+      <c r="H5" s="271"/>
+      <c r="I5" s="271"/>
+      <c r="J5" s="271"/>
+      <c r="K5" s="271"/>
+      <c r="L5" s="271"/>
+      <c r="M5" s="271"/>
+      <c r="N5" s="271"/>
+      <c r="O5" s="271"/>
+      <c r="P5" s="271"/>
+      <c r="Q5" s="271"/>
+      <c r="R5" s="271"/>
+      <c r="S5" s="271"/>
+      <c r="T5" s="271"/>
+      <c r="U5" s="271"/>
       <c r="V5" s="144"/>
       <c r="W5" s="144"/>
       <c r="X5" s="144"/>
@@ -4719,101 +4649,101 @@
       <c r="BD5" s="140"/>
     </row>
     <row r="6" spans="1:56" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="248" t="s">
+      <c r="A6" s="242" t="s">
         <v>310</v>
       </c>
-      <c r="B6" s="250" t="s">
+      <c r="B6" s="244" t="s">
         <v>160</v>
       </c>
-      <c r="C6" s="250" t="s">
+      <c r="C6" s="244" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="250" t="s">
+      <c r="D6" s="244" t="s">
         <v>292</v>
       </c>
-      <c r="E6" s="257" t="s">
+      <c r="E6" s="251" t="s">
         <v>159</v>
       </c>
-      <c r="F6" s="258"/>
-      <c r="G6" s="255" t="s">
+      <c r="F6" s="252"/>
+      <c r="G6" s="249" t="s">
         <v>293</v>
       </c>
-      <c r="H6" s="245" t="s">
+      <c r="H6" s="239" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="246"/>
-      <c r="J6" s="246"/>
-      <c r="K6" s="246"/>
-      <c r="L6" s="246"/>
-      <c r="M6" s="246"/>
-      <c r="N6" s="247"/>
-      <c r="O6" s="245" t="s">
+      <c r="I6" s="240"/>
+      <c r="J6" s="240"/>
+      <c r="K6" s="240"/>
+      <c r="L6" s="240"/>
+      <c r="M6" s="240"/>
+      <c r="N6" s="241"/>
+      <c r="O6" s="239" t="s">
         <v>136</v>
       </c>
-      <c r="P6" s="246"/>
-      <c r="Q6" s="246"/>
-      <c r="R6" s="246"/>
-      <c r="S6" s="246"/>
-      <c r="T6" s="246"/>
-      <c r="U6" s="247"/>
-      <c r="V6" s="245" t="s">
+      <c r="P6" s="240"/>
+      <c r="Q6" s="240"/>
+      <c r="R6" s="240"/>
+      <c r="S6" s="240"/>
+      <c r="T6" s="240"/>
+      <c r="U6" s="241"/>
+      <c r="V6" s="239" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="246"/>
-      <c r="X6" s="246"/>
-      <c r="Y6" s="246"/>
-      <c r="Z6" s="246"/>
-      <c r="AA6" s="246"/>
-      <c r="AB6" s="247"/>
-      <c r="AC6" s="245" t="s">
+      <c r="W6" s="240"/>
+      <c r="X6" s="240"/>
+      <c r="Y6" s="240"/>
+      <c r="Z6" s="240"/>
+      <c r="AA6" s="240"/>
+      <c r="AB6" s="241"/>
+      <c r="AC6" s="239" t="s">
         <v>137</v>
       </c>
-      <c r="AD6" s="246"/>
-      <c r="AE6" s="246"/>
-      <c r="AF6" s="246"/>
-      <c r="AG6" s="246"/>
-      <c r="AH6" s="246"/>
-      <c r="AI6" s="247"/>
-      <c r="AJ6" s="245" t="s">
+      <c r="AD6" s="240"/>
+      <c r="AE6" s="240"/>
+      <c r="AF6" s="240"/>
+      <c r="AG6" s="240"/>
+      <c r="AH6" s="240"/>
+      <c r="AI6" s="241"/>
+      <c r="AJ6" s="239" t="s">
         <v>84</v>
       </c>
-      <c r="AK6" s="246"/>
-      <c r="AL6" s="246"/>
-      <c r="AM6" s="246"/>
-      <c r="AN6" s="246"/>
-      <c r="AO6" s="246"/>
-      <c r="AP6" s="247"/>
-      <c r="AQ6" s="245" t="s">
+      <c r="AK6" s="240"/>
+      <c r="AL6" s="240"/>
+      <c r="AM6" s="240"/>
+      <c r="AN6" s="240"/>
+      <c r="AO6" s="240"/>
+      <c r="AP6" s="241"/>
+      <c r="AQ6" s="239" t="s">
         <v>138</v>
       </c>
-      <c r="AR6" s="246"/>
-      <c r="AS6" s="246"/>
-      <c r="AT6" s="246"/>
-      <c r="AU6" s="246"/>
-      <c r="AV6" s="246"/>
-      <c r="AW6" s="247"/>
-      <c r="AX6" s="245" t="s">
+      <c r="AR6" s="240"/>
+      <c r="AS6" s="240"/>
+      <c r="AT6" s="240"/>
+      <c r="AU6" s="240"/>
+      <c r="AV6" s="240"/>
+      <c r="AW6" s="241"/>
+      <c r="AX6" s="239" t="s">
         <v>139</v>
       </c>
-      <c r="AY6" s="246"/>
-      <c r="AZ6" s="246"/>
-      <c r="BA6" s="246"/>
-      <c r="BB6" s="246"/>
-      <c r="BC6" s="246"/>
-      <c r="BD6" s="247"/>
+      <c r="AY6" s="240"/>
+      <c r="AZ6" s="240"/>
+      <c r="BA6" s="240"/>
+      <c r="BB6" s="240"/>
+      <c r="BC6" s="240"/>
+      <c r="BD6" s="241"/>
     </row>
     <row r="7" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="249"/>
-      <c r="B7" s="251"/>
-      <c r="C7" s="251"/>
-      <c r="D7" s="251"/>
+      <c r="A7" s="243"/>
+      <c r="B7" s="245"/>
+      <c r="C7" s="245"/>
+      <c r="D7" s="245"/>
       <c r="E7" s="154" t="s">
         <v>158</v>
       </c>
       <c r="F7" s="154" t="s">
         <v>309</v>
       </c>
-      <c r="G7" s="256"/>
+      <c r="G7" s="250"/>
       <c r="H7" s="155" t="s">
         <v>297</v>
       </c>
@@ -5087,7 +5017,7 @@
       <c r="BD9" s="89"/>
     </row>
     <row r="10" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="252" t="s">
+      <c r="A10" s="246" t="s">
         <v>311</v>
       </c>
       <c r="B10" s="135"/>
@@ -5155,7 +5085,7 @@
       <c r="BD10" s="89"/>
     </row>
     <row r="11" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="253"/>
+      <c r="A11" s="247"/>
       <c r="B11" s="135"/>
       <c r="C11" s="90" t="s">
         <v>291</v>
@@ -5221,7 +5151,7 @@
       <c r="BD11" s="89"/>
     </row>
     <row r="12" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="254"/>
+      <c r="A12" s="248"/>
       <c r="B12" s="135"/>
       <c r="C12" s="90" t="s">
         <v>89</v>
@@ -5411,7 +5341,7 @@
       <c r="BD14" s="89"/>
     </row>
     <row r="15" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="252" t="s">
+      <c r="A15" s="246" t="s">
         <v>312</v>
       </c>
       <c r="B15" s="135"/>
@@ -5481,7 +5411,7 @@
       <c r="BD15" s="89"/>
     </row>
     <row r="16" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="253"/>
+      <c r="A16" s="247"/>
       <c r="B16" s="135"/>
       <c r="C16" s="95" t="s">
         <v>104</v>
@@ -5549,7 +5479,7 @@
       <c r="BD16" s="89"/>
     </row>
     <row r="17" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="253"/>
+      <c r="A17" s="247"/>
       <c r="B17" s="135"/>
       <c r="C17" s="95" t="s">
         <v>105</v>
@@ -5617,7 +5547,7 @@
       <c r="BD17" s="89"/>
     </row>
     <row r="18" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="253"/>
+      <c r="A18" s="247"/>
       <c r="B18" s="135"/>
       <c r="C18" s="95" t="s">
         <v>106</v>
@@ -5685,7 +5615,7 @@
       <c r="BD18" s="89"/>
     </row>
     <row r="19" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="253"/>
+      <c r="A19" s="247"/>
       <c r="B19" s="135"/>
       <c r="C19" s="95" t="s">
         <v>99</v>
@@ -5753,7 +5683,7 @@
       <c r="BD19" s="89"/>
     </row>
     <row r="20" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="253"/>
+      <c r="A20" s="247"/>
       <c r="B20" s="135"/>
       <c r="C20" s="95" t="s">
         <v>107</v>
@@ -5821,7 +5751,7 @@
       <c r="BD20" s="89"/>
     </row>
     <row r="21" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="253"/>
+      <c r="A21" s="247"/>
       <c r="B21" s="135"/>
       <c r="C21" s="95" t="s">
         <v>108</v>
@@ -5889,7 +5819,7 @@
       <c r="BD21" s="89"/>
     </row>
     <row r="22" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="253"/>
+      <c r="A22" s="247"/>
       <c r="B22" s="135"/>
       <c r="C22" s="95" t="s">
         <v>109</v>
@@ -5957,7 +5887,7 @@
       <c r="BD22" s="89"/>
     </row>
     <row r="23" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="253"/>
+      <c r="A23" s="247"/>
       <c r="B23" s="135"/>
       <c r="C23" s="95" t="s">
         <v>110</v>
@@ -6025,7 +5955,7 @@
       <c r="BD23" s="89"/>
     </row>
     <row r="24" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="253"/>
+      <c r="A24" s="247"/>
       <c r="B24" s="135"/>
       <c r="C24" s="95" t="s">
         <v>111</v>
@@ -6093,7 +6023,7 @@
       <c r="BD24" s="89"/>
     </row>
     <row r="25" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="253"/>
+      <c r="A25" s="247"/>
       <c r="B25" s="135"/>
       <c r="C25" s="95" t="s">
         <v>112</v>
@@ -6161,7 +6091,7 @@
       <c r="BD25" s="89"/>
     </row>
     <row r="26" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="253"/>
+      <c r="A26" s="247"/>
       <c r="B26" s="135"/>
       <c r="C26" s="95" t="s">
         <v>113</v>
@@ -6229,7 +6159,7 @@
       <c r="BD26" s="89"/>
     </row>
     <row r="27" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="253"/>
+      <c r="A27" s="247"/>
       <c r="B27" s="135"/>
       <c r="C27" s="95" t="s">
         <v>114</v>
@@ -6297,7 +6227,7 @@
       <c r="BD27" s="89"/>
     </row>
     <row r="28" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="253"/>
+      <c r="A28" s="247"/>
       <c r="B28" s="135"/>
       <c r="C28" s="95" t="s">
         <v>115</v>
@@ -6365,7 +6295,7 @@
       <c r="BD28" s="89"/>
     </row>
     <row r="29" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="253"/>
+      <c r="A29" s="247"/>
       <c r="B29" s="135"/>
       <c r="C29" s="95" t="s">
         <v>116</v>
@@ -6433,7 +6363,7 @@
       <c r="BD29" s="89"/>
     </row>
     <row r="30" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="254"/>
+      <c r="A30" s="248"/>
       <c r="B30" s="135"/>
       <c r="C30" s="95" t="s">
         <v>117</v>
@@ -6563,7 +6493,7 @@
       <c r="BD31" s="89"/>
     </row>
     <row r="32" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="252" t="s">
+      <c r="A32" s="246" t="s">
         <v>313</v>
       </c>
       <c r="B32" s="135"/>
@@ -6631,7 +6561,7 @@
       <c r="BD32" s="89"/>
     </row>
     <row r="33" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="253"/>
+      <c r="A33" s="247"/>
       <c r="B33" s="135"/>
       <c r="C33" s="95" t="s">
         <v>105</v>
@@ -6697,7 +6627,7 @@
       <c r="BD33" s="89"/>
     </row>
     <row r="34" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="253"/>
+      <c r="A34" s="247"/>
       <c r="B34" s="135"/>
       <c r="C34" s="95" t="s">
         <v>108</v>
@@ -6763,7 +6693,7 @@
       <c r="BD34" s="89"/>
     </row>
     <row r="35" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="254"/>
+      <c r="A35" s="248"/>
       <c r="B35" s="135"/>
       <c r="C35" s="95" t="s">
         <v>91</v>
@@ -6891,7 +6821,7 @@
       <c r="BD36" s="89"/>
     </row>
     <row r="37" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="252" t="s">
+      <c r="A37" s="246" t="s">
         <v>314</v>
       </c>
       <c r="B37" s="136" t="s">
@@ -6955,7 +6885,7 @@
       <c r="BD37" s="89"/>
     </row>
     <row r="38" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="253"/>
+      <c r="A38" s="247"/>
       <c r="B38" s="137" t="s">
         <v>164</v>
       </c>
@@ -7023,7 +6953,7 @@
       <c r="BD38" s="89"/>
     </row>
     <row r="39" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="253"/>
+      <c r="A39" s="247"/>
       <c r="B39" s="137" t="s">
         <v>165</v>
       </c>
@@ -7091,7 +7021,7 @@
       <c r="BD39" s="89"/>
     </row>
     <row r="40" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="253"/>
+      <c r="A40" s="247"/>
       <c r="B40" s="136" t="s">
         <v>225</v>
       </c>
@@ -7153,7 +7083,7 @@
       <c r="BD40" s="89"/>
     </row>
     <row r="41" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="253"/>
+      <c r="A41" s="247"/>
       <c r="B41" s="137" t="s">
         <v>226</v>
       </c>
@@ -7221,7 +7151,7 @@
       <c r="BD41" s="89"/>
     </row>
     <row r="42" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="253"/>
+      <c r="A42" s="247"/>
       <c r="B42" s="136" t="s">
         <v>227</v>
       </c>
@@ -7283,7 +7213,7 @@
       <c r="BD42" s="89"/>
     </row>
     <row r="43" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="253"/>
+      <c r="A43" s="247"/>
       <c r="B43" s="137" t="s">
         <v>228</v>
       </c>
@@ -7347,7 +7277,7 @@
       <c r="BD43" s="89"/>
     </row>
     <row r="44" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="253"/>
+      <c r="A44" s="247"/>
       <c r="B44" s="135"/>
       <c r="C44" s="90" t="s">
         <v>174</v>
@@ -7413,7 +7343,7 @@
       <c r="BD44" s="89"/>
     </row>
     <row r="45" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="253"/>
+      <c r="A45" s="247"/>
       <c r="B45" s="135"/>
       <c r="C45" s="90" t="s">
         <v>173</v>
@@ -7479,7 +7409,7 @@
       <c r="BD45" s="89"/>
     </row>
     <row r="46" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="253"/>
+      <c r="A46" s="247"/>
       <c r="B46" s="136" t="s">
         <v>229</v>
       </c>
@@ -7541,7 +7471,7 @@
       <c r="BD46" s="89"/>
     </row>
     <row r="47" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="253"/>
+      <c r="A47" s="247"/>
       <c r="B47" s="137" t="s">
         <v>230</v>
       </c>
@@ -7609,7 +7539,7 @@
       <c r="BD47" s="89"/>
     </row>
     <row r="48" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="253"/>
+      <c r="A48" s="247"/>
       <c r="B48" s="137" t="s">
         <v>231</v>
       </c>
@@ -7677,7 +7607,7 @@
       <c r="BD48" s="89"/>
     </row>
     <row r="49" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="253"/>
+      <c r="A49" s="247"/>
       <c r="B49" s="137" t="s">
         <v>232</v>
       </c>
@@ -7745,7 +7675,7 @@
       <c r="BD49" s="89"/>
     </row>
     <row r="50" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="253"/>
+      <c r="A50" s="247"/>
       <c r="B50" s="137" t="s">
         <v>233</v>
       </c>
@@ -7813,7 +7743,7 @@
       <c r="BD50" s="89"/>
     </row>
     <row r="51" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="253"/>
+      <c r="A51" s="247"/>
       <c r="B51" s="136" t="s">
         <v>234</v>
       </c>
@@ -7875,7 +7805,7 @@
       <c r="BD51" s="89"/>
     </row>
     <row r="52" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="253"/>
+      <c r="A52" s="247"/>
       <c r="B52" s="137" t="s">
         <v>235</v>
       </c>
@@ -7943,7 +7873,7 @@
       <c r="BD52" s="89"/>
     </row>
     <row r="53" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="253"/>
+      <c r="A53" s="247"/>
       <c r="B53" s="137" t="s">
         <v>236</v>
       </c>
@@ -8011,7 +7941,7 @@
       <c r="BD53" s="89"/>
     </row>
     <row r="54" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="253"/>
+      <c r="A54" s="247"/>
       <c r="B54" s="136" t="s">
         <v>237</v>
       </c>
@@ -8073,7 +8003,7 @@
       <c r="BD54" s="89"/>
     </row>
     <row r="55" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="253"/>
+      <c r="A55" s="247"/>
       <c r="B55" s="137" t="s">
         <v>238</v>
       </c>
@@ -8139,7 +8069,7 @@
       <c r="BD55" s="89"/>
     </row>
     <row r="56" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="253"/>
+      <c r="A56" s="247"/>
       <c r="B56" s="135"/>
       <c r="C56" s="90" t="s">
         <v>183</v>
@@ -8207,7 +8137,7 @@
       <c r="BD56" s="89"/>
     </row>
     <row r="57" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="253"/>
+      <c r="A57" s="247"/>
       <c r="B57" s="135"/>
       <c r="C57" s="90" t="s">
         <v>182</v>
@@ -8275,7 +8205,7 @@
       <c r="BD57" s="89"/>
     </row>
     <row r="58" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="253"/>
+      <c r="A58" s="247"/>
       <c r="B58" s="137" t="s">
         <v>239</v>
       </c>
@@ -8341,7 +8271,7 @@
       <c r="BD58" s="89"/>
     </row>
     <row r="59" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="253"/>
+      <c r="A59" s="247"/>
       <c r="B59" s="135"/>
       <c r="C59" s="90" t="s">
         <v>282</v>
@@ -8409,7 +8339,7 @@
       <c r="BD59" s="89"/>
     </row>
     <row r="60" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="253"/>
+      <c r="A60" s="247"/>
       <c r="B60" s="135"/>
       <c r="C60" s="90" t="s">
         <v>283</v>
@@ -8477,7 +8407,7 @@
       <c r="BD60" s="89"/>
     </row>
     <row r="61" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="253"/>
+      <c r="A61" s="247"/>
       <c r="B61" s="136" t="s">
         <v>240</v>
       </c>
@@ -8539,7 +8469,7 @@
       <c r="BD61" s="89"/>
     </row>
     <row r="62" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="253"/>
+      <c r="A62" s="247"/>
       <c r="B62" s="137" t="s">
         <v>241</v>
       </c>
@@ -8607,7 +8537,7 @@
       <c r="BD62" s="89"/>
     </row>
     <row r="63" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="253"/>
+      <c r="A63" s="247"/>
       <c r="B63" s="137" t="s">
         <v>242</v>
       </c>
@@ -8675,7 +8605,7 @@
       <c r="BD63" s="89"/>
     </row>
     <row r="64" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="253"/>
+      <c r="A64" s="247"/>
       <c r="B64" s="136" t="s">
         <v>243</v>
       </c>
@@ -8737,7 +8667,7 @@
       <c r="BD64" s="89"/>
     </row>
     <row r="65" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="253"/>
+      <c r="A65" s="247"/>
       <c r="B65" s="137" t="s">
         <v>244</v>
       </c>
@@ -8805,7 +8735,7 @@
       <c r="BD65" s="89"/>
     </row>
     <row r="66" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="253"/>
+      <c r="A66" s="247"/>
       <c r="B66" s="136" t="s">
         <v>247</v>
       </c>
@@ -8867,7 +8797,7 @@
       <c r="BD66" s="89"/>
     </row>
     <row r="67" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="253"/>
+      <c r="A67" s="247"/>
       <c r="B67" s="137" t="s">
         <v>248</v>
       </c>
@@ -8935,7 +8865,7 @@
       <c r="BD67" s="89"/>
     </row>
     <row r="68" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="253"/>
+      <c r="A68" s="247"/>
       <c r="B68" s="136" t="s">
         <v>251</v>
       </c>
@@ -8997,7 +8927,7 @@
       <c r="BD68" s="89"/>
     </row>
     <row r="69" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="253"/>
+      <c r="A69" s="247"/>
       <c r="B69" s="137" t="s">
         <v>252</v>
       </c>
@@ -9065,7 +8995,7 @@
       <c r="BD69" s="89"/>
     </row>
     <row r="70" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="253"/>
+      <c r="A70" s="247"/>
       <c r="B70" s="137" t="s">
         <v>253</v>
       </c>
@@ -9133,7 +9063,7 @@
       <c r="BD70" s="89"/>
     </row>
     <row r="71" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="253"/>
+      <c r="A71" s="247"/>
       <c r="B71" s="136" t="s">
         <v>254</v>
       </c>
@@ -9195,7 +9125,7 @@
       <c r="BD71" s="89"/>
     </row>
     <row r="72" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="253"/>
+      <c r="A72" s="247"/>
       <c r="B72" s="137" t="s">
         <v>255</v>
       </c>
@@ -9263,7 +9193,7 @@
       <c r="BD72" s="89"/>
     </row>
     <row r="73" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="253"/>
+      <c r="A73" s="247"/>
       <c r="B73" s="136" t="s">
         <v>256</v>
       </c>
@@ -9325,7 +9255,7 @@
       <c r="BD73" s="89"/>
     </row>
     <row r="74" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="254"/>
+      <c r="A74" s="248"/>
       <c r="B74" s="137" t="s">
         <v>257</v>
       </c>
@@ -9517,7 +9447,7 @@
       <c r="BD76" s="89"/>
     </row>
     <row r="77" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="252" t="s">
+      <c r="A77" s="246" t="s">
         <v>162</v>
       </c>
       <c r="B77" s="135"/>
@@ -9585,7 +9515,7 @@
       <c r="BD77" s="89"/>
     </row>
     <row r="78" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="254"/>
+      <c r="A78" s="248"/>
       <c r="B78" s="135"/>
       <c r="C78" s="90" t="s">
         <v>95</v>
@@ -9713,7 +9643,7 @@
       <c r="BD79" s="89"/>
     </row>
     <row r="80" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="252" t="s">
+      <c r="A80" s="246" t="s">
         <v>162</v>
       </c>
       <c r="B80" s="135"/>
@@ -9781,7 +9711,7 @@
       <c r="BD80" s="89"/>
     </row>
     <row r="81" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="254"/>
+      <c r="A81" s="248"/>
       <c r="B81" s="135"/>
       <c r="C81" s="90" t="s">
         <v>93</v>
@@ -9909,7 +9839,7 @@
       <c r="BD82" s="89"/>
     </row>
     <row r="83" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="252" t="s">
+      <c r="A83" s="246" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="135"/>
@@ -9977,7 +9907,7 @@
       <c r="BD83" s="89"/>
     </row>
     <row r="84" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="254"/>
+      <c r="A84" s="248"/>
       <c r="B84" s="135"/>
       <c r="C84" s="90" t="s">
         <v>134</v>
@@ -10167,7 +10097,7 @@
       <c r="BD86" s="89"/>
     </row>
     <row r="87" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="252" t="s">
+      <c r="A87" s="246" t="s">
         <v>316</v>
       </c>
       <c r="B87" s="135"/>
@@ -10235,7 +10165,7 @@
       <c r="BD87" s="89"/>
     </row>
     <row r="88" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="253"/>
+      <c r="A88" s="247"/>
       <c r="B88" s="135"/>
       <c r="C88" s="95" t="s">
         <v>119</v>
@@ -10301,7 +10231,7 @@
       <c r="BD88" s="89"/>
     </row>
     <row r="89" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="253"/>
+      <c r="A89" s="247"/>
       <c r="B89" s="135"/>
       <c r="C89" s="95" t="s">
         <v>120</v>
@@ -10367,7 +10297,7 @@
       <c r="BD89" s="89"/>
     </row>
     <row r="90" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="253"/>
+      <c r="A90" s="247"/>
       <c r="B90" s="135"/>
       <c r="C90" s="95" t="s">
         <v>121</v>
@@ -10433,7 +10363,7 @@
       <c r="BD90" s="89"/>
     </row>
     <row r="91" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="253"/>
+      <c r="A91" s="247"/>
       <c r="B91" s="135"/>
       <c r="C91" s="95" t="s">
         <v>122</v>
@@ -10499,7 +10429,7 @@
       <c r="BD91" s="89"/>
     </row>
     <row r="92" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="253"/>
+      <c r="A92" s="247"/>
       <c r="B92" s="135"/>
       <c r="C92" s="95" t="s">
         <v>123</v>
@@ -10565,7 +10495,7 @@
       <c r="BD92" s="89"/>
     </row>
     <row r="93" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="253"/>
+      <c r="A93" s="247"/>
       <c r="B93" s="135"/>
       <c r="C93" s="95" t="s">
         <v>124</v>
@@ -10631,7 +10561,7 @@
       <c r="BD93" s="89"/>
     </row>
     <row r="94" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="253"/>
+      <c r="A94" s="247"/>
       <c r="B94" s="135"/>
       <c r="C94" s="95" t="s">
         <v>125</v>
@@ -10697,7 +10627,7 @@
       <c r="BD94" s="89"/>
     </row>
     <row r="95" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="253"/>
+      <c r="A95" s="247"/>
       <c r="B95" s="135"/>
       <c r="C95" s="95" t="s">
         <v>126</v>
@@ -10763,7 +10693,7 @@
       <c r="BD95" s="89"/>
     </row>
     <row r="96" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="253"/>
+      <c r="A96" s="247"/>
       <c r="B96" s="135"/>
       <c r="C96" s="95" t="s">
         <v>127</v>
@@ -10829,7 +10759,7 @@
       <c r="BD96" s="89"/>
     </row>
     <row r="97" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="253"/>
+      <c r="A97" s="247"/>
       <c r="B97" s="135"/>
       <c r="C97" s="95" t="s">
         <v>128</v>
@@ -10895,7 +10825,7 @@
       <c r="BD97" s="89"/>
     </row>
     <row r="98" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="253"/>
+      <c r="A98" s="247"/>
       <c r="B98" s="135"/>
       <c r="C98" s="95" t="s">
         <v>129</v>
@@ -10961,7 +10891,7 @@
       <c r="BD98" s="89"/>
     </row>
     <row r="99" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="253"/>
+      <c r="A99" s="247"/>
       <c r="B99" s="135"/>
       <c r="C99" s="95" t="s">
         <v>130</v>
@@ -11027,7 +10957,7 @@
       <c r="BD99" s="89"/>
     </row>
     <row r="100" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="253"/>
+      <c r="A100" s="247"/>
       <c r="B100" s="135"/>
       <c r="C100" s="95" t="s">
         <v>131</v>
@@ -11093,7 +11023,7 @@
       <c r="BD100" s="89"/>
     </row>
     <row r="101" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="253"/>
+      <c r="A101" s="247"/>
       <c r="B101" s="135"/>
       <c r="C101" s="95" t="s">
         <v>132</v>
@@ -11159,7 +11089,7 @@
       <c r="BD101" s="89"/>
     </row>
     <row r="102" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="254"/>
+      <c r="A102" s="248"/>
       <c r="B102" s="135"/>
       <c r="C102" s="95" t="s">
         <v>133</v>
@@ -11287,7 +11217,7 @@
       <c r="BD103" s="89"/>
     </row>
     <row r="104" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="252" t="s">
+      <c r="A104" s="246" t="s">
         <v>315</v>
       </c>
       <c r="B104" s="136" t="s">
@@ -11351,7 +11281,7 @@
       <c r="BD104" s="89"/>
     </row>
     <row r="105" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="253"/>
+      <c r="A105" s="247"/>
       <c r="B105" s="137">
         <v>3.0101010000000001</v>
       </c>
@@ -11419,7 +11349,7 @@
       <c r="BD105" s="89"/>
     </row>
     <row r="106" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="253"/>
+      <c r="A106" s="247"/>
       <c r="B106" s="136" t="s">
         <v>224</v>
       </c>
@@ -11481,7 +11411,7 @@
       <c r="BD106" s="89"/>
     </row>
     <row r="107" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="253"/>
+      <c r="A107" s="247"/>
       <c r="B107" s="137" t="s">
         <v>164</v>
       </c>
@@ -11549,7 +11479,7 @@
       <c r="BD107" s="89"/>
     </row>
     <row r="108" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="253"/>
+      <c r="A108" s="247"/>
       <c r="B108" s="137" t="s">
         <v>165</v>
       </c>
@@ -11617,7 +11547,7 @@
       <c r="BD108" s="89"/>
     </row>
     <row r="109" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="253"/>
+      <c r="A109" s="247"/>
       <c r="B109" s="136" t="s">
         <v>225</v>
       </c>
@@ -11679,7 +11609,7 @@
       <c r="BD109" s="89"/>
     </row>
     <row r="110" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="253"/>
+      <c r="A110" s="247"/>
       <c r="B110" s="137" t="s">
         <v>226</v>
       </c>
@@ -11747,7 +11677,7 @@
       <c r="BD110" s="89"/>
     </row>
     <row r="111" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="253"/>
+      <c r="A111" s="247"/>
       <c r="B111" s="136" t="s">
         <v>227</v>
       </c>
@@ -11809,7 +11739,7 @@
       <c r="BD111" s="89"/>
     </row>
     <row r="112" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="253"/>
+      <c r="A112" s="247"/>
       <c r="B112" s="137" t="s">
         <v>228</v>
       </c>
@@ -11877,7 +11807,7 @@
       <c r="BD112" s="89"/>
     </row>
     <row r="113" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="253"/>
+      <c r="A113" s="247"/>
       <c r="B113" s="135"/>
       <c r="C113" s="90" t="s">
         <v>174</v>
@@ -11943,7 +11873,7 @@
       <c r="BD113" s="89"/>
     </row>
     <row r="114" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="253"/>
+      <c r="A114" s="247"/>
       <c r="B114" s="135"/>
       <c r="C114" s="90" t="s">
         <v>173</v>
@@ -12009,7 +11939,7 @@
       <c r="BD114" s="89"/>
     </row>
     <row r="115" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="253"/>
+      <c r="A115" s="247"/>
       <c r="B115" s="136" t="s">
         <v>229</v>
       </c>
@@ -12071,7 +12001,7 @@
       <c r="BD115" s="89"/>
     </row>
     <row r="116" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="253"/>
+      <c r="A116" s="247"/>
       <c r="B116" s="137" t="s">
         <v>230</v>
       </c>
@@ -12139,7 +12069,7 @@
       <c r="BD116" s="89"/>
     </row>
     <row r="117" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="253"/>
+      <c r="A117" s="247"/>
       <c r="B117" s="137" t="s">
         <v>231</v>
       </c>
@@ -12207,7 +12137,7 @@
       <c r="BD117" s="89"/>
     </row>
     <row r="118" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="253"/>
+      <c r="A118" s="247"/>
       <c r="B118" s="137" t="s">
         <v>232</v>
       </c>
@@ -12275,7 +12205,7 @@
       <c r="BD118" s="89"/>
     </row>
     <row r="119" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="253"/>
+      <c r="A119" s="247"/>
       <c r="B119" s="137" t="s">
         <v>233</v>
       </c>
@@ -12343,7 +12273,7 @@
       <c r="BD119" s="89"/>
     </row>
     <row r="120" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="253"/>
+      <c r="A120" s="247"/>
       <c r="B120" s="136" t="s">
         <v>234</v>
       </c>
@@ -12405,7 +12335,7 @@
       <c r="BD120" s="89"/>
     </row>
     <row r="121" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="253"/>
+      <c r="A121" s="247"/>
       <c r="B121" s="137" t="s">
         <v>235</v>
       </c>
@@ -12473,7 +12403,7 @@
       <c r="BD121" s="89"/>
     </row>
     <row r="122" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="253"/>
+      <c r="A122" s="247"/>
       <c r="B122" s="137" t="s">
         <v>236</v>
       </c>
@@ -12541,7 +12471,7 @@
       <c r="BD122" s="89"/>
     </row>
     <row r="123" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="253"/>
+      <c r="A123" s="247"/>
       <c r="B123" s="136" t="s">
         <v>237</v>
       </c>
@@ -12603,7 +12533,7 @@
       <c r="BD123" s="89"/>
     </row>
     <row r="124" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="253"/>
+      <c r="A124" s="247"/>
       <c r="B124" s="137" t="s">
         <v>238</v>
       </c>
@@ -12667,7 +12597,7 @@
       <c r="BD124" s="89"/>
     </row>
     <row r="125" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="253"/>
+      <c r="A125" s="247"/>
       <c r="B125" s="135"/>
       <c r="C125" s="90" t="s">
         <v>183</v>
@@ -12733,7 +12663,7 @@
       <c r="BD125" s="89"/>
     </row>
     <row r="126" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="253"/>
+      <c r="A126" s="247"/>
       <c r="B126" s="135"/>
       <c r="C126" s="90" t="s">
         <v>182</v>
@@ -12799,7 +12729,7 @@
       <c r="BD126" s="89"/>
     </row>
     <row r="127" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="253"/>
+      <c r="A127" s="247"/>
       <c r="B127" s="137" t="s">
         <v>239</v>
       </c>
@@ -12863,7 +12793,7 @@
       <c r="BD127" s="89"/>
     </row>
     <row r="128" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="253"/>
+      <c r="A128" s="247"/>
       <c r="B128" s="135"/>
       <c r="C128" s="90" t="s">
         <v>282</v>
@@ -12929,7 +12859,7 @@
       <c r="BD128" s="89"/>
     </row>
     <row r="129" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="253"/>
+      <c r="A129" s="247"/>
       <c r="B129" s="135"/>
       <c r="C129" s="90" t="s">
         <v>283</v>
@@ -12995,7 +12925,7 @@
       <c r="BD129" s="89"/>
     </row>
     <row r="130" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="253"/>
+      <c r="A130" s="247"/>
       <c r="B130" s="136" t="s">
         <v>240</v>
       </c>
@@ -13057,7 +12987,7 @@
       <c r="BD130" s="89"/>
     </row>
     <row r="131" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="253"/>
+      <c r="A131" s="247"/>
       <c r="B131" s="137" t="s">
         <v>241</v>
       </c>
@@ -13125,7 +13055,7 @@
       <c r="BD131" s="89"/>
     </row>
     <row r="132" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="253"/>
+      <c r="A132" s="247"/>
       <c r="B132" s="137" t="s">
         <v>242</v>
       </c>
@@ -13193,7 +13123,7 @@
       <c r="BD132" s="89"/>
     </row>
     <row r="133" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="253"/>
+      <c r="A133" s="247"/>
       <c r="B133" s="136" t="s">
         <v>243</v>
       </c>
@@ -13255,7 +13185,7 @@
       <c r="BD133" s="89"/>
     </row>
     <row r="134" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="253"/>
+      <c r="A134" s="247"/>
       <c r="B134" s="137" t="s">
         <v>244</v>
       </c>
@@ -13323,7 +13253,7 @@
       <c r="BD134" s="89"/>
     </row>
     <row r="135" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="253"/>
+      <c r="A135" s="247"/>
       <c r="B135" s="136" t="s">
         <v>247</v>
       </c>
@@ -13385,7 +13315,7 @@
       <c r="BD135" s="89"/>
     </row>
     <row r="136" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="253"/>
+      <c r="A136" s="247"/>
       <c r="B136" s="137" t="s">
         <v>248</v>
       </c>
@@ -13453,7 +13383,7 @@
       <c r="BD136" s="89"/>
     </row>
     <row r="137" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="253"/>
+      <c r="A137" s="247"/>
       <c r="B137" s="136" t="s">
         <v>249</v>
       </c>
@@ -13515,7 +13445,7 @@
       <c r="BD137" s="89"/>
     </row>
     <row r="138" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="253"/>
+      <c r="A138" s="247"/>
       <c r="B138" s="137" t="s">
         <v>250</v>
       </c>
@@ -13583,7 +13513,7 @@
       <c r="BD138" s="89"/>
     </row>
     <row r="139" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="253"/>
+      <c r="A139" s="247"/>
       <c r="B139" s="136" t="s">
         <v>251</v>
       </c>
@@ -13645,7 +13575,7 @@
       <c r="BD139" s="89"/>
     </row>
     <row r="140" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="253"/>
+      <c r="A140" s="247"/>
       <c r="B140" s="137" t="s">
         <v>252</v>
       </c>
@@ -13713,7 +13643,7 @@
       <c r="BD140" s="89"/>
     </row>
     <row r="141" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="253"/>
+      <c r="A141" s="247"/>
       <c r="B141" s="137" t="s">
         <v>253</v>
       </c>
@@ -13781,7 +13711,7 @@
       <c r="BD141" s="89"/>
     </row>
     <row r="142" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="253"/>
+      <c r="A142" s="247"/>
       <c r="B142" s="136" t="s">
         <v>254</v>
       </c>
@@ -13843,7 +13773,7 @@
       <c r="BD142" s="89"/>
     </row>
     <row r="143" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="253"/>
+      <c r="A143" s="247"/>
       <c r="B143" s="137" t="s">
         <v>255</v>
       </c>
@@ -13911,7 +13841,7 @@
       <c r="BD143" s="89"/>
     </row>
     <row r="144" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="253"/>
+      <c r="A144" s="247"/>
       <c r="B144" s="136" t="s">
         <v>256</v>
       </c>
@@ -13973,7 +13903,7 @@
       <c r="BD144" s="89"/>
     </row>
     <row r="145" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="253"/>
+      <c r="A145" s="247"/>
       <c r="B145" s="137" t="s">
         <v>257</v>
       </c>
@@ -14041,7 +13971,7 @@
       <c r="BD145" s="89"/>
     </row>
     <row r="146" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="253"/>
+      <c r="A146" s="247"/>
       <c r="B146" s="136" t="s">
         <v>258</v>
       </c>
@@ -14103,7 +14033,7 @@
       <c r="BD146" s="89"/>
     </row>
     <row r="147" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="253"/>
+      <c r="A147" s="247"/>
       <c r="B147" s="137" t="s">
         <v>259</v>
       </c>
@@ -14171,7 +14101,7 @@
       <c r="BD147" s="89"/>
     </row>
     <row r="148" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="253"/>
+      <c r="A148" s="247"/>
       <c r="B148" s="136" t="s">
         <v>260</v>
       </c>
@@ -14233,7 +14163,7 @@
       <c r="BD148" s="89"/>
     </row>
     <row r="149" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="253"/>
+      <c r="A149" s="247"/>
       <c r="B149" s="137" t="s">
         <v>261</v>
       </c>
@@ -14301,7 +14231,7 @@
       <c r="BD149" s="89"/>
     </row>
     <row r="150" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="253"/>
+      <c r="A150" s="247"/>
       <c r="B150" s="137" t="s">
         <v>262</v>
       </c>
@@ -14369,7 +14299,7 @@
       <c r="BD150" s="89"/>
     </row>
     <row r="151" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="253"/>
+      <c r="A151" s="247"/>
       <c r="B151" s="137" t="s">
         <v>263</v>
       </c>
@@ -14437,7 +14367,7 @@
       <c r="BD151" s="89"/>
     </row>
     <row r="152" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="253"/>
+      <c r="A152" s="247"/>
       <c r="B152" s="137" t="s">
         <v>264</v>
       </c>
@@ -14505,7 +14435,7 @@
       <c r="BD152" s="89"/>
     </row>
     <row r="153" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="253"/>
+      <c r="A153" s="247"/>
       <c r="B153" s="136" t="s">
         <v>265</v>
       </c>
@@ -14567,7 +14497,7 @@
       <c r="BD153" s="89"/>
     </row>
     <row r="154" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="253"/>
+      <c r="A154" s="247"/>
       <c r="B154" s="137" t="s">
         <v>266</v>
       </c>
@@ -14635,7 +14565,7 @@
       <c r="BD154" s="89"/>
     </row>
     <row r="155" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="253"/>
+      <c r="A155" s="247"/>
       <c r="B155" s="137" t="s">
         <v>267</v>
       </c>
@@ -14703,7 +14633,7 @@
       <c r="BD155" s="89"/>
     </row>
     <row r="156" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="253"/>
+      <c r="A156" s="247"/>
       <c r="B156" s="136" t="s">
         <v>268</v>
       </c>
@@ -14765,7 +14695,7 @@
       <c r="BD156" s="89"/>
     </row>
     <row r="157" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="253"/>
+      <c r="A157" s="247"/>
       <c r="B157" s="137" t="s">
         <v>269</v>
       </c>
@@ -14833,7 +14763,7 @@
       <c r="BD157" s="89"/>
     </row>
     <row r="158" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="253"/>
+      <c r="A158" s="247"/>
       <c r="B158" s="137" t="s">
         <v>270</v>
       </c>
@@ -14901,7 +14831,7 @@
       <c r="BD158" s="89"/>
     </row>
     <row r="159" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="253"/>
+      <c r="A159" s="247"/>
       <c r="B159" s="137" t="s">
         <v>271</v>
       </c>
@@ -14969,7 +14899,7 @@
       <c r="BD159" s="89"/>
     </row>
     <row r="160" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="253"/>
+      <c r="A160" s="247"/>
       <c r="B160" s="137" t="s">
         <v>272</v>
       </c>
@@ -15037,7 +14967,7 @@
       <c r="BD160" s="89"/>
     </row>
     <row r="161" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="253"/>
+      <c r="A161" s="247"/>
       <c r="B161" s="136" t="s">
         <v>273</v>
       </c>
@@ -15099,7 +15029,7 @@
       <c r="BD161" s="89"/>
     </row>
     <row r="162" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="253"/>
+      <c r="A162" s="247"/>
       <c r="B162" s="137" t="s">
         <v>274</v>
       </c>
@@ -15167,7 +15097,7 @@
       <c r="BD162" s="89"/>
     </row>
     <row r="163" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="253"/>
+      <c r="A163" s="247"/>
       <c r="B163" s="137" t="s">
         <v>275</v>
       </c>
@@ -15235,7 +15165,7 @@
       <c r="BD163" s="89"/>
     </row>
     <row r="164" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="253"/>
+      <c r="A164" s="247"/>
       <c r="B164" s="136" t="s">
         <v>276</v>
       </c>
@@ -15297,7 +15227,7 @@
       <c r="BD164" s="89"/>
     </row>
     <row r="165" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="253"/>
+      <c r="A165" s="247"/>
       <c r="B165" s="137" t="s">
         <v>277</v>
       </c>
@@ -15365,7 +15295,7 @@
       <c r="BD165" s="89"/>
     </row>
     <row r="166" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="253"/>
+      <c r="A166" s="247"/>
       <c r="B166" s="137" t="s">
         <v>278</v>
       </c>
@@ -15433,7 +15363,7 @@
       <c r="BD166" s="89"/>
     </row>
     <row r="167" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="253"/>
+      <c r="A167" s="247"/>
       <c r="B167" s="136" t="s">
         <v>279</v>
       </c>
@@ -15495,7 +15425,7 @@
       <c r="BD167" s="89"/>
     </row>
     <row r="168" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="259"/>
+      <c r="A168" s="253"/>
       <c r="B168" s="138" t="s">
         <v>280</v>
       </c>
@@ -15635,74 +15565,74 @@
         <f>SUM(K170:BD170)</f>
         <v>3500</v>
       </c>
-      <c r="E170" s="274" t="s">
+      <c r="E170" s="268" t="s">
         <v>321</v>
       </c>
-      <c r="F170" s="274"/>
-      <c r="G170" s="274"/>
-      <c r="H170" s="266"/>
-      <c r="I170" s="264"/>
-      <c r="J170" s="264"/>
-      <c r="K170" s="264">
+      <c r="F170" s="268"/>
+      <c r="G170" s="268"/>
+      <c r="H170" s="260"/>
+      <c r="I170" s="258"/>
+      <c r="J170" s="258"/>
+      <c r="K170" s="258">
         <v>500</v>
       </c>
-      <c r="L170" s="264"/>
-      <c r="M170" s="264"/>
-      <c r="N170" s="265"/>
-      <c r="O170" s="266"/>
-      <c r="P170" s="264"/>
-      <c r="Q170" s="264"/>
-      <c r="R170" s="264">
+      <c r="L170" s="258"/>
+      <c r="M170" s="258"/>
+      <c r="N170" s="259"/>
+      <c r="O170" s="260"/>
+      <c r="P170" s="258"/>
+      <c r="Q170" s="258"/>
+      <c r="R170" s="258">
         <v>500</v>
       </c>
-      <c r="S170" s="264"/>
-      <c r="T170" s="264"/>
-      <c r="U170" s="265"/>
-      <c r="V170" s="266"/>
-      <c r="W170" s="264"/>
-      <c r="X170" s="264"/>
-      <c r="Y170" s="264">
+      <c r="S170" s="258"/>
+      <c r="T170" s="258"/>
+      <c r="U170" s="259"/>
+      <c r="V170" s="260"/>
+      <c r="W170" s="258"/>
+      <c r="X170" s="258"/>
+      <c r="Y170" s="258">
         <v>500</v>
       </c>
-      <c r="Z170" s="264"/>
-      <c r="AA170" s="264"/>
-      <c r="AB170" s="265"/>
-      <c r="AC170" s="266"/>
-      <c r="AD170" s="264"/>
-      <c r="AE170" s="264"/>
-      <c r="AF170" s="264">
+      <c r="Z170" s="258"/>
+      <c r="AA170" s="258"/>
+      <c r="AB170" s="259"/>
+      <c r="AC170" s="260"/>
+      <c r="AD170" s="258"/>
+      <c r="AE170" s="258"/>
+      <c r="AF170" s="258">
         <v>500</v>
       </c>
-      <c r="AG170" s="264"/>
-      <c r="AH170" s="264"/>
-      <c r="AI170" s="265"/>
-      <c r="AJ170" s="266"/>
-      <c r="AK170" s="264"/>
-      <c r="AL170" s="264"/>
-      <c r="AM170" s="264">
+      <c r="AG170" s="258"/>
+      <c r="AH170" s="258"/>
+      <c r="AI170" s="259"/>
+      <c r="AJ170" s="260"/>
+      <c r="AK170" s="258"/>
+      <c r="AL170" s="258"/>
+      <c r="AM170" s="258">
         <v>500</v>
       </c>
-      <c r="AN170" s="264"/>
-      <c r="AO170" s="264"/>
-      <c r="AP170" s="265"/>
-      <c r="AQ170" s="266"/>
-      <c r="AR170" s="264"/>
-      <c r="AS170" s="264"/>
-      <c r="AT170" s="264">
+      <c r="AN170" s="258"/>
+      <c r="AO170" s="258"/>
+      <c r="AP170" s="259"/>
+      <c r="AQ170" s="260"/>
+      <c r="AR170" s="258"/>
+      <c r="AS170" s="258"/>
+      <c r="AT170" s="258">
         <v>500</v>
       </c>
-      <c r="AU170" s="264"/>
-      <c r="AV170" s="264"/>
-      <c r="AW170" s="265"/>
-      <c r="AX170" s="266"/>
-      <c r="AY170" s="264"/>
-      <c r="AZ170" s="264"/>
-      <c r="BA170" s="264">
+      <c r="AU170" s="258"/>
+      <c r="AV170" s="258"/>
+      <c r="AW170" s="259"/>
+      <c r="AX170" s="260"/>
+      <c r="AY170" s="258"/>
+      <c r="AZ170" s="258"/>
+      <c r="BA170" s="258">
         <v>500</v>
       </c>
-      <c r="BB170" s="264"/>
-      <c r="BC170" s="264"/>
-      <c r="BD170" s="265"/>
+      <c r="BB170" s="258"/>
+      <c r="BC170" s="258"/>
+      <c r="BD170" s="259"/>
     </row>
     <row r="171" spans="1:56" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A171" s="150"/>
@@ -15714,74 +15644,74 @@
         <f>SUM(K171:BD171)</f>
         <v>4410</v>
       </c>
-      <c r="E171" s="274" t="s">
+      <c r="E171" s="268" t="s">
         <v>320</v>
       </c>
-      <c r="F171" s="274"/>
-      <c r="G171" s="274"/>
-      <c r="H171" s="266"/>
-      <c r="I171" s="264"/>
-      <c r="J171" s="264"/>
-      <c r="K171" s="264">
+      <c r="F171" s="268"/>
+      <c r="G171" s="268"/>
+      <c r="H171" s="260"/>
+      <c r="I171" s="258"/>
+      <c r="J171" s="258"/>
+      <c r="K171" s="258">
         <v>630</v>
       </c>
-      <c r="L171" s="264"/>
-      <c r="M171" s="264"/>
-      <c r="N171" s="265"/>
-      <c r="O171" s="266"/>
-      <c r="P171" s="264"/>
-      <c r="Q171" s="264"/>
-      <c r="R171" s="264">
+      <c r="L171" s="258"/>
+      <c r="M171" s="258"/>
+      <c r="N171" s="259"/>
+      <c r="O171" s="260"/>
+      <c r="P171" s="258"/>
+      <c r="Q171" s="258"/>
+      <c r="R171" s="258">
         <v>630</v>
       </c>
-      <c r="S171" s="264"/>
-      <c r="T171" s="264"/>
-      <c r="U171" s="265"/>
-      <c r="V171" s="266"/>
-      <c r="W171" s="264"/>
-      <c r="X171" s="264"/>
-      <c r="Y171" s="264">
+      <c r="S171" s="258"/>
+      <c r="T171" s="258"/>
+      <c r="U171" s="259"/>
+      <c r="V171" s="260"/>
+      <c r="W171" s="258"/>
+      <c r="X171" s="258"/>
+      <c r="Y171" s="258">
         <v>630</v>
       </c>
-      <c r="Z171" s="264"/>
-      <c r="AA171" s="264"/>
-      <c r="AB171" s="265"/>
-      <c r="AC171" s="266"/>
-      <c r="AD171" s="264"/>
-      <c r="AE171" s="264"/>
-      <c r="AF171" s="264">
+      <c r="Z171" s="258"/>
+      <c r="AA171" s="258"/>
+      <c r="AB171" s="259"/>
+      <c r="AC171" s="260"/>
+      <c r="AD171" s="258"/>
+      <c r="AE171" s="258"/>
+      <c r="AF171" s="258">
         <v>630</v>
       </c>
-      <c r="AG171" s="264"/>
-      <c r="AH171" s="264"/>
-      <c r="AI171" s="265"/>
-      <c r="AJ171" s="266"/>
-      <c r="AK171" s="264"/>
-      <c r="AL171" s="264"/>
-      <c r="AM171" s="264">
+      <c r="AG171" s="258"/>
+      <c r="AH171" s="258"/>
+      <c r="AI171" s="259"/>
+      <c r="AJ171" s="260"/>
+      <c r="AK171" s="258"/>
+      <c r="AL171" s="258"/>
+      <c r="AM171" s="258">
         <v>630</v>
       </c>
-      <c r="AN171" s="264"/>
-      <c r="AO171" s="264"/>
-      <c r="AP171" s="265"/>
-      <c r="AQ171" s="266"/>
-      <c r="AR171" s="264"/>
-      <c r="AS171" s="264"/>
-      <c r="AT171" s="264">
+      <c r="AN171" s="258"/>
+      <c r="AO171" s="258"/>
+      <c r="AP171" s="259"/>
+      <c r="AQ171" s="260"/>
+      <c r="AR171" s="258"/>
+      <c r="AS171" s="258"/>
+      <c r="AT171" s="258">
         <v>630</v>
       </c>
-      <c r="AU171" s="264"/>
-      <c r="AV171" s="264"/>
-      <c r="AW171" s="265"/>
-      <c r="AX171" s="266"/>
-      <c r="AY171" s="264"/>
-      <c r="AZ171" s="264"/>
-      <c r="BA171" s="264">
+      <c r="AU171" s="258"/>
+      <c r="AV171" s="258"/>
+      <c r="AW171" s="259"/>
+      <c r="AX171" s="260"/>
+      <c r="AY171" s="258"/>
+      <c r="AZ171" s="258"/>
+      <c r="BA171" s="258">
         <v>630</v>
       </c>
-      <c r="BB171" s="264"/>
-      <c r="BC171" s="264"/>
-      <c r="BD171" s="265"/>
+      <c r="BB171" s="258"/>
+      <c r="BC171" s="258"/>
+      <c r="BD171" s="259"/>
     </row>
     <row r="172" spans="1:56" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="152"/>
@@ -15793,74 +15723,74 @@
         <f>+D169+D171</f>
         <v>9910</v>
       </c>
-      <c r="E172" s="267" t="s">
+      <c r="E172" s="261" t="s">
         <v>304</v>
       </c>
-      <c r="F172" s="267"/>
-      <c r="G172" s="267"/>
-      <c r="H172" s="262"/>
-      <c r="I172" s="263"/>
-      <c r="J172" s="263"/>
-      <c r="K172" s="260">
+      <c r="F172" s="261"/>
+      <c r="G172" s="261"/>
+      <c r="H172" s="256"/>
+      <c r="I172" s="257"/>
+      <c r="J172" s="257"/>
+      <c r="K172" s="254">
         <v>44607</v>
       </c>
-      <c r="L172" s="260"/>
-      <c r="M172" s="260"/>
-      <c r="N172" s="261"/>
-      <c r="O172" s="262"/>
-      <c r="P172" s="263"/>
-      <c r="Q172" s="263"/>
-      <c r="R172" s="260">
+      <c r="L172" s="254"/>
+      <c r="M172" s="254"/>
+      <c r="N172" s="255"/>
+      <c r="O172" s="256"/>
+      <c r="P172" s="257"/>
+      <c r="Q172" s="257"/>
+      <c r="R172" s="254">
         <v>44607</v>
       </c>
-      <c r="S172" s="260"/>
-      <c r="T172" s="260"/>
-      <c r="U172" s="261"/>
-      <c r="V172" s="262"/>
-      <c r="W172" s="263"/>
-      <c r="X172" s="263"/>
-      <c r="Y172" s="260">
+      <c r="S172" s="254"/>
+      <c r="T172" s="254"/>
+      <c r="U172" s="255"/>
+      <c r="V172" s="256"/>
+      <c r="W172" s="257"/>
+      <c r="X172" s="257"/>
+      <c r="Y172" s="254">
         <v>44607</v>
       </c>
-      <c r="Z172" s="260"/>
-      <c r="AA172" s="260"/>
-      <c r="AB172" s="261"/>
-      <c r="AC172" s="262"/>
-      <c r="AD172" s="263"/>
-      <c r="AE172" s="263"/>
-      <c r="AF172" s="260">
+      <c r="Z172" s="254"/>
+      <c r="AA172" s="254"/>
+      <c r="AB172" s="255"/>
+      <c r="AC172" s="256"/>
+      <c r="AD172" s="257"/>
+      <c r="AE172" s="257"/>
+      <c r="AF172" s="254">
         <v>44607</v>
       </c>
-      <c r="AG172" s="260"/>
-      <c r="AH172" s="260"/>
-      <c r="AI172" s="261"/>
-      <c r="AJ172" s="262"/>
-      <c r="AK172" s="263"/>
-      <c r="AL172" s="263"/>
-      <c r="AM172" s="260">
+      <c r="AG172" s="254"/>
+      <c r="AH172" s="254"/>
+      <c r="AI172" s="255"/>
+      <c r="AJ172" s="256"/>
+      <c r="AK172" s="257"/>
+      <c r="AL172" s="257"/>
+      <c r="AM172" s="254">
         <v>44607</v>
       </c>
-      <c r="AN172" s="260"/>
-      <c r="AO172" s="260"/>
-      <c r="AP172" s="261"/>
-      <c r="AQ172" s="262"/>
-      <c r="AR172" s="263"/>
-      <c r="AS172" s="263"/>
-      <c r="AT172" s="260">
+      <c r="AN172" s="254"/>
+      <c r="AO172" s="254"/>
+      <c r="AP172" s="255"/>
+      <c r="AQ172" s="256"/>
+      <c r="AR172" s="257"/>
+      <c r="AS172" s="257"/>
+      <c r="AT172" s="254">
         <v>44607</v>
       </c>
-      <c r="AU172" s="260"/>
-      <c r="AV172" s="260"/>
-      <c r="AW172" s="261"/>
-      <c r="AX172" s="262"/>
-      <c r="AY172" s="263"/>
-      <c r="AZ172" s="263"/>
-      <c r="BA172" s="260">
+      <c r="AU172" s="254"/>
+      <c r="AV172" s="254"/>
+      <c r="AW172" s="255"/>
+      <c r="AX172" s="256"/>
+      <c r="AY172" s="257"/>
+      <c r="AZ172" s="257"/>
+      <c r="BA172" s="254">
         <v>44607</v>
       </c>
-      <c r="BB172" s="260"/>
-      <c r="BC172" s="260"/>
-      <c r="BD172" s="261"/>
+      <c r="BB172" s="254"/>
+      <c r="BC172" s="254"/>
+      <c r="BD172" s="255"/>
     </row>
     <row r="173" spans="1:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="163"/>
@@ -16092,7 +16022,7 @@
   <dimension ref="B1:AG36"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="129" zoomScaleNormal="129" zoomScaleSheetLayoutView="129" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:F12"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -16100,8 +16030,10 @@
     <col min="1" max="1" width="4.7109375" style="183" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="183" customWidth="1"/>
     <col min="3" max="3" width="65" style="183" customWidth="1"/>
-    <col min="4" max="5" width="10.28515625" style="183" customWidth="1"/>
-    <col min="6" max="7" width="9.28515625" style="183" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="183" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="183" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="183" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="183" customWidth="1"/>
     <col min="8" max="8" width="12" style="183" customWidth="1"/>
     <col min="9" max="9" width="14" style="183" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" style="183" customWidth="1"/>
@@ -16115,15 +16047,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="287" t="s">
-        <v>356</v>
-      </c>
-      <c r="D1" s="287"/>
-      <c r="E1" s="287"/>
-      <c r="F1" s="287"/>
-      <c r="G1" s="287"/>
-      <c r="H1" s="287"/>
-      <c r="I1" s="287"/>
+      <c r="C1" s="275" t="s">
+        <v>348</v>
+      </c>
+      <c r="D1" s="275"/>
+      <c r="E1" s="275"/>
+      <c r="F1" s="275"/>
+      <c r="G1" s="275"/>
+      <c r="H1" s="275"/>
+      <c r="I1" s="275"/>
       <c r="J1" s="193"/>
       <c r="K1" s="193"/>
       <c r="L1" s="193"/>
@@ -16151,13 +16083,13 @@
     </row>
     <row r="2" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="193"/>
-      <c r="C2" s="287"/>
-      <c r="D2" s="287"/>
-      <c r="E2" s="287"/>
-      <c r="F2" s="287"/>
-      <c r="G2" s="287"/>
-      <c r="H2" s="287"/>
-      <c r="I2" s="287"/>
+      <c r="C2" s="275"/>
+      <c r="D2" s="275"/>
+      <c r="E2" s="275"/>
+      <c r="F2" s="275"/>
+      <c r="G2" s="275"/>
+      <c r="H2" s="275"/>
+      <c r="I2" s="275"/>
       <c r="J2" s="193"/>
       <c r="K2" s="193"/>
       <c r="L2" s="193"/>
@@ -16219,16 +16151,16 @@
     </row>
     <row r="4" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="202" t="s">
+        <v>350</v>
+      </c>
+      <c r="D4" s="276" t="s">
         <v>337</v>
       </c>
-      <c r="D4" s="288" t="s">
-        <v>338</v>
-      </c>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="288"/>
-      <c r="H4" s="288"/>
-      <c r="I4" s="289"/>
+      <c r="E4" s="276"/>
+      <c r="F4" s="276"/>
+      <c r="G4" s="276"/>
+      <c r="H4" s="276"/>
+      <c r="I4" s="277"/>
       <c r="J4" s="193"/>
       <c r="K4" s="193"/>
       <c r="L4" s="193"/>
@@ -16256,16 +16188,16 @@
     </row>
     <row r="5" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="202" t="s">
-        <v>343</v>
-      </c>
-      <c r="D5" s="288" t="s">
-        <v>363</v>
-      </c>
-      <c r="E5" s="288"/>
-      <c r="F5" s="288"/>
-      <c r="G5" s="288"/>
-      <c r="H5" s="288"/>
-      <c r="I5" s="289"/>
+        <v>340</v>
+      </c>
+      <c r="D5" s="276" t="s">
+        <v>349</v>
+      </c>
+      <c r="E5" s="276"/>
+      <c r="F5" s="276"/>
+      <c r="G5" s="276"/>
+      <c r="H5" s="276"/>
+      <c r="I5" s="277"/>
       <c r="J5" s="193"/>
       <c r="K5" s="193"/>
       <c r="L5" s="193"/>
@@ -16327,16 +16259,14 @@
     </row>
     <row r="7" spans="2:33" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="200" t="s">
-        <v>344</v>
-      </c>
-      <c r="D7" s="290"/>
-      <c r="E7" s="291"/>
+        <v>341</v>
+      </c>
+      <c r="D7" s="278"/>
+      <c r="E7" s="279"/>
       <c r="F7" s="225"/>
       <c r="G7" s="225"/>
-      <c r="H7" s="188" t="s">
-        <v>357</v>
-      </c>
-      <c r="I7" s="232"/>
+      <c r="H7" s="188"/>
+      <c r="I7" s="188"/>
       <c r="J7" s="193"/>
       <c r="K7" s="193"/>
       <c r="L7" s="193"/>
@@ -16364,16 +16294,14 @@
     </row>
     <row r="8" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="200" t="s">
-        <v>345</v>
-      </c>
-      <c r="D8" s="290"/>
-      <c r="E8" s="291"/>
+        <v>342</v>
+      </c>
+      <c r="D8" s="278"/>
+      <c r="E8" s="279"/>
       <c r="F8" s="225"/>
       <c r="G8" s="225"/>
-      <c r="H8" s="188" t="s">
-        <v>358</v>
-      </c>
-      <c r="I8" s="227"/>
+      <c r="H8" s="188"/>
+      <c r="I8" s="188"/>
       <c r="J8" s="193"/>
       <c r="K8" s="193"/>
       <c r="L8" s="193"/>
@@ -16401,15 +16329,12 @@
     </row>
     <row r="9" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="200" t="s">
-        <v>346</v>
-      </c>
-      <c r="D9" s="290"/>
-      <c r="E9" s="291"/>
+        <v>343</v>
+      </c>
+      <c r="D9" s="278"/>
+      <c r="E9" s="279"/>
       <c r="F9" s="188"/>
-      <c r="H9" s="183" t="s">
-        <v>359</v>
-      </c>
-      <c r="I9" s="228"/>
+      <c r="I9" s="193"/>
       <c r="L9" s="193"/>
       <c r="M9" s="193"/>
       <c r="N9" s="193"/>
@@ -16438,10 +16363,7 @@
       <c r="D10" s="224"/>
       <c r="E10" s="188"/>
       <c r="F10" s="188"/>
-      <c r="H10" s="183" t="s">
-        <v>360</v>
-      </c>
-      <c r="I10" s="229"/>
+      <c r="I10" s="193"/>
       <c r="L10" s="193"/>
       <c r="M10" s="193"/>
       <c r="N10" s="193"/>
@@ -16467,18 +16389,16 @@
     </row>
     <row r="11" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="202" t="s">
-        <v>339</v>
-      </c>
-      <c r="D11" s="292" t="s">
-        <v>341</v>
-      </c>
-      <c r="E11" s="288"/>
-      <c r="F11" s="289"/>
+        <v>351</v>
+      </c>
+      <c r="D11" s="280" t="s">
+        <v>338</v>
+      </c>
+      <c r="E11" s="276"/>
+      <c r="F11" s="277"/>
       <c r="G11" s="180"/>
-      <c r="H11" s="180" t="s">
-        <v>361</v>
-      </c>
-      <c r="I11" s="230"/>
+      <c r="H11" s="180"/>
+      <c r="I11" s="180"/>
       <c r="L11" s="193"/>
       <c r="M11" s="193"/>
       <c r="N11" s="193"/>
@@ -16500,18 +16420,16 @@
     </row>
     <row r="12" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="202" t="s">
-        <v>340</v>
-      </c>
-      <c r="D12" s="327" t="s">
-        <v>342</v>
-      </c>
-      <c r="E12" s="328"/>
-      <c r="F12" s="329"/>
+        <v>352</v>
+      </c>
+      <c r="D12" s="281" t="s">
+        <v>339</v>
+      </c>
+      <c r="E12" s="282"/>
+      <c r="F12" s="283"/>
       <c r="G12" s="226"/>
-      <c r="H12" s="226" t="s">
-        <v>362</v>
-      </c>
-      <c r="I12" s="231"/>
+      <c r="H12" s="226"/>
+      <c r="I12" s="226"/>
       <c r="J12" s="193"/>
       <c r="K12" s="193"/>
       <c r="L12" s="193"/>
@@ -16583,23 +16501,23 @@
       <c r="AC14" s="186"/>
     </row>
     <row r="15" spans="2:33" s="182" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="293" t="s">
+      <c r="B15" s="284" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="303" t="s">
-        <v>347</v>
-      </c>
-      <c r="D15" s="279" t="s">
+      <c r="C15" s="294" t="s">
+        <v>344</v>
+      </c>
+      <c r="D15" s="299" t="s">
         <v>301</v>
       </c>
-      <c r="E15" s="280"/>
-      <c r="F15" s="281"/>
-      <c r="G15" s="279" t="s">
-        <v>355</v>
-      </c>
-      <c r="H15" s="280"/>
-      <c r="I15" s="280"/>
-      <c r="J15" s="281"/>
+      <c r="E15" s="300"/>
+      <c r="F15" s="301"/>
+      <c r="G15" s="299" t="s">
+        <v>357</v>
+      </c>
+      <c r="H15" s="300"/>
+      <c r="I15" s="300"/>
+      <c r="J15" s="301"/>
       <c r="K15" s="189"/>
       <c r="L15" s="189"/>
       <c r="M15" s="189"/>
@@ -16625,15 +16543,15 @@
       <c r="AG15" s="183"/>
     </row>
     <row r="16" spans="2:33" s="182" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="294"/>
-      <c r="C16" s="304"/>
-      <c r="D16" s="282"/>
-      <c r="E16" s="283"/>
-      <c r="F16" s="284"/>
-      <c r="G16" s="282"/>
-      <c r="H16" s="283"/>
-      <c r="I16" s="283"/>
-      <c r="J16" s="284"/>
+      <c r="B16" s="285"/>
+      <c r="C16" s="295"/>
+      <c r="D16" s="302"/>
+      <c r="E16" s="303"/>
+      <c r="F16" s="304"/>
+      <c r="G16" s="302"/>
+      <c r="H16" s="303"/>
+      <c r="I16" s="303"/>
+      <c r="J16" s="304"/>
       <c r="K16" s="190"/>
       <c r="L16" s="190"/>
       <c r="M16" s="190"/>
@@ -16659,51 +16577,51 @@
       <c r="AG16" s="183"/>
     </row>
     <row r="17" spans="2:29" s="182" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="294"/>
-      <c r="C17" s="304"/>
-      <c r="D17" s="297" t="s">
-        <v>348</v>
-      </c>
-      <c r="E17" s="297" t="s">
-        <v>349</v>
-      </c>
-      <c r="F17" s="305" t="s">
-        <v>350</v>
-      </c>
-      <c r="G17" s="285" t="s">
-        <v>351</v>
-      </c>
-      <c r="H17" s="285" t="s">
-        <v>352</v>
-      </c>
-      <c r="I17" s="299" t="s">
+      <c r="B17" s="285"/>
+      <c r="C17" s="295"/>
+      <c r="D17" s="288" t="s">
+        <v>345</v>
+      </c>
+      <c r="E17" s="288" t="s">
+        <v>346</v>
+      </c>
+      <c r="F17" s="296" t="s">
+        <v>347</v>
+      </c>
+      <c r="G17" s="273" t="s">
         <v>353</v>
       </c>
-      <c r="J17" s="306" t="s">
+      <c r="H17" s="273" t="s">
         <v>354</v>
       </c>
+      <c r="I17" s="290" t="s">
+        <v>355</v>
+      </c>
+      <c r="J17" s="297" t="s">
+        <v>356</v>
+      </c>
     </row>
     <row r="18" spans="2:29" s="182" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="294"/>
-      <c r="C18" s="304"/>
-      <c r="D18" s="297"/>
-      <c r="E18" s="297"/>
-      <c r="F18" s="285"/>
-      <c r="G18" s="285"/>
-      <c r="H18" s="285"/>
-      <c r="I18" s="297"/>
-      <c r="J18" s="306"/>
+      <c r="B18" s="285"/>
+      <c r="C18" s="295"/>
+      <c r="D18" s="288"/>
+      <c r="E18" s="288"/>
+      <c r="F18" s="273"/>
+      <c r="G18" s="273"/>
+      <c r="H18" s="273"/>
+      <c r="I18" s="288"/>
+      <c r="J18" s="297"/>
     </row>
     <row r="19" spans="2:29" s="182" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="295"/>
-      <c r="C19" s="304"/>
-      <c r="D19" s="298"/>
-      <c r="E19" s="298"/>
-      <c r="F19" s="286"/>
-      <c r="G19" s="286"/>
-      <c r="H19" s="286"/>
-      <c r="I19" s="298"/>
-      <c r="J19" s="307"/>
+      <c r="B19" s="286"/>
+      <c r="C19" s="295"/>
+      <c r="D19" s="289"/>
+      <c r="E19" s="289"/>
+      <c r="F19" s="274"/>
+      <c r="G19" s="274"/>
+      <c r="H19" s="274"/>
+      <c r="I19" s="289"/>
+      <c r="J19" s="298"/>
     </row>
     <row r="20" spans="2:29" s="182" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B20" s="208"/>
@@ -16739,16 +16657,16 @@
     </row>
     <row r="23" spans="2:29" s="182" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="181"/>
-      <c r="C23" s="233"/>
-      <c r="D23" s="233"/>
-      <c r="E23" s="233"/>
-      <c r="F23" s="233"/>
-      <c r="G23" s="233"/>
-      <c r="H23" s="234"/>
-      <c r="I23" s="234"/>
-      <c r="J23" s="300"/>
-      <c r="K23" s="300"/>
-      <c r="L23" s="300"/>
+      <c r="C23" s="227"/>
+      <c r="D23" s="227"/>
+      <c r="E23" s="227"/>
+      <c r="F23" s="227"/>
+      <c r="G23" s="227"/>
+      <c r="H23" s="228"/>
+      <c r="I23" s="228"/>
+      <c r="J23" s="291"/>
+      <c r="K23" s="291"/>
+      <c r="L23" s="291"/>
       <c r="M23" s="206"/>
       <c r="N23" s="206"/>
       <c r="O23" s="206"/>
@@ -16758,24 +16676,24 @@
       <c r="S23" s="206"/>
       <c r="T23" s="206"/>
       <c r="U23" s="206"/>
-      <c r="V23" s="301"/>
-      <c r="W23" s="301"/>
-      <c r="X23" s="300"/>
-      <c r="Y23" s="300"/>
-      <c r="Z23" s="300"/>
-      <c r="AA23" s="300"/>
-      <c r="AB23" s="300"/>
+      <c r="V23" s="292"/>
+      <c r="W23" s="292"/>
+      <c r="X23" s="291"/>
+      <c r="Y23" s="291"/>
+      <c r="Z23" s="291"/>
+      <c r="AA23" s="291"/>
+      <c r="AB23" s="291"/>
       <c r="AC23" s="204"/>
     </row>
     <row r="24" spans="2:29" s="182" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="181"/>
-      <c r="C24" s="235"/>
-      <c r="D24" s="235"/>
-      <c r="E24" s="235"/>
-      <c r="F24" s="235"/>
-      <c r="G24" s="235"/>
-      <c r="H24" s="234"/>
-      <c r="I24" s="234"/>
+      <c r="C24" s="229"/>
+      <c r="D24" s="229"/>
+      <c r="E24" s="229"/>
+      <c r="F24" s="229"/>
+      <c r="G24" s="229"/>
+      <c r="H24" s="228"/>
+      <c r="I24" s="228"/>
       <c r="J24" s="204"/>
       <c r="O24" s="206"/>
       <c r="P24" s="206"/>
@@ -16795,16 +16713,16 @@
     </row>
     <row r="25" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="181"/>
-      <c r="C25" s="236"/>
-      <c r="D25" s="236"/>
-      <c r="E25" s="236"/>
-      <c r="F25" s="236"/>
-      <c r="G25" s="236"/>
-      <c r="H25" s="234"/>
-      <c r="I25" s="234"/>
-      <c r="J25" s="300"/>
-      <c r="K25" s="300"/>
-      <c r="L25" s="300"/>
+      <c r="C25" s="230"/>
+      <c r="D25" s="230"/>
+      <c r="E25" s="230"/>
+      <c r="F25" s="230"/>
+      <c r="G25" s="230"/>
+      <c r="H25" s="228"/>
+      <c r="I25" s="228"/>
+      <c r="J25" s="291"/>
+      <c r="K25" s="291"/>
+      <c r="L25" s="291"/>
       <c r="M25" s="206"/>
       <c r="N25" s="206"/>
       <c r="O25" s="206"/>
@@ -16815,9 +16733,9 @@
       <c r="T25" s="206"/>
       <c r="U25" s="206"/>
       <c r="V25" s="206"/>
-      <c r="W25" s="302"/>
-      <c r="X25" s="302"/>
-      <c r="Y25" s="302"/>
+      <c r="W25" s="293"/>
+      <c r="X25" s="293"/>
+      <c r="Y25" s="293"/>
       <c r="Z25" s="206"/>
       <c r="AA25" s="206"/>
       <c r="AB25" s="206"/>
@@ -16825,13 +16743,13 @@
     </row>
     <row r="26" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="181"/>
-      <c r="C26" s="236"/>
-      <c r="D26" s="236"/>
-      <c r="E26" s="236"/>
-      <c r="F26" s="236"/>
-      <c r="G26" s="236"/>
-      <c r="H26" s="234"/>
-      <c r="I26" s="234"/>
+      <c r="C26" s="230"/>
+      <c r="D26" s="230"/>
+      <c r="E26" s="230"/>
+      <c r="F26" s="230"/>
+      <c r="G26" s="230"/>
+      <c r="H26" s="228"/>
+      <c r="I26" s="228"/>
       <c r="J26" s="206"/>
       <c r="K26" s="206"/>
       <c r="L26" s="206"/>
@@ -16845,24 +16763,24 @@
       <c r="T26" s="206"/>
       <c r="U26" s="206"/>
       <c r="V26" s="206"/>
-      <c r="W26" s="296"/>
-      <c r="X26" s="296"/>
-      <c r="Y26" s="296"/>
-      <c r="Z26" s="296"/>
-      <c r="AA26" s="296"/>
+      <c r="W26" s="287"/>
+      <c r="X26" s="287"/>
+      <c r="Y26" s="287"/>
+      <c r="Z26" s="287"/>
+      <c r="AA26" s="287"/>
       <c r="AB26" s="206"/>
       <c r="AC26" s="206"/>
     </row>
     <row r="27" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="181"/>
-      <c r="C27" s="235"/>
-      <c r="D27" s="235"/>
-      <c r="E27" s="235"/>
-      <c r="F27" s="235"/>
-      <c r="G27" s="235"/>
-      <c r="H27" s="234"/>
-      <c r="I27" s="234"/>
-      <c r="J27" s="238"/>
+      <c r="C27" s="229"/>
+      <c r="D27" s="229"/>
+      <c r="E27" s="229"/>
+      <c r="F27" s="229"/>
+      <c r="G27" s="229"/>
+      <c r="H27" s="228"/>
+      <c r="I27" s="228"/>
+      <c r="J27" s="232"/>
       <c r="K27" s="206"/>
       <c r="L27" s="206"/>
       <c r="M27" s="206"/>
@@ -16884,13 +16802,13 @@
       <c r="AC27" s="206"/>
     </row>
     <row r="28" spans="2:29" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="237"/>
-      <c r="D28" s="237"/>
-      <c r="E28" s="237"/>
-      <c r="F28" s="237"/>
-      <c r="G28" s="237"/>
-      <c r="H28" s="234"/>
-      <c r="I28" s="234"/>
+      <c r="C28" s="231"/>
+      <c r="D28" s="231"/>
+      <c r="E28" s="231"/>
+      <c r="F28" s="231"/>
+      <c r="G28" s="231"/>
+      <c r="H28" s="228"/>
+      <c r="I28" s="228"/>
       <c r="J28" s="184"/>
       <c r="W28" s="185"/>
     </row>
@@ -16936,7 +16854,7 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="82" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -16964,72 +16882,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="309" t="s">
+      <c r="B2" s="306" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="310"/>
-      <c r="D2" s="310"/>
-      <c r="E2" s="310"/>
-      <c r="F2" s="310"/>
-      <c r="G2" s="310"/>
-      <c r="H2" s="310"/>
-      <c r="I2" s="310"/>
-      <c r="J2" s="310"/>
-      <c r="K2" s="310"/>
-      <c r="L2" s="310"/>
-      <c r="M2" s="311"/>
+      <c r="C2" s="307"/>
+      <c r="D2" s="307"/>
+      <c r="E2" s="307"/>
+      <c r="F2" s="307"/>
+      <c r="G2" s="307"/>
+      <c r="H2" s="307"/>
+      <c r="I2" s="307"/>
+      <c r="J2" s="307"/>
+      <c r="K2" s="307"/>
+      <c r="L2" s="307"/>
+      <c r="M2" s="308"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="312" t="s">
+      <c r="B3" s="309" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="314" t="s">
+      <c r="C3" s="311" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="314" t="s">
+      <c r="D3" s="311" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="316" t="s">
+      <c r="E3" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="318" t="s">
+      <c r="F3" s="315" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="319"/>
-      <c r="H3" s="319"/>
-      <c r="I3" s="319"/>
-      <c r="J3" s="319"/>
-      <c r="K3" s="319"/>
-      <c r="L3" s="319"/>
-      <c r="M3" s="320"/>
+      <c r="G3" s="316"/>
+      <c r="H3" s="316"/>
+      <c r="I3" s="316"/>
+      <c r="J3" s="316"/>
+      <c r="K3" s="316"/>
+      <c r="L3" s="316"/>
+      <c r="M3" s="317"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="313"/>
-      <c r="C4" s="315"/>
-      <c r="D4" s="315"/>
-      <c r="E4" s="317"/>
-      <c r="F4" s="321"/>
-      <c r="G4" s="322"/>
-      <c r="H4" s="322"/>
-      <c r="I4" s="322"/>
-      <c r="J4" s="322"/>
-      <c r="K4" s="322"/>
-      <c r="L4" s="322"/>
-      <c r="M4" s="323"/>
+      <c r="B4" s="310"/>
+      <c r="C4" s="312"/>
+      <c r="D4" s="312"/>
+      <c r="E4" s="314"/>
+      <c r="F4" s="318"/>
+      <c r="G4" s="319"/>
+      <c r="H4" s="319"/>
+      <c r="I4" s="319"/>
+      <c r="J4" s="319"/>
+      <c r="K4" s="319"/>
+      <c r="L4" s="319"/>
+      <c r="M4" s="320"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="308"/>
-      <c r="C5" s="308"/>
-      <c r="D5" s="308"/>
-      <c r="E5" s="308"/>
-      <c r="F5" s="308"/>
-      <c r="G5" s="308"/>
-      <c r="H5" s="308"/>
-      <c r="I5" s="308"/>
-      <c r="J5" s="308"/>
-      <c r="K5" s="308"/>
-      <c r="L5" s="308"/>
-      <c r="M5" s="308"/>
+      <c r="B5" s="305"/>
+      <c r="C5" s="305"/>
+      <c r="D5" s="305"/>
+      <c r="E5" s="305"/>
+      <c r="F5" s="305"/>
+      <c r="G5" s="305"/>
+      <c r="H5" s="305"/>
+      <c r="I5" s="305"/>
+      <c r="J5" s="305"/>
+      <c r="K5" s="305"/>
+      <c r="L5" s="305"/>
+      <c r="M5" s="305"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -17642,72 +17560,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="309" t="s">
+      <c r="B2" s="306" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="310"/>
-      <c r="D2" s="310"/>
-      <c r="E2" s="310"/>
-      <c r="F2" s="310"/>
-      <c r="G2" s="310"/>
-      <c r="H2" s="310"/>
-      <c r="I2" s="310"/>
-      <c r="J2" s="310"/>
-      <c r="K2" s="310"/>
-      <c r="L2" s="310"/>
-      <c r="M2" s="311"/>
+      <c r="C2" s="307"/>
+      <c r="D2" s="307"/>
+      <c r="E2" s="307"/>
+      <c r="F2" s="307"/>
+      <c r="G2" s="307"/>
+      <c r="H2" s="307"/>
+      <c r="I2" s="307"/>
+      <c r="J2" s="307"/>
+      <c r="K2" s="307"/>
+      <c r="L2" s="307"/>
+      <c r="M2" s="308"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="312" t="s">
+      <c r="B3" s="309" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="314" t="s">
+      <c r="C3" s="311" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="314" t="s">
+      <c r="D3" s="311" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="316" t="s">
+      <c r="E3" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="318" t="s">
+      <c r="F3" s="315" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="319"/>
-      <c r="H3" s="319"/>
-      <c r="I3" s="319"/>
-      <c r="J3" s="319"/>
-      <c r="K3" s="319"/>
-      <c r="L3" s="319"/>
-      <c r="M3" s="320"/>
+      <c r="G3" s="316"/>
+      <c r="H3" s="316"/>
+      <c r="I3" s="316"/>
+      <c r="J3" s="316"/>
+      <c r="K3" s="316"/>
+      <c r="L3" s="316"/>
+      <c r="M3" s="317"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="313"/>
-      <c r="C4" s="315"/>
-      <c r="D4" s="315"/>
-      <c r="E4" s="317"/>
-      <c r="F4" s="321"/>
-      <c r="G4" s="322"/>
-      <c r="H4" s="322"/>
-      <c r="I4" s="322"/>
-      <c r="J4" s="322"/>
-      <c r="K4" s="322"/>
-      <c r="L4" s="322"/>
-      <c r="M4" s="323"/>
+      <c r="B4" s="310"/>
+      <c r="C4" s="312"/>
+      <c r="D4" s="312"/>
+      <c r="E4" s="314"/>
+      <c r="F4" s="318"/>
+      <c r="G4" s="319"/>
+      <c r="H4" s="319"/>
+      <c r="I4" s="319"/>
+      <c r="J4" s="319"/>
+      <c r="K4" s="319"/>
+      <c r="L4" s="319"/>
+      <c r="M4" s="320"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="308"/>
-      <c r="C5" s="308"/>
-      <c r="D5" s="308"/>
-      <c r="E5" s="308"/>
-      <c r="F5" s="324"/>
-      <c r="G5" s="324"/>
-      <c r="H5" s="324"/>
-      <c r="I5" s="324"/>
-      <c r="J5" s="324"/>
-      <c r="K5" s="324"/>
-      <c r="L5" s="324"/>
-      <c r="M5" s="324"/>
+      <c r="B5" s="305"/>
+      <c r="C5" s="305"/>
+      <c r="D5" s="305"/>
+      <c r="E5" s="305"/>
+      <c r="F5" s="321"/>
+      <c r="G5" s="321"/>
+      <c r="H5" s="321"/>
+      <c r="I5" s="321"/>
+      <c r="J5" s="321"/>
+      <c r="K5" s="321"/>
+      <c r="L5" s="321"/>
+      <c r="M5" s="321"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">
@@ -18308,72 +18226,72 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="309" t="s">
+      <c r="B2" s="306" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="310"/>
-      <c r="D2" s="310"/>
-      <c r="E2" s="310"/>
-      <c r="F2" s="310"/>
-      <c r="G2" s="310"/>
-      <c r="H2" s="310"/>
-      <c r="I2" s="310"/>
-      <c r="J2" s="310"/>
-      <c r="K2" s="310"/>
-      <c r="L2" s="310"/>
-      <c r="M2" s="311"/>
+      <c r="C2" s="307"/>
+      <c r="D2" s="307"/>
+      <c r="E2" s="307"/>
+      <c r="F2" s="307"/>
+      <c r="G2" s="307"/>
+      <c r="H2" s="307"/>
+      <c r="I2" s="307"/>
+      <c r="J2" s="307"/>
+      <c r="K2" s="307"/>
+      <c r="L2" s="307"/>
+      <c r="M2" s="308"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="312" t="s">
+      <c r="B3" s="309" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="314" t="s">
+      <c r="C3" s="311" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="314" t="s">
+      <c r="D3" s="311" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="316" t="s">
+      <c r="E3" s="313" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="318" t="s">
+      <c r="F3" s="315" t="s">
         <v>84</v>
       </c>
-      <c r="G3" s="319"/>
-      <c r="H3" s="319"/>
-      <c r="I3" s="319"/>
-      <c r="J3" s="319"/>
-      <c r="K3" s="319"/>
-      <c r="L3" s="319"/>
-      <c r="M3" s="320"/>
+      <c r="G3" s="316"/>
+      <c r="H3" s="316"/>
+      <c r="I3" s="316"/>
+      <c r="J3" s="316"/>
+      <c r="K3" s="316"/>
+      <c r="L3" s="316"/>
+      <c r="M3" s="317"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="313"/>
-      <c r="C4" s="315"/>
-      <c r="D4" s="315"/>
-      <c r="E4" s="317"/>
-      <c r="F4" s="321"/>
-      <c r="G4" s="322"/>
-      <c r="H4" s="322"/>
-      <c r="I4" s="322"/>
-      <c r="J4" s="322"/>
-      <c r="K4" s="322"/>
-      <c r="L4" s="322"/>
-      <c r="M4" s="323"/>
+      <c r="B4" s="310"/>
+      <c r="C4" s="312"/>
+      <c r="D4" s="312"/>
+      <c r="E4" s="314"/>
+      <c r="F4" s="318"/>
+      <c r="G4" s="319"/>
+      <c r="H4" s="319"/>
+      <c r="I4" s="319"/>
+      <c r="J4" s="319"/>
+      <c r="K4" s="319"/>
+      <c r="L4" s="319"/>
+      <c r="M4" s="320"/>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="325"/>
-      <c r="C5" s="308"/>
-      <c r="D5" s="308"/>
-      <c r="E5" s="308"/>
-      <c r="F5" s="308"/>
-      <c r="G5" s="308"/>
-      <c r="H5" s="308"/>
-      <c r="I5" s="308"/>
-      <c r="J5" s="308"/>
-      <c r="K5" s="308"/>
-      <c r="L5" s="308"/>
-      <c r="M5" s="326"/>
+      <c r="B5" s="322"/>
+      <c r="C5" s="305"/>
+      <c r="D5" s="305"/>
+      <c r="E5" s="305"/>
+      <c r="F5" s="305"/>
+      <c r="G5" s="305"/>
+      <c r="H5" s="305"/>
+      <c r="I5" s="305"/>
+      <c r="J5" s="305"/>
+      <c r="K5" s="305"/>
+      <c r="L5" s="305"/>
+      <c r="M5" s="323"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="12" t="s">

</xml_diff>

<commit_message>
Reports that are ordered the same as in the system (levels)
</commit_message>
<xml_diff>
--- a/public/templates/report_template_project.xlsx
+++ b/public/templates/report_template_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyecto_quisvar\quisvar_proyect_ft\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\gpro1\MyFiles\QuisVar\quisvar_proyect_ft\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FDA1AD1-BC86-4884-BA71-8D0CF9C80C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F386C06-1639-4ABB-B057-455B4093DD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="482" firstSheet="1" activeTab="1" xr2:uid="{F98A2DB2-54A5-485C-A701-CE43CF6B2BAF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="482" firstSheet="1" activeTab="1" xr2:uid="{F98A2DB2-54A5-485C-A701-CE43CF6B2BAF}"/>
   </bookViews>
   <sheets>
     <sheet name="LIQUIDACION" sheetId="9" state="hidden" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="357">
   <si>
     <t>ITEM</t>
   </si>
@@ -1644,13 +1644,10 @@
     <t>Total de dias</t>
   </si>
   <si>
-    <t>total de tareas</t>
-  </si>
-  <si>
     <t>Nivel</t>
   </si>
   <si>
-    <t>Mas informacion</t>
+    <t>Total de tareas</t>
   </si>
 </sst>
 </file>
@@ -1658,13 +1655,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="00.00.00.00"/>
-    <numFmt numFmtId="167" formatCode="00.00.00"/>
-    <numFmt numFmtId="168" formatCode="&quot;S/&quot;#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="170" formatCode="&quot;S/&quot;\ #,##0.00"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;S/&quot;* #,##0.00_-;\-&quot;S/&quot;* #,##0.00_-;_-&quot;S/&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="00.00.00.00"/>
+    <numFmt numFmtId="166" formatCode="00.00.00"/>
+    <numFmt numFmtId="167" formatCode="&quot;S/&quot;#,##0.00"/>
+    <numFmt numFmtId="168" formatCode="_ &quot;S/.&quot;\ * #,##0.00_ ;_ &quot;S/.&quot;\ * \-#,##0.00_ ;_ &quot;S/.&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="169" formatCode="&quot;S/&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="38" x14ac:knownFonts="1">
     <font>
@@ -3053,11 +3050,11 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="324">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3094,10 +3091,10 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3365,25 +3362,19 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="37" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="39" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="38" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3392,7 +3383,13 @@
     <xf numFmtId="166" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3472,7 +3469,7 @@
     <xf numFmtId="0" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3490,7 +3487,7 @@
     <xf numFmtId="0" fontId="17" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="9" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3505,13 +3502,13 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="9" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="44" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="9" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3532,7 +3529,7 @@
     <xf numFmtId="0" fontId="34" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="27" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="27" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3547,7 +3544,7 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="24" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3565,7 +3562,7 @@
     <xf numFmtId="0" fontId="28" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="31" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="31" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3604,7 +3601,7 @@
     <xf numFmtId="0" fontId="28" fillId="9" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="31" fillId="9" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="31" fillId="9" borderId="71" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3625,7 +3622,7 @@
     <xf numFmtId="0" fontId="28" fillId="9" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="31" fillId="9" borderId="63" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="31" fillId="9" borderId="63" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3656,7 +3653,7 @@
     <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="33" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="33" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3671,6 +3668,108 @@
     <xf numFmtId="0" fontId="37" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="9" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -3689,107 +3788,44 @@
     <xf numFmtId="0" fontId="13" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="9" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="9" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="9" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="9" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="19" fillId="9" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3797,6 +3833,30 @@
     <xf numFmtId="0" fontId="22" fillId="10" borderId="78" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3823,69 +3883,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="79" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="81" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="80" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="10" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4311,174 +4308,174 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:56" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="267" t="s">
+      <c r="A1" s="248" t="s">
         <v>325</v>
       </c>
-      <c r="B1" s="266"/>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="266"/>
-      <c r="F1" s="266"/>
-      <c r="G1" s="266"/>
-      <c r="H1" s="266"/>
-      <c r="I1" s="266"/>
-      <c r="J1" s="266"/>
-      <c r="K1" s="266"/>
-      <c r="L1" s="266"/>
-      <c r="M1" s="266"/>
-      <c r="N1" s="266"/>
-      <c r="O1" s="265" t="s">
+      <c r="B1" s="247"/>
+      <c r="C1" s="247"/>
+      <c r="D1" s="247"/>
+      <c r="E1" s="247"/>
+      <c r="F1" s="247"/>
+      <c r="G1" s="247"/>
+      <c r="H1" s="247"/>
+      <c r="I1" s="247"/>
+      <c r="J1" s="247"/>
+      <c r="K1" s="247"/>
+      <c r="L1" s="247"/>
+      <c r="M1" s="247"/>
+      <c r="N1" s="247"/>
+      <c r="O1" s="246" t="s">
         <v>323</v>
       </c>
-      <c r="P1" s="265"/>
-      <c r="Q1" s="265"/>
-      <c r="R1" s="265"/>
-      <c r="S1" s="265"/>
-      <c r="T1" s="265"/>
-      <c r="U1" s="265"/>
-      <c r="V1" s="265"/>
-      <c r="W1" s="265"/>
-      <c r="X1" s="265"/>
-      <c r="Y1" s="265"/>
-      <c r="Z1" s="265"/>
-      <c r="AA1" s="265"/>
-      <c r="AB1" s="265"/>
-      <c r="AC1" s="265"/>
-      <c r="AD1" s="265"/>
-      <c r="AE1" s="265"/>
-      <c r="AF1" s="265"/>
-      <c r="AG1" s="265"/>
-      <c r="AH1" s="266" t="s">
+      <c r="P1" s="246"/>
+      <c r="Q1" s="246"/>
+      <c r="R1" s="246"/>
+      <c r="S1" s="246"/>
+      <c r="T1" s="246"/>
+      <c r="U1" s="246"/>
+      <c r="V1" s="246"/>
+      <c r="W1" s="246"/>
+      <c r="X1" s="246"/>
+      <c r="Y1" s="246"/>
+      <c r="Z1" s="246"/>
+      <c r="AA1" s="246"/>
+      <c r="AB1" s="246"/>
+      <c r="AC1" s="246"/>
+      <c r="AD1" s="246"/>
+      <c r="AE1" s="246"/>
+      <c r="AF1" s="246"/>
+      <c r="AG1" s="246"/>
+      <c r="AH1" s="247" t="s">
         <v>317</v>
       </c>
-      <c r="AI1" s="266"/>
-      <c r="AJ1" s="266"/>
-      <c r="AK1" s="266"/>
-      <c r="AL1" s="263" t="s">
+      <c r="AI1" s="247"/>
+      <c r="AJ1" s="247"/>
+      <c r="AK1" s="247"/>
+      <c r="AL1" s="244" t="s">
         <v>324</v>
       </c>
-      <c r="AM1" s="263"/>
-      <c r="AN1" s="263"/>
-      <c r="AO1" s="263"/>
-      <c r="AP1" s="263"/>
-      <c r="AQ1" s="263"/>
-      <c r="AR1" s="263"/>
-      <c r="AS1" s="263"/>
-      <c r="AT1" s="263"/>
-      <c r="AU1" s="263"/>
-      <c r="AV1" s="263"/>
-      <c r="AW1" s="263"/>
-      <c r="AX1" s="263"/>
-      <c r="AY1" s="263"/>
-      <c r="AZ1" s="263"/>
-      <c r="BA1" s="263"/>
-      <c r="BB1" s="263"/>
-      <c r="BC1" s="263"/>
-      <c r="BD1" s="264"/>
+      <c r="AM1" s="244"/>
+      <c r="AN1" s="244"/>
+      <c r="AO1" s="244"/>
+      <c r="AP1" s="244"/>
+      <c r="AQ1" s="244"/>
+      <c r="AR1" s="244"/>
+      <c r="AS1" s="244"/>
+      <c r="AT1" s="244"/>
+      <c r="AU1" s="244"/>
+      <c r="AV1" s="244"/>
+      <c r="AW1" s="244"/>
+      <c r="AX1" s="244"/>
+      <c r="AY1" s="244"/>
+      <c r="AZ1" s="244"/>
+      <c r="BA1" s="244"/>
+      <c r="BB1" s="244"/>
+      <c r="BC1" s="244"/>
+      <c r="BD1" s="245"/>
     </row>
     <row r="2" spans="1:56" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="233" t="s">
+      <c r="A2" s="267" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="234"/>
+      <c r="B2" s="268"/>
       <c r="C2" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D2" s="237" t="s">
+      <c r="D2" s="271" t="s">
         <v>327</v>
       </c>
-      <c r="E2" s="237"/>
-      <c r="F2" s="269" t="s">
+      <c r="E2" s="271"/>
+      <c r="F2" s="236" t="s">
         <v>326</v>
       </c>
-      <c r="G2" s="269"/>
-      <c r="H2" s="269"/>
-      <c r="I2" s="269"/>
-      <c r="J2" s="269"/>
-      <c r="K2" s="269"/>
-      <c r="L2" s="269"/>
-      <c r="M2" s="269"/>
-      <c r="N2" s="269"/>
-      <c r="O2" s="269"/>
-      <c r="P2" s="269"/>
-      <c r="Q2" s="269"/>
-      <c r="R2" s="269"/>
-      <c r="S2" s="269"/>
-      <c r="T2" s="269"/>
-      <c r="U2" s="269"/>
-      <c r="V2" s="269"/>
-      <c r="W2" s="269"/>
-      <c r="X2" s="269"/>
-      <c r="Y2" s="269"/>
-      <c r="Z2" s="269"/>
-      <c r="AA2" s="269"/>
-      <c r="AB2" s="269"/>
-      <c r="AC2" s="269"/>
-      <c r="AD2" s="269"/>
-      <c r="AE2" s="269"/>
-      <c r="AF2" s="269"/>
-      <c r="AG2" s="269"/>
-      <c r="AH2" s="269"/>
-      <c r="AI2" s="269"/>
-      <c r="AJ2" s="269"/>
-      <c r="AK2" s="269"/>
-      <c r="AL2" s="269"/>
-      <c r="AM2" s="269"/>
-      <c r="AN2" s="269"/>
-      <c r="AO2" s="269"/>
-      <c r="AP2" s="269"/>
-      <c r="AQ2" s="269"/>
-      <c r="AR2" s="269"/>
-      <c r="AS2" s="269"/>
-      <c r="AT2" s="269"/>
-      <c r="AU2" s="269"/>
-      <c r="AV2" s="269"/>
-      <c r="AW2" s="269"/>
-      <c r="AX2" s="269"/>
-      <c r="AY2" s="269"/>
-      <c r="AZ2" s="269"/>
-      <c r="BA2" s="269"/>
-      <c r="BB2" s="269"/>
-      <c r="BC2" s="269"/>
-      <c r="BD2" s="270"/>
+      <c r="G2" s="236"/>
+      <c r="H2" s="236"/>
+      <c r="I2" s="236"/>
+      <c r="J2" s="236"/>
+      <c r="K2" s="236"/>
+      <c r="L2" s="236"/>
+      <c r="M2" s="236"/>
+      <c r="N2" s="236"/>
+      <c r="O2" s="236"/>
+      <c r="P2" s="236"/>
+      <c r="Q2" s="236"/>
+      <c r="R2" s="236"/>
+      <c r="S2" s="236"/>
+      <c r="T2" s="236"/>
+      <c r="U2" s="236"/>
+      <c r="V2" s="236"/>
+      <c r="W2" s="236"/>
+      <c r="X2" s="236"/>
+      <c r="Y2" s="236"/>
+      <c r="Z2" s="236"/>
+      <c r="AA2" s="236"/>
+      <c r="AB2" s="236"/>
+      <c r="AC2" s="236"/>
+      <c r="AD2" s="236"/>
+      <c r="AE2" s="236"/>
+      <c r="AF2" s="236"/>
+      <c r="AG2" s="236"/>
+      <c r="AH2" s="236"/>
+      <c r="AI2" s="236"/>
+      <c r="AJ2" s="236"/>
+      <c r="AK2" s="236"/>
+      <c r="AL2" s="236"/>
+      <c r="AM2" s="236"/>
+      <c r="AN2" s="236"/>
+      <c r="AO2" s="236"/>
+      <c r="AP2" s="236"/>
+      <c r="AQ2" s="236"/>
+      <c r="AR2" s="236"/>
+      <c r="AS2" s="236"/>
+      <c r="AT2" s="236"/>
+      <c r="AU2" s="236"/>
+      <c r="AV2" s="236"/>
+      <c r="AW2" s="236"/>
+      <c r="AX2" s="236"/>
+      <c r="AY2" s="236"/>
+      <c r="AZ2" s="236"/>
+      <c r="BA2" s="236"/>
+      <c r="BB2" s="236"/>
+      <c r="BC2" s="236"/>
+      <c r="BD2" s="237"/>
     </row>
     <row r="3" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="233" t="s">
+      <c r="A3" s="267" t="s">
         <v>295</v>
       </c>
-      <c r="B3" s="234"/>
+      <c r="B3" s="268"/>
       <c r="C3" s="141" t="s">
         <v>286</v>
       </c>
-      <c r="D3" s="262" t="s">
+      <c r="D3" s="250" t="s">
         <v>328</v>
       </c>
-      <c r="E3" s="262"/>
+      <c r="E3" s="250"/>
       <c r="F3" s="145">
         <v>75263586</v>
       </c>
       <c r="G3" s="145"/>
       <c r="H3" s="145"/>
-      <c r="I3" s="262" t="s">
+      <c r="I3" s="250" t="s">
         <v>332</v>
       </c>
-      <c r="J3" s="262"/>
-      <c r="K3" s="262"/>
-      <c r="L3" s="262"/>
-      <c r="M3" s="262"/>
-      <c r="N3" s="262"/>
-      <c r="O3" s="262"/>
-      <c r="P3" s="262"/>
-      <c r="Q3" s="262"/>
-      <c r="R3" s="272" t="s">
+      <c r="J3" s="250"/>
+      <c r="K3" s="250"/>
+      <c r="L3" s="250"/>
+      <c r="M3" s="250"/>
+      <c r="N3" s="250"/>
+      <c r="O3" s="250"/>
+      <c r="P3" s="250"/>
+      <c r="Q3" s="250"/>
+      <c r="R3" s="239" t="s">
         <v>334</v>
       </c>
-      <c r="S3" s="272"/>
-      <c r="T3" s="272"/>
-      <c r="U3" s="272"/>
-      <c r="V3" s="272"/>
-      <c r="W3" s="272"/>
-      <c r="X3" s="272"/>
+      <c r="S3" s="239"/>
+      <c r="T3" s="239"/>
+      <c r="U3" s="239"/>
+      <c r="V3" s="239"/>
+      <c r="W3" s="239"/>
+      <c r="X3" s="239"/>
       <c r="Y3" s="143"/>
       <c r="Z3" s="143"/>
       <c r="AA3" s="143"/>
@@ -4513,42 +4510,42 @@
       <c r="BD3" s="139"/>
     </row>
     <row r="4" spans="1:56" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="233" t="s">
+      <c r="A4" s="267" t="s">
         <v>296</v>
       </c>
-      <c r="B4" s="234"/>
+      <c r="B4" s="268"/>
       <c r="C4" s="141" t="s">
         <v>287</v>
       </c>
-      <c r="D4" s="262" t="s">
+      <c r="D4" s="250" t="s">
         <v>329</v>
       </c>
-      <c r="E4" s="262"/>
+      <c r="E4" s="250"/>
       <c r="F4" s="145">
         <v>99826036</v>
       </c>
       <c r="G4" s="145"/>
       <c r="H4" s="145"/>
-      <c r="I4" s="262" t="s">
+      <c r="I4" s="250" t="s">
         <v>333</v>
       </c>
-      <c r="J4" s="262"/>
-      <c r="K4" s="262"/>
-      <c r="L4" s="262"/>
-      <c r="M4" s="262"/>
-      <c r="N4" s="262"/>
-      <c r="O4" s="262"/>
-      <c r="P4" s="262"/>
-      <c r="Q4" s="262"/>
-      <c r="R4" s="272" t="s">
+      <c r="J4" s="250"/>
+      <c r="K4" s="250"/>
+      <c r="L4" s="250"/>
+      <c r="M4" s="250"/>
+      <c r="N4" s="250"/>
+      <c r="O4" s="250"/>
+      <c r="P4" s="250"/>
+      <c r="Q4" s="250"/>
+      <c r="R4" s="239" t="s">
         <v>335</v>
       </c>
-      <c r="S4" s="272"/>
-      <c r="T4" s="272"/>
-      <c r="U4" s="272"/>
-      <c r="V4" s="272"/>
-      <c r="W4" s="272"/>
-      <c r="X4" s="272"/>
+      <c r="S4" s="239"/>
+      <c r="T4" s="239"/>
+      <c r="U4" s="239"/>
+      <c r="V4" s="239"/>
+      <c r="W4" s="239"/>
+      <c r="X4" s="239"/>
       <c r="Y4" s="143"/>
       <c r="Z4" s="143"/>
       <c r="AA4" s="143"/>
@@ -4583,35 +4580,35 @@
       <c r="BD4" s="139"/>
     </row>
     <row r="5" spans="1:56" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="235" t="s">
+      <c r="A5" s="269" t="s">
         <v>302</v>
       </c>
-      <c r="B5" s="236"/>
+      <c r="B5" s="270"/>
       <c r="C5" s="142" t="s">
         <v>288</v>
       </c>
-      <c r="D5" s="238" t="s">
+      <c r="D5" s="272" t="s">
         <v>330</v>
       </c>
-      <c r="E5" s="238"/>
-      <c r="F5" s="271" t="s">
+      <c r="E5" s="272"/>
+      <c r="F5" s="238" t="s">
         <v>331</v>
       </c>
-      <c r="G5" s="271"/>
-      <c r="H5" s="271"/>
-      <c r="I5" s="271"/>
-      <c r="J5" s="271"/>
-      <c r="K5" s="271"/>
-      <c r="L5" s="271"/>
-      <c r="M5" s="271"/>
-      <c r="N5" s="271"/>
-      <c r="O5" s="271"/>
-      <c r="P5" s="271"/>
-      <c r="Q5" s="271"/>
-      <c r="R5" s="271"/>
-      <c r="S5" s="271"/>
-      <c r="T5" s="271"/>
-      <c r="U5" s="271"/>
+      <c r="G5" s="238"/>
+      <c r="H5" s="238"/>
+      <c r="I5" s="238"/>
+      <c r="J5" s="238"/>
+      <c r="K5" s="238"/>
+      <c r="L5" s="238"/>
+      <c r="M5" s="238"/>
+      <c r="N5" s="238"/>
+      <c r="O5" s="238"/>
+      <c r="P5" s="238"/>
+      <c r="Q5" s="238"/>
+      <c r="R5" s="238"/>
+      <c r="S5" s="238"/>
+      <c r="T5" s="238"/>
+      <c r="U5" s="238"/>
       <c r="V5" s="144"/>
       <c r="W5" s="144"/>
       <c r="X5" s="144"/>
@@ -4649,101 +4646,101 @@
       <c r="BD5" s="140"/>
     </row>
     <row r="6" spans="1:56" s="80" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="242" t="s">
+      <c r="A6" s="259" t="s">
         <v>310</v>
       </c>
-      <c r="B6" s="244" t="s">
+      <c r="B6" s="261" t="s">
         <v>160</v>
       </c>
-      <c r="C6" s="244" t="s">
+      <c r="C6" s="261" t="s">
         <v>157</v>
       </c>
-      <c r="D6" s="244" t="s">
+      <c r="D6" s="261" t="s">
         <v>292</v>
       </c>
-      <c r="E6" s="251" t="s">
+      <c r="E6" s="265" t="s">
         <v>159</v>
       </c>
-      <c r="F6" s="252"/>
-      <c r="G6" s="249" t="s">
+      <c r="F6" s="266"/>
+      <c r="G6" s="263" t="s">
         <v>293</v>
       </c>
-      <c r="H6" s="239" t="s">
+      <c r="H6" s="241" t="s">
         <v>135</v>
       </c>
-      <c r="I6" s="240"/>
-      <c r="J6" s="240"/>
-      <c r="K6" s="240"/>
-      <c r="L6" s="240"/>
-      <c r="M6" s="240"/>
-      <c r="N6" s="241"/>
-      <c r="O6" s="239" t="s">
+      <c r="I6" s="242"/>
+      <c r="J6" s="242"/>
+      <c r="K6" s="242"/>
+      <c r="L6" s="242"/>
+      <c r="M6" s="242"/>
+      <c r="N6" s="243"/>
+      <c r="O6" s="241" t="s">
         <v>136</v>
       </c>
-      <c r="P6" s="240"/>
-      <c r="Q6" s="240"/>
-      <c r="R6" s="240"/>
-      <c r="S6" s="240"/>
-      <c r="T6" s="240"/>
-      <c r="U6" s="241"/>
-      <c r="V6" s="239" t="s">
+      <c r="P6" s="242"/>
+      <c r="Q6" s="242"/>
+      <c r="R6" s="242"/>
+      <c r="S6" s="242"/>
+      <c r="T6" s="242"/>
+      <c r="U6" s="243"/>
+      <c r="V6" s="241" t="s">
         <v>1</v>
       </c>
-      <c r="W6" s="240"/>
-      <c r="X6" s="240"/>
-      <c r="Y6" s="240"/>
-      <c r="Z6" s="240"/>
-      <c r="AA6" s="240"/>
-      <c r="AB6" s="241"/>
-      <c r="AC6" s="239" t="s">
+      <c r="W6" s="242"/>
+      <c r="X6" s="242"/>
+      <c r="Y6" s="242"/>
+      <c r="Z6" s="242"/>
+      <c r="AA6" s="242"/>
+      <c r="AB6" s="243"/>
+      <c r="AC6" s="241" t="s">
         <v>137</v>
       </c>
-      <c r="AD6" s="240"/>
-      <c r="AE6" s="240"/>
-      <c r="AF6" s="240"/>
-      <c r="AG6" s="240"/>
-      <c r="AH6" s="240"/>
-      <c r="AI6" s="241"/>
-      <c r="AJ6" s="239" t="s">
+      <c r="AD6" s="242"/>
+      <c r="AE6" s="242"/>
+      <c r="AF6" s="242"/>
+      <c r="AG6" s="242"/>
+      <c r="AH6" s="242"/>
+      <c r="AI6" s="243"/>
+      <c r="AJ6" s="241" t="s">
         <v>84</v>
       </c>
-      <c r="AK6" s="240"/>
-      <c r="AL6" s="240"/>
-      <c r="AM6" s="240"/>
-      <c r="AN6" s="240"/>
-      <c r="AO6" s="240"/>
-      <c r="AP6" s="241"/>
-      <c r="AQ6" s="239" t="s">
+      <c r="AK6" s="242"/>
+      <c r="AL6" s="242"/>
+      <c r="AM6" s="242"/>
+      <c r="AN6" s="242"/>
+      <c r="AO6" s="242"/>
+      <c r="AP6" s="243"/>
+      <c r="AQ6" s="241" t="s">
         <v>138</v>
       </c>
-      <c r="AR6" s="240"/>
-      <c r="AS6" s="240"/>
-      <c r="AT6" s="240"/>
-      <c r="AU6" s="240"/>
-      <c r="AV6" s="240"/>
-      <c r="AW6" s="241"/>
-      <c r="AX6" s="239" t="s">
+      <c r="AR6" s="242"/>
+      <c r="AS6" s="242"/>
+      <c r="AT6" s="242"/>
+      <c r="AU6" s="242"/>
+      <c r="AV6" s="242"/>
+      <c r="AW6" s="243"/>
+      <c r="AX6" s="241" t="s">
         <v>139</v>
       </c>
-      <c r="AY6" s="240"/>
-      <c r="AZ6" s="240"/>
-      <c r="BA6" s="240"/>
-      <c r="BB6" s="240"/>
-      <c r="BC6" s="240"/>
-      <c r="BD6" s="241"/>
+      <c r="AY6" s="242"/>
+      <c r="AZ6" s="242"/>
+      <c r="BA6" s="242"/>
+      <c r="BB6" s="242"/>
+      <c r="BC6" s="242"/>
+      <c r="BD6" s="243"/>
     </row>
     <row r="7" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="243"/>
-      <c r="B7" s="245"/>
-      <c r="C7" s="245"/>
-      <c r="D7" s="245"/>
+      <c r="A7" s="260"/>
+      <c r="B7" s="262"/>
+      <c r="C7" s="262"/>
+      <c r="D7" s="262"/>
       <c r="E7" s="154" t="s">
         <v>158</v>
       </c>
       <c r="F7" s="154" t="s">
         <v>309</v>
       </c>
-      <c r="G7" s="250"/>
+      <c r="G7" s="264"/>
       <c r="H7" s="155" t="s">
         <v>297</v>
       </c>
@@ -5017,7 +5014,7 @@
       <c r="BD9" s="89"/>
     </row>
     <row r="10" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="246" t="s">
+      <c r="A10" s="255" t="s">
         <v>311</v>
       </c>
       <c r="B10" s="135"/>
@@ -5085,7 +5082,7 @@
       <c r="BD10" s="89"/>
     </row>
     <row r="11" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="247"/>
+      <c r="A11" s="256"/>
       <c r="B11" s="135"/>
       <c r="C11" s="90" t="s">
         <v>291</v>
@@ -5151,7 +5148,7 @@
       <c r="BD11" s="89"/>
     </row>
     <row r="12" spans="1:56" s="80" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="248"/>
+      <c r="A12" s="258"/>
       <c r="B12" s="135"/>
       <c r="C12" s="90" t="s">
         <v>89</v>
@@ -5341,7 +5338,7 @@
       <c r="BD14" s="89"/>
     </row>
     <row r="15" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="246" t="s">
+      <c r="A15" s="255" t="s">
         <v>312</v>
       </c>
       <c r="B15" s="135"/>
@@ -5411,7 +5408,7 @@
       <c r="BD15" s="89"/>
     </row>
     <row r="16" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="247"/>
+      <c r="A16" s="256"/>
       <c r="B16" s="135"/>
       <c r="C16" s="95" t="s">
         <v>104</v>
@@ -5479,7 +5476,7 @@
       <c r="BD16" s="89"/>
     </row>
     <row r="17" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="247"/>
+      <c r="A17" s="256"/>
       <c r="B17" s="135"/>
       <c r="C17" s="95" t="s">
         <v>105</v>
@@ -5547,7 +5544,7 @@
       <c r="BD17" s="89"/>
     </row>
     <row r="18" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="247"/>
+      <c r="A18" s="256"/>
       <c r="B18" s="135"/>
       <c r="C18" s="95" t="s">
         <v>106</v>
@@ -5615,7 +5612,7 @@
       <c r="BD18" s="89"/>
     </row>
     <row r="19" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="247"/>
+      <c r="A19" s="256"/>
       <c r="B19" s="135"/>
       <c r="C19" s="95" t="s">
         <v>99</v>
@@ -5683,7 +5680,7 @@
       <c r="BD19" s="89"/>
     </row>
     <row r="20" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="247"/>
+      <c r="A20" s="256"/>
       <c r="B20" s="135"/>
       <c r="C20" s="95" t="s">
         <v>107</v>
@@ -5751,7 +5748,7 @@
       <c r="BD20" s="89"/>
     </row>
     <row r="21" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="247"/>
+      <c r="A21" s="256"/>
       <c r="B21" s="135"/>
       <c r="C21" s="95" t="s">
         <v>108</v>
@@ -5819,7 +5816,7 @@
       <c r="BD21" s="89"/>
     </row>
     <row r="22" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="247"/>
+      <c r="A22" s="256"/>
       <c r="B22" s="135"/>
       <c r="C22" s="95" t="s">
         <v>109</v>
@@ -5887,7 +5884,7 @@
       <c r="BD22" s="89"/>
     </row>
     <row r="23" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="247"/>
+      <c r="A23" s="256"/>
       <c r="B23" s="135"/>
       <c r="C23" s="95" t="s">
         <v>110</v>
@@ -5955,7 +5952,7 @@
       <c r="BD23" s="89"/>
     </row>
     <row r="24" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="247"/>
+      <c r="A24" s="256"/>
       <c r="B24" s="135"/>
       <c r="C24" s="95" t="s">
         <v>111</v>
@@ -6023,7 +6020,7 @@
       <c r="BD24" s="89"/>
     </row>
     <row r="25" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="247"/>
+      <c r="A25" s="256"/>
       <c r="B25" s="135"/>
       <c r="C25" s="95" t="s">
         <v>112</v>
@@ -6091,7 +6088,7 @@
       <c r="BD25" s="89"/>
     </row>
     <row r="26" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="247"/>
+      <c r="A26" s="256"/>
       <c r="B26" s="135"/>
       <c r="C26" s="95" t="s">
         <v>113</v>
@@ -6159,7 +6156,7 @@
       <c r="BD26" s="89"/>
     </row>
     <row r="27" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="247"/>
+      <c r="A27" s="256"/>
       <c r="B27" s="135"/>
       <c r="C27" s="95" t="s">
         <v>114</v>
@@ -6227,7 +6224,7 @@
       <c r="BD27" s="89"/>
     </row>
     <row r="28" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="247"/>
+      <c r="A28" s="256"/>
       <c r="B28" s="135"/>
       <c r="C28" s="95" t="s">
         <v>115</v>
@@ -6295,7 +6292,7 @@
       <c r="BD28" s="89"/>
     </row>
     <row r="29" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="247"/>
+      <c r="A29" s="256"/>
       <c r="B29" s="135"/>
       <c r="C29" s="95" t="s">
         <v>116</v>
@@ -6363,7 +6360,7 @@
       <c r="BD29" s="89"/>
     </row>
     <row r="30" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="248"/>
+      <c r="A30" s="258"/>
       <c r="B30" s="135"/>
       <c r="C30" s="95" t="s">
         <v>117</v>
@@ -6493,7 +6490,7 @@
       <c r="BD31" s="89"/>
     </row>
     <row r="32" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="246" t="s">
+      <c r="A32" s="255" t="s">
         <v>313</v>
       </c>
       <c r="B32" s="135"/>
@@ -6561,7 +6558,7 @@
       <c r="BD32" s="89"/>
     </row>
     <row r="33" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="247"/>
+      <c r="A33" s="256"/>
       <c r="B33" s="135"/>
       <c r="C33" s="95" t="s">
         <v>105</v>
@@ -6627,7 +6624,7 @@
       <c r="BD33" s="89"/>
     </row>
     <row r="34" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="247"/>
+      <c r="A34" s="256"/>
       <c r="B34" s="135"/>
       <c r="C34" s="95" t="s">
         <v>108</v>
@@ -6693,7 +6690,7 @@
       <c r="BD34" s="89"/>
     </row>
     <row r="35" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="248"/>
+      <c r="A35" s="258"/>
       <c r="B35" s="135"/>
       <c r="C35" s="95" t="s">
         <v>91</v>
@@ -6821,7 +6818,7 @@
       <c r="BD36" s="89"/>
     </row>
     <row r="37" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="246" t="s">
+      <c r="A37" s="255" t="s">
         <v>314</v>
       </c>
       <c r="B37" s="136" t="s">
@@ -6885,7 +6882,7 @@
       <c r="BD37" s="89"/>
     </row>
     <row r="38" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="247"/>
+      <c r="A38" s="256"/>
       <c r="B38" s="137" t="s">
         <v>164</v>
       </c>
@@ -6953,7 +6950,7 @@
       <c r="BD38" s="89"/>
     </row>
     <row r="39" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="247"/>
+      <c r="A39" s="256"/>
       <c r="B39" s="137" t="s">
         <v>165</v>
       </c>
@@ -7021,7 +7018,7 @@
       <c r="BD39" s="89"/>
     </row>
     <row r="40" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="247"/>
+      <c r="A40" s="256"/>
       <c r="B40" s="136" t="s">
         <v>225</v>
       </c>
@@ -7083,7 +7080,7 @@
       <c r="BD40" s="89"/>
     </row>
     <row r="41" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="247"/>
+      <c r="A41" s="256"/>
       <c r="B41" s="137" t="s">
         <v>226</v>
       </c>
@@ -7151,7 +7148,7 @@
       <c r="BD41" s="89"/>
     </row>
     <row r="42" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="247"/>
+      <c r="A42" s="256"/>
       <c r="B42" s="136" t="s">
         <v>227</v>
       </c>
@@ -7213,7 +7210,7 @@
       <c r="BD42" s="89"/>
     </row>
     <row r="43" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="247"/>
+      <c r="A43" s="256"/>
       <c r="B43" s="137" t="s">
         <v>228</v>
       </c>
@@ -7277,7 +7274,7 @@
       <c r="BD43" s="89"/>
     </row>
     <row r="44" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="247"/>
+      <c r="A44" s="256"/>
       <c r="B44" s="135"/>
       <c r="C44" s="90" t="s">
         <v>174</v>
@@ -7343,7 +7340,7 @@
       <c r="BD44" s="89"/>
     </row>
     <row r="45" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="247"/>
+      <c r="A45" s="256"/>
       <c r="B45" s="135"/>
       <c r="C45" s="90" t="s">
         <v>173</v>
@@ -7409,7 +7406,7 @@
       <c r="BD45" s="89"/>
     </row>
     <row r="46" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="247"/>
+      <c r="A46" s="256"/>
       <c r="B46" s="136" t="s">
         <v>229</v>
       </c>
@@ -7471,7 +7468,7 @@
       <c r="BD46" s="89"/>
     </row>
     <row r="47" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="247"/>
+      <c r="A47" s="256"/>
       <c r="B47" s="137" t="s">
         <v>230</v>
       </c>
@@ -7539,7 +7536,7 @@
       <c r="BD47" s="89"/>
     </row>
     <row r="48" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="247"/>
+      <c r="A48" s="256"/>
       <c r="B48" s="137" t="s">
         <v>231</v>
       </c>
@@ -7607,7 +7604,7 @@
       <c r="BD48" s="89"/>
     </row>
     <row r="49" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="247"/>
+      <c r="A49" s="256"/>
       <c r="B49" s="137" t="s">
         <v>232</v>
       </c>
@@ -7675,7 +7672,7 @@
       <c r="BD49" s="89"/>
     </row>
     <row r="50" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="247"/>
+      <c r="A50" s="256"/>
       <c r="B50" s="137" t="s">
         <v>233</v>
       </c>
@@ -7743,7 +7740,7 @@
       <c r="BD50" s="89"/>
     </row>
     <row r="51" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="247"/>
+      <c r="A51" s="256"/>
       <c r="B51" s="136" t="s">
         <v>234</v>
       </c>
@@ -7805,7 +7802,7 @@
       <c r="BD51" s="89"/>
     </row>
     <row r="52" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="247"/>
+      <c r="A52" s="256"/>
       <c r="B52" s="137" t="s">
         <v>235</v>
       </c>
@@ -7873,7 +7870,7 @@
       <c r="BD52" s="89"/>
     </row>
     <row r="53" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="247"/>
+      <c r="A53" s="256"/>
       <c r="B53" s="137" t="s">
         <v>236</v>
       </c>
@@ -7941,7 +7938,7 @@
       <c r="BD53" s="89"/>
     </row>
     <row r="54" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="247"/>
+      <c r="A54" s="256"/>
       <c r="B54" s="136" t="s">
         <v>237</v>
       </c>
@@ -8003,7 +8000,7 @@
       <c r="BD54" s="89"/>
     </row>
     <row r="55" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="247"/>
+      <c r="A55" s="256"/>
       <c r="B55" s="137" t="s">
         <v>238</v>
       </c>
@@ -8069,7 +8066,7 @@
       <c r="BD55" s="89"/>
     </row>
     <row r="56" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="247"/>
+      <c r="A56" s="256"/>
       <c r="B56" s="135"/>
       <c r="C56" s="90" t="s">
         <v>183</v>
@@ -8137,7 +8134,7 @@
       <c r="BD56" s="89"/>
     </row>
     <row r="57" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="247"/>
+      <c r="A57" s="256"/>
       <c r="B57" s="135"/>
       <c r="C57" s="90" t="s">
         <v>182</v>
@@ -8205,7 +8202,7 @@
       <c r="BD57" s="89"/>
     </row>
     <row r="58" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="247"/>
+      <c r="A58" s="256"/>
       <c r="B58" s="137" t="s">
         <v>239</v>
       </c>
@@ -8271,7 +8268,7 @@
       <c r="BD58" s="89"/>
     </row>
     <row r="59" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="247"/>
+      <c r="A59" s="256"/>
       <c r="B59" s="135"/>
       <c r="C59" s="90" t="s">
         <v>282</v>
@@ -8339,7 +8336,7 @@
       <c r="BD59" s="89"/>
     </row>
     <row r="60" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="247"/>
+      <c r="A60" s="256"/>
       <c r="B60" s="135"/>
       <c r="C60" s="90" t="s">
         <v>283</v>
@@ -8407,7 +8404,7 @@
       <c r="BD60" s="89"/>
     </row>
     <row r="61" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="247"/>
+      <c r="A61" s="256"/>
       <c r="B61" s="136" t="s">
         <v>240</v>
       </c>
@@ -8469,7 +8466,7 @@
       <c r="BD61" s="89"/>
     </row>
     <row r="62" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="247"/>
+      <c r="A62" s="256"/>
       <c r="B62" s="137" t="s">
         <v>241</v>
       </c>
@@ -8537,7 +8534,7 @@
       <c r="BD62" s="89"/>
     </row>
     <row r="63" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="247"/>
+      <c r="A63" s="256"/>
       <c r="B63" s="137" t="s">
         <v>242</v>
       </c>
@@ -8605,7 +8602,7 @@
       <c r="BD63" s="89"/>
     </row>
     <row r="64" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="247"/>
+      <c r="A64" s="256"/>
       <c r="B64" s="136" t="s">
         <v>243</v>
       </c>
@@ -8667,7 +8664,7 @@
       <c r="BD64" s="89"/>
     </row>
     <row r="65" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="247"/>
+      <c r="A65" s="256"/>
       <c r="B65" s="137" t="s">
         <v>244</v>
       </c>
@@ -8735,7 +8732,7 @@
       <c r="BD65" s="89"/>
     </row>
     <row r="66" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="247"/>
+      <c r="A66" s="256"/>
       <c r="B66" s="136" t="s">
         <v>247</v>
       </c>
@@ -8797,7 +8794,7 @@
       <c r="BD66" s="89"/>
     </row>
     <row r="67" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="247"/>
+      <c r="A67" s="256"/>
       <c r="B67" s="137" t="s">
         <v>248</v>
       </c>
@@ -8865,7 +8862,7 @@
       <c r="BD67" s="89"/>
     </row>
     <row r="68" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="247"/>
+      <c r="A68" s="256"/>
       <c r="B68" s="136" t="s">
         <v>251</v>
       </c>
@@ -8927,7 +8924,7 @@
       <c r="BD68" s="89"/>
     </row>
     <row r="69" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="247"/>
+      <c r="A69" s="256"/>
       <c r="B69" s="137" t="s">
         <v>252</v>
       </c>
@@ -8995,7 +8992,7 @@
       <c r="BD69" s="89"/>
     </row>
     <row r="70" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="247"/>
+      <c r="A70" s="256"/>
       <c r="B70" s="137" t="s">
         <v>253</v>
       </c>
@@ -9063,7 +9060,7 @@
       <c r="BD70" s="89"/>
     </row>
     <row r="71" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="247"/>
+      <c r="A71" s="256"/>
       <c r="B71" s="136" t="s">
         <v>254</v>
       </c>
@@ -9125,7 +9122,7 @@
       <c r="BD71" s="89"/>
     </row>
     <row r="72" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="247"/>
+      <c r="A72" s="256"/>
       <c r="B72" s="137" t="s">
         <v>255</v>
       </c>
@@ -9193,7 +9190,7 @@
       <c r="BD72" s="89"/>
     </row>
     <row r="73" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="247"/>
+      <c r="A73" s="256"/>
       <c r="B73" s="136" t="s">
         <v>256</v>
       </c>
@@ -9255,7 +9252,7 @@
       <c r="BD73" s="89"/>
     </row>
     <row r="74" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="248"/>
+      <c r="A74" s="258"/>
       <c r="B74" s="137" t="s">
         <v>257</v>
       </c>
@@ -9447,7 +9444,7 @@
       <c r="BD76" s="89"/>
     </row>
     <row r="77" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="246" t="s">
+      <c r="A77" s="255" t="s">
         <v>162</v>
       </c>
       <c r="B77" s="135"/>
@@ -9515,7 +9512,7 @@
       <c r="BD77" s="89"/>
     </row>
     <row r="78" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="248"/>
+      <c r="A78" s="258"/>
       <c r="B78" s="135"/>
       <c r="C78" s="90" t="s">
         <v>95</v>
@@ -9643,7 +9640,7 @@
       <c r="BD79" s="89"/>
     </row>
     <row r="80" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="246" t="s">
+      <c r="A80" s="255" t="s">
         <v>162</v>
       </c>
       <c r="B80" s="135"/>
@@ -9711,7 +9708,7 @@
       <c r="BD80" s="89"/>
     </row>
     <row r="81" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="248"/>
+      <c r="A81" s="258"/>
       <c r="B81" s="135"/>
       <c r="C81" s="90" t="s">
         <v>93</v>
@@ -9839,7 +9836,7 @@
       <c r="BD82" s="89"/>
     </row>
     <row r="83" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="246" t="s">
+      <c r="A83" s="255" t="s">
         <v>162</v>
       </c>
       <c r="B83" s="135"/>
@@ -9907,7 +9904,7 @@
       <c r="BD83" s="89"/>
     </row>
     <row r="84" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="248"/>
+      <c r="A84" s="258"/>
       <c r="B84" s="135"/>
       <c r="C84" s="90" t="s">
         <v>134</v>
@@ -10097,7 +10094,7 @@
       <c r="BD86" s="89"/>
     </row>
     <row r="87" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="246" t="s">
+      <c r="A87" s="255" t="s">
         <v>316</v>
       </c>
       <c r="B87" s="135"/>
@@ -10165,7 +10162,7 @@
       <c r="BD87" s="89"/>
     </row>
     <row r="88" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="247"/>
+      <c r="A88" s="256"/>
       <c r="B88" s="135"/>
       <c r="C88" s="95" t="s">
         <v>119</v>
@@ -10231,7 +10228,7 @@
       <c r="BD88" s="89"/>
     </row>
     <row r="89" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="247"/>
+      <c r="A89" s="256"/>
       <c r="B89" s="135"/>
       <c r="C89" s="95" t="s">
         <v>120</v>
@@ -10297,7 +10294,7 @@
       <c r="BD89" s="89"/>
     </row>
     <row r="90" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="247"/>
+      <c r="A90" s="256"/>
       <c r="B90" s="135"/>
       <c r="C90" s="95" t="s">
         <v>121</v>
@@ -10363,7 +10360,7 @@
       <c r="BD90" s="89"/>
     </row>
     <row r="91" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="247"/>
+      <c r="A91" s="256"/>
       <c r="B91" s="135"/>
       <c r="C91" s="95" t="s">
         <v>122</v>
@@ -10429,7 +10426,7 @@
       <c r="BD91" s="89"/>
     </row>
     <row r="92" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="247"/>
+      <c r="A92" s="256"/>
       <c r="B92" s="135"/>
       <c r="C92" s="95" t="s">
         <v>123</v>
@@ -10495,7 +10492,7 @@
       <c r="BD92" s="89"/>
     </row>
     <row r="93" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="247"/>
+      <c r="A93" s="256"/>
       <c r="B93" s="135"/>
       <c r="C93" s="95" t="s">
         <v>124</v>
@@ -10561,7 +10558,7 @@
       <c r="BD93" s="89"/>
     </row>
     <row r="94" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="247"/>
+      <c r="A94" s="256"/>
       <c r="B94" s="135"/>
       <c r="C94" s="95" t="s">
         <v>125</v>
@@ -10627,7 +10624,7 @@
       <c r="BD94" s="89"/>
     </row>
     <row r="95" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="247"/>
+      <c r="A95" s="256"/>
       <c r="B95" s="135"/>
       <c r="C95" s="95" t="s">
         <v>126</v>
@@ -10693,7 +10690,7 @@
       <c r="BD95" s="89"/>
     </row>
     <row r="96" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="247"/>
+      <c r="A96" s="256"/>
       <c r="B96" s="135"/>
       <c r="C96" s="95" t="s">
         <v>127</v>
@@ -10759,7 +10756,7 @@
       <c r="BD96" s="89"/>
     </row>
     <row r="97" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="247"/>
+      <c r="A97" s="256"/>
       <c r="B97" s="135"/>
       <c r="C97" s="95" t="s">
         <v>128</v>
@@ -10825,7 +10822,7 @@
       <c r="BD97" s="89"/>
     </row>
     <row r="98" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="247"/>
+      <c r="A98" s="256"/>
       <c r="B98" s="135"/>
       <c r="C98" s="95" t="s">
         <v>129</v>
@@ -10891,7 +10888,7 @@
       <c r="BD98" s="89"/>
     </row>
     <row r="99" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="247"/>
+      <c r="A99" s="256"/>
       <c r="B99" s="135"/>
       <c r="C99" s="95" t="s">
         <v>130</v>
@@ -10957,7 +10954,7 @@
       <c r="BD99" s="89"/>
     </row>
     <row r="100" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="247"/>
+      <c r="A100" s="256"/>
       <c r="B100" s="135"/>
       <c r="C100" s="95" t="s">
         <v>131</v>
@@ -11023,7 +11020,7 @@
       <c r="BD100" s="89"/>
     </row>
     <row r="101" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="247"/>
+      <c r="A101" s="256"/>
       <c r="B101" s="135"/>
       <c r="C101" s="95" t="s">
         <v>132</v>
@@ -11089,7 +11086,7 @@
       <c r="BD101" s="89"/>
     </row>
     <row r="102" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="248"/>
+      <c r="A102" s="258"/>
       <c r="B102" s="135"/>
       <c r="C102" s="95" t="s">
         <v>133</v>
@@ -11217,7 +11214,7 @@
       <c r="BD103" s="89"/>
     </row>
     <row r="104" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="246" t="s">
+      <c r="A104" s="255" t="s">
         <v>315</v>
       </c>
       <c r="B104" s="136" t="s">
@@ -11281,7 +11278,7 @@
       <c r="BD104" s="89"/>
     </row>
     <row r="105" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="247"/>
+      <c r="A105" s="256"/>
       <c r="B105" s="137">
         <v>3.0101010000000001</v>
       </c>
@@ -11349,7 +11346,7 @@
       <c r="BD105" s="89"/>
     </row>
     <row r="106" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="247"/>
+      <c r="A106" s="256"/>
       <c r="B106" s="136" t="s">
         <v>224</v>
       </c>
@@ -11411,7 +11408,7 @@
       <c r="BD106" s="89"/>
     </row>
     <row r="107" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="247"/>
+      <c r="A107" s="256"/>
       <c r="B107" s="137" t="s">
         <v>164</v>
       </c>
@@ -11479,7 +11476,7 @@
       <c r="BD107" s="89"/>
     </row>
     <row r="108" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="247"/>
+      <c r="A108" s="256"/>
       <c r="B108" s="137" t="s">
         <v>165</v>
       </c>
@@ -11547,7 +11544,7 @@
       <c r="BD108" s="89"/>
     </row>
     <row r="109" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="247"/>
+      <c r="A109" s="256"/>
       <c r="B109" s="136" t="s">
         <v>225</v>
       </c>
@@ -11609,7 +11606,7 @@
       <c r="BD109" s="89"/>
     </row>
     <row r="110" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="247"/>
+      <c r="A110" s="256"/>
       <c r="B110" s="137" t="s">
         <v>226</v>
       </c>
@@ -11677,7 +11674,7 @@
       <c r="BD110" s="89"/>
     </row>
     <row r="111" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="247"/>
+      <c r="A111" s="256"/>
       <c r="B111" s="136" t="s">
         <v>227</v>
       </c>
@@ -11739,7 +11736,7 @@
       <c r="BD111" s="89"/>
     </row>
     <row r="112" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="247"/>
+      <c r="A112" s="256"/>
       <c r="B112" s="137" t="s">
         <v>228</v>
       </c>
@@ -11807,7 +11804,7 @@
       <c r="BD112" s="89"/>
     </row>
     <row r="113" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="247"/>
+      <c r="A113" s="256"/>
       <c r="B113" s="135"/>
       <c r="C113" s="90" t="s">
         <v>174</v>
@@ -11873,7 +11870,7 @@
       <c r="BD113" s="89"/>
     </row>
     <row r="114" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="247"/>
+      <c r="A114" s="256"/>
       <c r="B114" s="135"/>
       <c r="C114" s="90" t="s">
         <v>173</v>
@@ -11939,7 +11936,7 @@
       <c r="BD114" s="89"/>
     </row>
     <row r="115" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="247"/>
+      <c r="A115" s="256"/>
       <c r="B115" s="136" t="s">
         <v>229</v>
       </c>
@@ -12001,7 +11998,7 @@
       <c r="BD115" s="89"/>
     </row>
     <row r="116" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="247"/>
+      <c r="A116" s="256"/>
       <c r="B116" s="137" t="s">
         <v>230</v>
       </c>
@@ -12069,7 +12066,7 @@
       <c r="BD116" s="89"/>
     </row>
     <row r="117" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="247"/>
+      <c r="A117" s="256"/>
       <c r="B117" s="137" t="s">
         <v>231</v>
       </c>
@@ -12137,7 +12134,7 @@
       <c r="BD117" s="89"/>
     </row>
     <row r="118" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="247"/>
+      <c r="A118" s="256"/>
       <c r="B118" s="137" t="s">
         <v>232</v>
       </c>
@@ -12205,7 +12202,7 @@
       <c r="BD118" s="89"/>
     </row>
     <row r="119" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="247"/>
+      <c r="A119" s="256"/>
       <c r="B119" s="137" t="s">
         <v>233</v>
       </c>
@@ -12273,7 +12270,7 @@
       <c r="BD119" s="89"/>
     </row>
     <row r="120" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="247"/>
+      <c r="A120" s="256"/>
       <c r="B120" s="136" t="s">
         <v>234</v>
       </c>
@@ -12335,7 +12332,7 @@
       <c r="BD120" s="89"/>
     </row>
     <row r="121" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="247"/>
+      <c r="A121" s="256"/>
       <c r="B121" s="137" t="s">
         <v>235</v>
       </c>
@@ -12403,7 +12400,7 @@
       <c r="BD121" s="89"/>
     </row>
     <row r="122" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="247"/>
+      <c r="A122" s="256"/>
       <c r="B122" s="137" t="s">
         <v>236</v>
       </c>
@@ -12471,7 +12468,7 @@
       <c r="BD122" s="89"/>
     </row>
     <row r="123" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="247"/>
+      <c r="A123" s="256"/>
       <c r="B123" s="136" t="s">
         <v>237</v>
       </c>
@@ -12533,7 +12530,7 @@
       <c r="BD123" s="89"/>
     </row>
     <row r="124" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="247"/>
+      <c r="A124" s="256"/>
       <c r="B124" s="137" t="s">
         <v>238</v>
       </c>
@@ -12597,7 +12594,7 @@
       <c r="BD124" s="89"/>
     </row>
     <row r="125" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="247"/>
+      <c r="A125" s="256"/>
       <c r="B125" s="135"/>
       <c r="C125" s="90" t="s">
         <v>183</v>
@@ -12663,7 +12660,7 @@
       <c r="BD125" s="89"/>
     </row>
     <row r="126" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="247"/>
+      <c r="A126" s="256"/>
       <c r="B126" s="135"/>
       <c r="C126" s="90" t="s">
         <v>182</v>
@@ -12729,7 +12726,7 @@
       <c r="BD126" s="89"/>
     </row>
     <row r="127" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="247"/>
+      <c r="A127" s="256"/>
       <c r="B127" s="137" t="s">
         <v>239</v>
       </c>
@@ -12793,7 +12790,7 @@
       <c r="BD127" s="89"/>
     </row>
     <row r="128" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="247"/>
+      <c r="A128" s="256"/>
       <c r="B128" s="135"/>
       <c r="C128" s="90" t="s">
         <v>282</v>
@@ -12859,7 +12856,7 @@
       <c r="BD128" s="89"/>
     </row>
     <row r="129" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="247"/>
+      <c r="A129" s="256"/>
       <c r="B129" s="135"/>
       <c r="C129" s="90" t="s">
         <v>283</v>
@@ -12925,7 +12922,7 @@
       <c r="BD129" s="89"/>
     </row>
     <row r="130" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="247"/>
+      <c r="A130" s="256"/>
       <c r="B130" s="136" t="s">
         <v>240</v>
       </c>
@@ -12987,7 +12984,7 @@
       <c r="BD130" s="89"/>
     </row>
     <row r="131" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="247"/>
+      <c r="A131" s="256"/>
       <c r="B131" s="137" t="s">
         <v>241</v>
       </c>
@@ -13055,7 +13052,7 @@
       <c r="BD131" s="89"/>
     </row>
     <row r="132" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="247"/>
+      <c r="A132" s="256"/>
       <c r="B132" s="137" t="s">
         <v>242</v>
       </c>
@@ -13123,7 +13120,7 @@
       <c r="BD132" s="89"/>
     </row>
     <row r="133" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="247"/>
+      <c r="A133" s="256"/>
       <c r="B133" s="136" t="s">
         <v>243</v>
       </c>
@@ -13185,7 +13182,7 @@
       <c r="BD133" s="89"/>
     </row>
     <row r="134" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="247"/>
+      <c r="A134" s="256"/>
       <c r="B134" s="137" t="s">
         <v>244</v>
       </c>
@@ -13253,7 +13250,7 @@
       <c r="BD134" s="89"/>
     </row>
     <row r="135" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="247"/>
+      <c r="A135" s="256"/>
       <c r="B135" s="136" t="s">
         <v>247</v>
       </c>
@@ -13315,7 +13312,7 @@
       <c r="BD135" s="89"/>
     </row>
     <row r="136" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="247"/>
+      <c r="A136" s="256"/>
       <c r="B136" s="137" t="s">
         <v>248</v>
       </c>
@@ -13383,7 +13380,7 @@
       <c r="BD136" s="89"/>
     </row>
     <row r="137" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="247"/>
+      <c r="A137" s="256"/>
       <c r="B137" s="136" t="s">
         <v>249</v>
       </c>
@@ -13445,7 +13442,7 @@
       <c r="BD137" s="89"/>
     </row>
     <row r="138" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="247"/>
+      <c r="A138" s="256"/>
       <c r="B138" s="137" t="s">
         <v>250</v>
       </c>
@@ -13513,7 +13510,7 @@
       <c r="BD138" s="89"/>
     </row>
     <row r="139" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="247"/>
+      <c r="A139" s="256"/>
       <c r="B139" s="136" t="s">
         <v>251</v>
       </c>
@@ -13575,7 +13572,7 @@
       <c r="BD139" s="89"/>
     </row>
     <row r="140" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="247"/>
+      <c r="A140" s="256"/>
       <c r="B140" s="137" t="s">
         <v>252</v>
       </c>
@@ -13643,7 +13640,7 @@
       <c r="BD140" s="89"/>
     </row>
     <row r="141" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="247"/>
+      <c r="A141" s="256"/>
       <c r="B141" s="137" t="s">
         <v>253</v>
       </c>
@@ -13711,7 +13708,7 @@
       <c r="BD141" s="89"/>
     </row>
     <row r="142" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="247"/>
+      <c r="A142" s="256"/>
       <c r="B142" s="136" t="s">
         <v>254</v>
       </c>
@@ -13773,7 +13770,7 @@
       <c r="BD142" s="89"/>
     </row>
     <row r="143" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A143" s="247"/>
+      <c r="A143" s="256"/>
       <c r="B143" s="137" t="s">
         <v>255</v>
       </c>
@@ -13841,7 +13838,7 @@
       <c r="BD143" s="89"/>
     </row>
     <row r="144" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="247"/>
+      <c r="A144" s="256"/>
       <c r="B144" s="136" t="s">
         <v>256</v>
       </c>
@@ -13903,7 +13900,7 @@
       <c r="BD144" s="89"/>
     </row>
     <row r="145" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="247"/>
+      <c r="A145" s="256"/>
       <c r="B145" s="137" t="s">
         <v>257</v>
       </c>
@@ -13971,7 +13968,7 @@
       <c r="BD145" s="89"/>
     </row>
     <row r="146" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="247"/>
+      <c r="A146" s="256"/>
       <c r="B146" s="136" t="s">
         <v>258</v>
       </c>
@@ -14033,7 +14030,7 @@
       <c r="BD146" s="89"/>
     </row>
     <row r="147" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="247"/>
+      <c r="A147" s="256"/>
       <c r="B147" s="137" t="s">
         <v>259</v>
       </c>
@@ -14101,7 +14098,7 @@
       <c r="BD147" s="89"/>
     </row>
     <row r="148" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="247"/>
+      <c r="A148" s="256"/>
       <c r="B148" s="136" t="s">
         <v>260</v>
       </c>
@@ -14163,7 +14160,7 @@
       <c r="BD148" s="89"/>
     </row>
     <row r="149" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="247"/>
+      <c r="A149" s="256"/>
       <c r="B149" s="137" t="s">
         <v>261</v>
       </c>
@@ -14231,7 +14228,7 @@
       <c r="BD149" s="89"/>
     </row>
     <row r="150" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="247"/>
+      <c r="A150" s="256"/>
       <c r="B150" s="137" t="s">
         <v>262</v>
       </c>
@@ -14299,7 +14296,7 @@
       <c r="BD150" s="89"/>
     </row>
     <row r="151" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="247"/>
+      <c r="A151" s="256"/>
       <c r="B151" s="137" t="s">
         <v>263</v>
       </c>
@@ -14367,7 +14364,7 @@
       <c r="BD151" s="89"/>
     </row>
     <row r="152" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="247"/>
+      <c r="A152" s="256"/>
       <c r="B152" s="137" t="s">
         <v>264</v>
       </c>
@@ -14435,7 +14432,7 @@
       <c r="BD152" s="89"/>
     </row>
     <row r="153" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="247"/>
+      <c r="A153" s="256"/>
       <c r="B153" s="136" t="s">
         <v>265</v>
       </c>
@@ -14497,7 +14494,7 @@
       <c r="BD153" s="89"/>
     </row>
     <row r="154" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="247"/>
+      <c r="A154" s="256"/>
       <c r="B154" s="137" t="s">
         <v>266</v>
       </c>
@@ -14565,7 +14562,7 @@
       <c r="BD154" s="89"/>
     </row>
     <row r="155" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="247"/>
+      <c r="A155" s="256"/>
       <c r="B155" s="137" t="s">
         <v>267</v>
       </c>
@@ -14633,7 +14630,7 @@
       <c r="BD155" s="89"/>
     </row>
     <row r="156" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="247"/>
+      <c r="A156" s="256"/>
       <c r="B156" s="136" t="s">
         <v>268</v>
       </c>
@@ -14695,7 +14692,7 @@
       <c r="BD156" s="89"/>
     </row>
     <row r="157" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="247"/>
+      <c r="A157" s="256"/>
       <c r="B157" s="137" t="s">
         <v>269</v>
       </c>
@@ -14763,7 +14760,7 @@
       <c r="BD157" s="89"/>
     </row>
     <row r="158" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="247"/>
+      <c r="A158" s="256"/>
       <c r="B158" s="137" t="s">
         <v>270</v>
       </c>
@@ -14831,7 +14828,7 @@
       <c r="BD158" s="89"/>
     </row>
     <row r="159" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="247"/>
+      <c r="A159" s="256"/>
       <c r="B159" s="137" t="s">
         <v>271</v>
       </c>
@@ -14899,7 +14896,7 @@
       <c r="BD159" s="89"/>
     </row>
     <row r="160" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A160" s="247"/>
+      <c r="A160" s="256"/>
       <c r="B160" s="137" t="s">
         <v>272</v>
       </c>
@@ -14967,7 +14964,7 @@
       <c r="BD160" s="89"/>
     </row>
     <row r="161" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A161" s="247"/>
+      <c r="A161" s="256"/>
       <c r="B161" s="136" t="s">
         <v>273</v>
       </c>
@@ -15029,7 +15026,7 @@
       <c r="BD161" s="89"/>
     </row>
     <row r="162" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A162" s="247"/>
+      <c r="A162" s="256"/>
       <c r="B162" s="137" t="s">
         <v>274</v>
       </c>
@@ -15097,7 +15094,7 @@
       <c r="BD162" s="89"/>
     </row>
     <row r="163" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A163" s="247"/>
+      <c r="A163" s="256"/>
       <c r="B163" s="137" t="s">
         <v>275</v>
       </c>
@@ -15165,7 +15162,7 @@
       <c r="BD163" s="89"/>
     </row>
     <row r="164" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A164" s="247"/>
+      <c r="A164" s="256"/>
       <c r="B164" s="136" t="s">
         <v>276</v>
       </c>
@@ -15227,7 +15224,7 @@
       <c r="BD164" s="89"/>
     </row>
     <row r="165" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A165" s="247"/>
+      <c r="A165" s="256"/>
       <c r="B165" s="137" t="s">
         <v>277</v>
       </c>
@@ -15295,7 +15292,7 @@
       <c r="BD165" s="89"/>
     </row>
     <row r="166" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A166" s="247"/>
+      <c r="A166" s="256"/>
       <c r="B166" s="137" t="s">
         <v>278</v>
       </c>
@@ -15363,7 +15360,7 @@
       <c r="BD166" s="89"/>
     </row>
     <row r="167" spans="1:56" s="80" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A167" s="247"/>
+      <c r="A167" s="256"/>
       <c r="B167" s="136" t="s">
         <v>279</v>
       </c>
@@ -15425,7 +15422,7 @@
       <c r="BD167" s="89"/>
     </row>
     <row r="168" spans="1:56" s="80" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="253"/>
+      <c r="A168" s="257"/>
       <c r="B168" s="138" t="s">
         <v>280</v>
       </c>
@@ -15565,74 +15562,74 @@
         <f>SUM(K170:BD170)</f>
         <v>3500</v>
       </c>
-      <c r="E170" s="268" t="s">
+      <c r="E170" s="240" t="s">
         <v>321</v>
       </c>
-      <c r="F170" s="268"/>
-      <c r="G170" s="268"/>
-      <c r="H170" s="260"/>
-      <c r="I170" s="258"/>
-      <c r="J170" s="258"/>
-      <c r="K170" s="258">
+      <c r="F170" s="240"/>
+      <c r="G170" s="240"/>
+      <c r="H170" s="235"/>
+      <c r="I170" s="233"/>
+      <c r="J170" s="233"/>
+      <c r="K170" s="233">
         <v>500</v>
       </c>
-      <c r="L170" s="258"/>
-      <c r="M170" s="258"/>
-      <c r="N170" s="259"/>
-      <c r="O170" s="260"/>
-      <c r="P170" s="258"/>
-      <c r="Q170" s="258"/>
-      <c r="R170" s="258">
+      <c r="L170" s="233"/>
+      <c r="M170" s="233"/>
+      <c r="N170" s="234"/>
+      <c r="O170" s="235"/>
+      <c r="P170" s="233"/>
+      <c r="Q170" s="233"/>
+      <c r="R170" s="233">
         <v>500</v>
       </c>
-      <c r="S170" s="258"/>
-      <c r="T170" s="258"/>
-      <c r="U170" s="259"/>
-      <c r="V170" s="260"/>
-      <c r="W170" s="258"/>
-      <c r="X170" s="258"/>
-      <c r="Y170" s="258">
+      <c r="S170" s="233"/>
+      <c r="T170" s="233"/>
+      <c r="U170" s="234"/>
+      <c r="V170" s="235"/>
+      <c r="W170" s="233"/>
+      <c r="X170" s="233"/>
+      <c r="Y170" s="233">
         <v>500</v>
       </c>
-      <c r="Z170" s="258"/>
-      <c r="AA170" s="258"/>
-      <c r="AB170" s="259"/>
-      <c r="AC170" s="260"/>
-      <c r="AD170" s="258"/>
-      <c r="AE170" s="258"/>
-      <c r="AF170" s="258">
+      <c r="Z170" s="233"/>
+      <c r="AA170" s="233"/>
+      <c r="AB170" s="234"/>
+      <c r="AC170" s="235"/>
+      <c r="AD170" s="233"/>
+      <c r="AE170" s="233"/>
+      <c r="AF170" s="233">
         <v>500</v>
       </c>
-      <c r="AG170" s="258"/>
-      <c r="AH170" s="258"/>
-      <c r="AI170" s="259"/>
-      <c r="AJ170" s="260"/>
-      <c r="AK170" s="258"/>
-      <c r="AL170" s="258"/>
-      <c r="AM170" s="258">
+      <c r="AG170" s="233"/>
+      <c r="AH170" s="233"/>
+      <c r="AI170" s="234"/>
+      <c r="AJ170" s="235"/>
+      <c r="AK170" s="233"/>
+      <c r="AL170" s="233"/>
+      <c r="AM170" s="233">
         <v>500</v>
       </c>
-      <c r="AN170" s="258"/>
-      <c r="AO170" s="258"/>
-      <c r="AP170" s="259"/>
-      <c r="AQ170" s="260"/>
-      <c r="AR170" s="258"/>
-      <c r="AS170" s="258"/>
-      <c r="AT170" s="258">
+      <c r="AN170" s="233"/>
+      <c r="AO170" s="233"/>
+      <c r="AP170" s="234"/>
+      <c r="AQ170" s="235"/>
+      <c r="AR170" s="233"/>
+      <c r="AS170" s="233"/>
+      <c r="AT170" s="233">
         <v>500</v>
       </c>
-      <c r="AU170" s="258"/>
-      <c r="AV170" s="258"/>
-      <c r="AW170" s="259"/>
-      <c r="AX170" s="260"/>
-      <c r="AY170" s="258"/>
-      <c r="AZ170" s="258"/>
-      <c r="BA170" s="258">
+      <c r="AU170" s="233"/>
+      <c r="AV170" s="233"/>
+      <c r="AW170" s="234"/>
+      <c r="AX170" s="235"/>
+      <c r="AY170" s="233"/>
+      <c r="AZ170" s="233"/>
+      <c r="BA170" s="233">
         <v>500</v>
       </c>
-      <c r="BB170" s="258"/>
-      <c r="BC170" s="258"/>
-      <c r="BD170" s="259"/>
+      <c r="BB170" s="233"/>
+      <c r="BC170" s="233"/>
+      <c r="BD170" s="234"/>
     </row>
     <row r="171" spans="1:56" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A171" s="150"/>
@@ -15644,74 +15641,74 @@
         <f>SUM(K171:BD171)</f>
         <v>4410</v>
       </c>
-      <c r="E171" s="268" t="s">
+      <c r="E171" s="240" t="s">
         <v>320</v>
       </c>
-      <c r="F171" s="268"/>
-      <c r="G171" s="268"/>
-      <c r="H171" s="260"/>
-      <c r="I171" s="258"/>
-      <c r="J171" s="258"/>
-      <c r="K171" s="258">
+      <c r="F171" s="240"/>
+      <c r="G171" s="240"/>
+      <c r="H171" s="235"/>
+      <c r="I171" s="233"/>
+      <c r="J171" s="233"/>
+      <c r="K171" s="233">
         <v>630</v>
       </c>
-      <c r="L171" s="258"/>
-      <c r="M171" s="258"/>
-      <c r="N171" s="259"/>
-      <c r="O171" s="260"/>
-      <c r="P171" s="258"/>
-      <c r="Q171" s="258"/>
-      <c r="R171" s="258">
+      <c r="L171" s="233"/>
+      <c r="M171" s="233"/>
+      <c r="N171" s="234"/>
+      <c r="O171" s="235"/>
+      <c r="P171" s="233"/>
+      <c r="Q171" s="233"/>
+      <c r="R171" s="233">
         <v>630</v>
       </c>
-      <c r="S171" s="258"/>
-      <c r="T171" s="258"/>
-      <c r="U171" s="259"/>
-      <c r="V171" s="260"/>
-      <c r="W171" s="258"/>
-      <c r="X171" s="258"/>
-      <c r="Y171" s="258">
+      <c r="S171" s="233"/>
+      <c r="T171" s="233"/>
+      <c r="U171" s="234"/>
+      <c r="V171" s="235"/>
+      <c r="W171" s="233"/>
+      <c r="X171" s="233"/>
+      <c r="Y171" s="233">
         <v>630</v>
       </c>
-      <c r="Z171" s="258"/>
-      <c r="AA171" s="258"/>
-      <c r="AB171" s="259"/>
-      <c r="AC171" s="260"/>
-      <c r="AD171" s="258"/>
-      <c r="AE171" s="258"/>
-      <c r="AF171" s="258">
+      <c r="Z171" s="233"/>
+      <c r="AA171" s="233"/>
+      <c r="AB171" s="234"/>
+      <c r="AC171" s="235"/>
+      <c r="AD171" s="233"/>
+      <c r="AE171" s="233"/>
+      <c r="AF171" s="233">
         <v>630</v>
       </c>
-      <c r="AG171" s="258"/>
-      <c r="AH171" s="258"/>
-      <c r="AI171" s="259"/>
-      <c r="AJ171" s="260"/>
-      <c r="AK171" s="258"/>
-      <c r="AL171" s="258"/>
-      <c r="AM171" s="258">
+      <c r="AG171" s="233"/>
+      <c r="AH171" s="233"/>
+      <c r="AI171" s="234"/>
+      <c r="AJ171" s="235"/>
+      <c r="AK171" s="233"/>
+      <c r="AL171" s="233"/>
+      <c r="AM171" s="233">
         <v>630</v>
       </c>
-      <c r="AN171" s="258"/>
-      <c r="AO171" s="258"/>
-      <c r="AP171" s="259"/>
-      <c r="AQ171" s="260"/>
-      <c r="AR171" s="258"/>
-      <c r="AS171" s="258"/>
-      <c r="AT171" s="258">
+      <c r="AN171" s="233"/>
+      <c r="AO171" s="233"/>
+      <c r="AP171" s="234"/>
+      <c r="AQ171" s="235"/>
+      <c r="AR171" s="233"/>
+      <c r="AS171" s="233"/>
+      <c r="AT171" s="233">
         <v>630</v>
       </c>
-      <c r="AU171" s="258"/>
-      <c r="AV171" s="258"/>
-      <c r="AW171" s="259"/>
-      <c r="AX171" s="260"/>
-      <c r="AY171" s="258"/>
-      <c r="AZ171" s="258"/>
-      <c r="BA171" s="258">
+      <c r="AU171" s="233"/>
+      <c r="AV171" s="233"/>
+      <c r="AW171" s="234"/>
+      <c r="AX171" s="235"/>
+      <c r="AY171" s="233"/>
+      <c r="AZ171" s="233"/>
+      <c r="BA171" s="233">
         <v>630</v>
       </c>
-      <c r="BB171" s="258"/>
-      <c r="BC171" s="258"/>
-      <c r="BD171" s="259"/>
+      <c r="BB171" s="233"/>
+      <c r="BC171" s="233"/>
+      <c r="BD171" s="234"/>
     </row>
     <row r="172" spans="1:56" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="152"/>
@@ -15723,74 +15720,74 @@
         <f>+D169+D171</f>
         <v>9910</v>
       </c>
-      <c r="E172" s="261" t="s">
+      <c r="E172" s="249" t="s">
         <v>304</v>
       </c>
-      <c r="F172" s="261"/>
-      <c r="G172" s="261"/>
-      <c r="H172" s="256"/>
-      <c r="I172" s="257"/>
-      <c r="J172" s="257"/>
-      <c r="K172" s="254">
+      <c r="F172" s="249"/>
+      <c r="G172" s="249"/>
+      <c r="H172" s="251"/>
+      <c r="I172" s="252"/>
+      <c r="J172" s="252"/>
+      <c r="K172" s="253">
         <v>44607</v>
       </c>
-      <c r="L172" s="254"/>
-      <c r="M172" s="254"/>
-      <c r="N172" s="255"/>
-      <c r="O172" s="256"/>
-      <c r="P172" s="257"/>
-      <c r="Q172" s="257"/>
-      <c r="R172" s="254">
+      <c r="L172" s="253"/>
+      <c r="M172" s="253"/>
+      <c r="N172" s="254"/>
+      <c r="O172" s="251"/>
+      <c r="P172" s="252"/>
+      <c r="Q172" s="252"/>
+      <c r="R172" s="253">
         <v>44607</v>
       </c>
-      <c r="S172" s="254"/>
-      <c r="T172" s="254"/>
-      <c r="U172" s="255"/>
-      <c r="V172" s="256"/>
-      <c r="W172" s="257"/>
-      <c r="X172" s="257"/>
-      <c r="Y172" s="254">
+      <c r="S172" s="253"/>
+      <c r="T172" s="253"/>
+      <c r="U172" s="254"/>
+      <c r="V172" s="251"/>
+      <c r="W172" s="252"/>
+      <c r="X172" s="252"/>
+      <c r="Y172" s="253">
         <v>44607</v>
       </c>
-      <c r="Z172" s="254"/>
-      <c r="AA172" s="254"/>
-      <c r="AB172" s="255"/>
-      <c r="AC172" s="256"/>
-      <c r="AD172" s="257"/>
-      <c r="AE172" s="257"/>
-      <c r="AF172" s="254">
+      <c r="Z172" s="253"/>
+      <c r="AA172" s="253"/>
+      <c r="AB172" s="254"/>
+      <c r="AC172" s="251"/>
+      <c r="AD172" s="252"/>
+      <c r="AE172" s="252"/>
+      <c r="AF172" s="253">
         <v>44607</v>
       </c>
-      <c r="AG172" s="254"/>
-      <c r="AH172" s="254"/>
-      <c r="AI172" s="255"/>
-      <c r="AJ172" s="256"/>
-      <c r="AK172" s="257"/>
-      <c r="AL172" s="257"/>
-      <c r="AM172" s="254">
+      <c r="AG172" s="253"/>
+      <c r="AH172" s="253"/>
+      <c r="AI172" s="254"/>
+      <c r="AJ172" s="251"/>
+      <c r="AK172" s="252"/>
+      <c r="AL172" s="252"/>
+      <c r="AM172" s="253">
         <v>44607</v>
       </c>
-      <c r="AN172" s="254"/>
-      <c r="AO172" s="254"/>
-      <c r="AP172" s="255"/>
-      <c r="AQ172" s="256"/>
-      <c r="AR172" s="257"/>
-      <c r="AS172" s="257"/>
-      <c r="AT172" s="254">
+      <c r="AN172" s="253"/>
+      <c r="AO172" s="253"/>
+      <c r="AP172" s="254"/>
+      <c r="AQ172" s="251"/>
+      <c r="AR172" s="252"/>
+      <c r="AS172" s="252"/>
+      <c r="AT172" s="253">
         <v>44607</v>
       </c>
-      <c r="AU172" s="254"/>
-      <c r="AV172" s="254"/>
-      <c r="AW172" s="255"/>
-      <c r="AX172" s="256"/>
-      <c r="AY172" s="257"/>
-      <c r="AZ172" s="257"/>
-      <c r="BA172" s="254">
+      <c r="AU172" s="253"/>
+      <c r="AV172" s="253"/>
+      <c r="AW172" s="254"/>
+      <c r="AX172" s="251"/>
+      <c r="AY172" s="252"/>
+      <c r="AZ172" s="252"/>
+      <c r="BA172" s="253">
         <v>44607</v>
       </c>
-      <c r="BB172" s="254"/>
-      <c r="BC172" s="254"/>
-      <c r="BD172" s="255"/>
+      <c r="BB172" s="253"/>
+      <c r="BC172" s="253"/>
+      <c r="BD172" s="254"/>
     </row>
     <row r="173" spans="1:56" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="163"/>
@@ -15915,6 +15912,75 @@
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="AJ6:AP6"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A15:A30"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="O6:U6"/>
+    <mergeCell ref="V6:AB6"/>
+    <mergeCell ref="AC6:AI6"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:N6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A104:A168"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A87:A102"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A37:A74"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="R172:U172"/>
+    <mergeCell ref="V172:X172"/>
+    <mergeCell ref="Y170:AB170"/>
+    <mergeCell ref="AC170:AE170"/>
+    <mergeCell ref="AF170:AI170"/>
+    <mergeCell ref="V170:X170"/>
+    <mergeCell ref="R170:U170"/>
+    <mergeCell ref="AQ172:AS172"/>
+    <mergeCell ref="AT172:AW172"/>
+    <mergeCell ref="AX172:AZ172"/>
+    <mergeCell ref="BA172:BD172"/>
+    <mergeCell ref="Y172:AB172"/>
+    <mergeCell ref="AC172:AE172"/>
+    <mergeCell ref="AF172:AI172"/>
+    <mergeCell ref="AJ172:AL172"/>
+    <mergeCell ref="AM172:AP172"/>
+    <mergeCell ref="E172:G172"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="I3:Q3"/>
+    <mergeCell ref="I4:Q4"/>
+    <mergeCell ref="H172:J172"/>
+    <mergeCell ref="K172:N172"/>
+    <mergeCell ref="O172:Q172"/>
+    <mergeCell ref="H170:J170"/>
+    <mergeCell ref="K170:N170"/>
+    <mergeCell ref="O170:Q170"/>
+    <mergeCell ref="AL1:BD1"/>
+    <mergeCell ref="O1:AG1"/>
+    <mergeCell ref="AH1:AK1"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="E171:G171"/>
+    <mergeCell ref="H171:J171"/>
+    <mergeCell ref="K171:N171"/>
+    <mergeCell ref="O171:Q171"/>
+    <mergeCell ref="R171:U171"/>
+    <mergeCell ref="V171:X171"/>
+    <mergeCell ref="Y171:AB171"/>
+    <mergeCell ref="AC171:AE171"/>
+    <mergeCell ref="AF171:AI171"/>
+    <mergeCell ref="AJ171:AL171"/>
+    <mergeCell ref="AM171:AP171"/>
+    <mergeCell ref="AQ171:AS171"/>
     <mergeCell ref="AT171:AW171"/>
     <mergeCell ref="AX171:AZ171"/>
     <mergeCell ref="BA171:BD171"/>
@@ -15931,75 +15997,6 @@
     <mergeCell ref="AQ170:AS170"/>
     <mergeCell ref="AQ6:AW6"/>
     <mergeCell ref="AX6:BD6"/>
-    <mergeCell ref="AL1:BD1"/>
-    <mergeCell ref="O1:AG1"/>
-    <mergeCell ref="AH1:AK1"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="E171:G171"/>
-    <mergeCell ref="H171:J171"/>
-    <mergeCell ref="K171:N171"/>
-    <mergeCell ref="O171:Q171"/>
-    <mergeCell ref="R171:U171"/>
-    <mergeCell ref="V171:X171"/>
-    <mergeCell ref="Y171:AB171"/>
-    <mergeCell ref="AC171:AE171"/>
-    <mergeCell ref="AF171:AI171"/>
-    <mergeCell ref="AJ171:AL171"/>
-    <mergeCell ref="AM171:AP171"/>
-    <mergeCell ref="AQ171:AS171"/>
-    <mergeCell ref="E172:G172"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="I3:Q3"/>
-    <mergeCell ref="I4:Q4"/>
-    <mergeCell ref="H172:J172"/>
-    <mergeCell ref="K172:N172"/>
-    <mergeCell ref="O172:Q172"/>
-    <mergeCell ref="H170:J170"/>
-    <mergeCell ref="K170:N170"/>
-    <mergeCell ref="O170:Q170"/>
-    <mergeCell ref="AQ172:AS172"/>
-    <mergeCell ref="AT172:AW172"/>
-    <mergeCell ref="AX172:AZ172"/>
-    <mergeCell ref="BA172:BD172"/>
-    <mergeCell ref="Y172:AB172"/>
-    <mergeCell ref="AC172:AE172"/>
-    <mergeCell ref="AF172:AI172"/>
-    <mergeCell ref="AJ172:AL172"/>
-    <mergeCell ref="AM172:AP172"/>
-    <mergeCell ref="R172:U172"/>
-    <mergeCell ref="V172:X172"/>
-    <mergeCell ref="Y170:AB170"/>
-    <mergeCell ref="AC170:AE170"/>
-    <mergeCell ref="AF170:AI170"/>
-    <mergeCell ref="V170:X170"/>
-    <mergeCell ref="R170:U170"/>
-    <mergeCell ref="A104:A168"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A87:A102"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A37:A74"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="AJ6:AP6"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A15:A30"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="O6:U6"/>
-    <mergeCell ref="V6:AB6"/>
-    <mergeCell ref="AC6:AI6"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:N6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D5:E5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -16022,7 +16019,7 @@
   <dimension ref="B1:AG36"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="129" zoomScaleNormal="129" zoomScaleSheetLayoutView="129" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -16030,12 +16027,12 @@
     <col min="1" max="1" width="4.7109375" style="183" customWidth="1"/>
     <col min="2" max="2" width="16.140625" style="183" customWidth="1"/>
     <col min="3" max="3" width="65" style="183" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="183" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="183" customWidth="1"/>
+    <col min="4" max="4" width="15" style="183" customWidth="1"/>
+    <col min="5" max="5" width="13" style="183" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" style="183" customWidth="1"/>
     <col min="7" max="7" width="10.140625" style="183" customWidth="1"/>
     <col min="8" max="8" width="12" style="183" customWidth="1"/>
-    <col min="9" max="9" width="14" style="183" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="183" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" style="183" customWidth="1"/>
     <col min="11" max="11" width="4.7109375" style="183" customWidth="1"/>
     <col min="12" max="15" width="5.7109375" style="183" customWidth="1"/>
@@ -16047,15 +16044,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="275" t="s">
+      <c r="C1" s="296" t="s">
         <v>348</v>
       </c>
-      <c r="D1" s="275"/>
-      <c r="E1" s="275"/>
-      <c r="F1" s="275"/>
-      <c r="G1" s="275"/>
-      <c r="H1" s="275"/>
-      <c r="I1" s="275"/>
+      <c r="D1" s="296"/>
+      <c r="E1" s="296"/>
+      <c r="F1" s="296"/>
+      <c r="G1" s="296"/>
+      <c r="H1" s="296"/>
+      <c r="I1" s="296"/>
       <c r="J1" s="193"/>
       <c r="K1" s="193"/>
       <c r="L1" s="193"/>
@@ -16083,13 +16080,13 @@
     </row>
     <row r="2" spans="2:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="193"/>
-      <c r="C2" s="275"/>
-      <c r="D2" s="275"/>
-      <c r="E2" s="275"/>
-      <c r="F2" s="275"/>
-      <c r="G2" s="275"/>
-      <c r="H2" s="275"/>
-      <c r="I2" s="275"/>
+      <c r="C2" s="296"/>
+      <c r="D2" s="296"/>
+      <c r="E2" s="296"/>
+      <c r="F2" s="296"/>
+      <c r="G2" s="296"/>
+      <c r="H2" s="296"/>
+      <c r="I2" s="296"/>
       <c r="J2" s="193"/>
       <c r="K2" s="193"/>
       <c r="L2" s="193"/>
@@ -16153,14 +16150,14 @@
       <c r="C4" s="202" t="s">
         <v>350</v>
       </c>
-      <c r="D4" s="276" t="s">
+      <c r="D4" s="297" t="s">
         <v>337</v>
       </c>
-      <c r="E4" s="276"/>
-      <c r="F4" s="276"/>
-      <c r="G4" s="276"/>
-      <c r="H4" s="276"/>
-      <c r="I4" s="277"/>
+      <c r="E4" s="297"/>
+      <c r="F4" s="297"/>
+      <c r="G4" s="297"/>
+      <c r="H4" s="297"/>
+      <c r="I4" s="298"/>
       <c r="J4" s="193"/>
       <c r="K4" s="193"/>
       <c r="L4" s="193"/>
@@ -16190,14 +16187,14 @@
       <c r="C5" s="202" t="s">
         <v>340</v>
       </c>
-      <c r="D5" s="276" t="s">
+      <c r="D5" s="297" t="s">
         <v>349</v>
       </c>
-      <c r="E5" s="276"/>
-      <c r="F5" s="276"/>
-      <c r="G5" s="276"/>
-      <c r="H5" s="276"/>
-      <c r="I5" s="277"/>
+      <c r="E5" s="297"/>
+      <c r="F5" s="297"/>
+      <c r="G5" s="297"/>
+      <c r="H5" s="297"/>
+      <c r="I5" s="298"/>
       <c r="J5" s="193"/>
       <c r="K5" s="193"/>
       <c r="L5" s="193"/>
@@ -16261,8 +16258,8 @@
       <c r="C7" s="200" t="s">
         <v>341</v>
       </c>
-      <c r="D7" s="278"/>
-      <c r="E7" s="279"/>
+      <c r="D7" s="299"/>
+      <c r="E7" s="300"/>
       <c r="F7" s="225"/>
       <c r="G7" s="225"/>
       <c r="H7" s="188"/>
@@ -16296,8 +16293,8 @@
       <c r="C8" s="200" t="s">
         <v>342</v>
       </c>
-      <c r="D8" s="278"/>
-      <c r="E8" s="279"/>
+      <c r="D8" s="299"/>
+      <c r="E8" s="300"/>
       <c r="F8" s="225"/>
       <c r="G8" s="225"/>
       <c r="H8" s="188"/>
@@ -16331,8 +16328,8 @@
       <c r="C9" s="200" t="s">
         <v>343</v>
       </c>
-      <c r="D9" s="278"/>
-      <c r="E9" s="279"/>
+      <c r="D9" s="299"/>
+      <c r="E9" s="300"/>
       <c r="F9" s="188"/>
       <c r="I9" s="193"/>
       <c r="L9" s="193"/>
@@ -16391,11 +16388,11 @@
       <c r="C11" s="202" t="s">
         <v>351</v>
       </c>
-      <c r="D11" s="280" t="s">
+      <c r="D11" s="301" t="s">
         <v>338</v>
       </c>
-      <c r="E11" s="276"/>
-      <c r="F11" s="277"/>
+      <c r="E11" s="297"/>
+      <c r="F11" s="298"/>
       <c r="G11" s="180"/>
       <c r="H11" s="180"/>
       <c r="I11" s="180"/>
@@ -16422,11 +16419,11 @@
       <c r="C12" s="202" t="s">
         <v>352</v>
       </c>
-      <c r="D12" s="281" t="s">
+      <c r="D12" s="302" t="s">
         <v>339</v>
       </c>
-      <c r="E12" s="282"/>
-      <c r="F12" s="283"/>
+      <c r="E12" s="303"/>
+      <c r="F12" s="304"/>
       <c r="G12" s="226"/>
       <c r="H12" s="226"/>
       <c r="I12" s="226"/>
@@ -16501,23 +16498,21 @@
       <c r="AC14" s="186"/>
     </row>
     <row r="15" spans="2:33" s="182" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="284" t="s">
+      <c r="B15" s="273" t="s">
         <v>160</v>
       </c>
-      <c r="C15" s="294" t="s">
+      <c r="C15" s="283" t="s">
         <v>344</v>
       </c>
-      <c r="D15" s="299" t="s">
+      <c r="D15" s="290"/>
+      <c r="E15" s="291"/>
+      <c r="F15" s="290" t="s">
         <v>301</v>
       </c>
-      <c r="E15" s="300"/>
-      <c r="F15" s="301"/>
-      <c r="G15" s="299" t="s">
-        <v>357</v>
-      </c>
-      <c r="H15" s="300"/>
-      <c r="I15" s="300"/>
-      <c r="J15" s="301"/>
+      <c r="G15" s="291"/>
+      <c r="H15" s="292"/>
+      <c r="I15" s="291"/>
+      <c r="J15" s="292"/>
       <c r="K15" s="189"/>
       <c r="L15" s="189"/>
       <c r="M15" s="189"/>
@@ -16542,16 +16537,16 @@
       <c r="AF15" s="183"/>
       <c r="AG15" s="183"/>
     </row>
-    <row r="16" spans="2:33" s="182" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="285"/>
-      <c r="C16" s="295"/>
-      <c r="D16" s="302"/>
-      <c r="E16" s="303"/>
-      <c r="F16" s="304"/>
-      <c r="G16" s="302"/>
-      <c r="H16" s="303"/>
-      <c r="I16" s="303"/>
-      <c r="J16" s="304"/>
+    <row r="16" spans="2:33" s="182" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="274"/>
+      <c r="C16" s="284"/>
+      <c r="D16" s="293"/>
+      <c r="E16" s="294"/>
+      <c r="F16" s="293"/>
+      <c r="G16" s="294"/>
+      <c r="H16" s="295"/>
+      <c r="I16" s="294"/>
+      <c r="J16" s="295"/>
       <c r="K16" s="190"/>
       <c r="L16" s="190"/>
       <c r="M16" s="190"/>
@@ -16577,51 +16572,51 @@
       <c r="AG16" s="183"/>
     </row>
     <row r="17" spans="2:29" s="182" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="285"/>
-      <c r="C17" s="295"/>
-      <c r="D17" s="288" t="s">
+      <c r="B17" s="274"/>
+      <c r="C17" s="284"/>
+      <c r="D17" s="277" t="s">
+        <v>354</v>
+      </c>
+      <c r="E17" s="277" t="s">
+        <v>353</v>
+      </c>
+      <c r="F17" s="285" t="s">
         <v>345</v>
       </c>
-      <c r="E17" s="288" t="s">
+      <c r="G17" s="286" t="s">
         <v>346</v>
       </c>
-      <c r="F17" s="296" t="s">
+      <c r="H17" s="286" t="s">
         <v>347</v>
       </c>
-      <c r="G17" s="273" t="s">
-        <v>353</v>
-      </c>
-      <c r="H17" s="273" t="s">
-        <v>354</v>
-      </c>
-      <c r="I17" s="290" t="s">
+      <c r="I17" s="279" t="s">
+        <v>356</v>
+      </c>
+      <c r="J17" s="288" t="s">
         <v>355</v>
       </c>
-      <c r="J17" s="297" t="s">
-        <v>356</v>
-      </c>
     </row>
     <row r="18" spans="2:29" s="182" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="285"/>
-      <c r="C18" s="295"/>
-      <c r="D18" s="288"/>
-      <c r="E18" s="288"/>
-      <c r="F18" s="273"/>
-      <c r="G18" s="273"/>
-      <c r="H18" s="273"/>
-      <c r="I18" s="288"/>
-      <c r="J18" s="297"/>
-    </row>
-    <row r="19" spans="2:29" s="182" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="286"/>
-      <c r="C19" s="295"/>
-      <c r="D19" s="289"/>
-      <c r="E19" s="289"/>
-      <c r="F19" s="274"/>
-      <c r="G19" s="274"/>
-      <c r="H19" s="274"/>
-      <c r="I19" s="289"/>
-      <c r="J19" s="298"/>
+      <c r="B18" s="274"/>
+      <c r="C18" s="284"/>
+      <c r="D18" s="277"/>
+      <c r="E18" s="277"/>
+      <c r="F18" s="286"/>
+      <c r="G18" s="286"/>
+      <c r="H18" s="286"/>
+      <c r="I18" s="277"/>
+      <c r="J18" s="288"/>
+    </row>
+    <row r="19" spans="2:29" s="182" customFormat="1" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="275"/>
+      <c r="C19" s="284"/>
+      <c r="D19" s="278"/>
+      <c r="E19" s="278"/>
+      <c r="F19" s="287"/>
+      <c r="G19" s="287"/>
+      <c r="H19" s="287"/>
+      <c r="I19" s="278"/>
+      <c r="J19" s="289"/>
     </row>
     <row r="20" spans="2:29" s="182" customFormat="1" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B20" s="208"/>
@@ -16664,9 +16659,9 @@
       <c r="G23" s="227"/>
       <c r="H23" s="228"/>
       <c r="I23" s="228"/>
-      <c r="J23" s="291"/>
-      <c r="K23" s="291"/>
-      <c r="L23" s="291"/>
+      <c r="J23" s="280"/>
+      <c r="K23" s="280"/>
+      <c r="L23" s="280"/>
       <c r="M23" s="206"/>
       <c r="N23" s="206"/>
       <c r="O23" s="206"/>
@@ -16676,13 +16671,13 @@
       <c r="S23" s="206"/>
       <c r="T23" s="206"/>
       <c r="U23" s="206"/>
-      <c r="V23" s="292"/>
-      <c r="W23" s="292"/>
-      <c r="X23" s="291"/>
-      <c r="Y23" s="291"/>
-      <c r="Z23" s="291"/>
-      <c r="AA23" s="291"/>
-      <c r="AB23" s="291"/>
+      <c r="V23" s="281"/>
+      <c r="W23" s="281"/>
+      <c r="X23" s="280"/>
+      <c r="Y23" s="280"/>
+      <c r="Z23" s="280"/>
+      <c r="AA23" s="280"/>
+      <c r="AB23" s="280"/>
       <c r="AC23" s="204"/>
     </row>
     <row r="24" spans="2:29" s="182" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -16720,9 +16715,9 @@
       <c r="G25" s="230"/>
       <c r="H25" s="228"/>
       <c r="I25" s="228"/>
-      <c r="J25" s="291"/>
-      <c r="K25" s="291"/>
-      <c r="L25" s="291"/>
+      <c r="J25" s="280"/>
+      <c r="K25" s="280"/>
+      <c r="L25" s="280"/>
       <c r="M25" s="206"/>
       <c r="N25" s="206"/>
       <c r="O25" s="206"/>
@@ -16733,9 +16728,9 @@
       <c r="T25" s="206"/>
       <c r="U25" s="206"/>
       <c r="V25" s="206"/>
-      <c r="W25" s="293"/>
-      <c r="X25" s="293"/>
-      <c r="Y25" s="293"/>
+      <c r="W25" s="282"/>
+      <c r="X25" s="282"/>
+      <c r="Y25" s="282"/>
       <c r="Z25" s="206"/>
       <c r="AA25" s="206"/>
       <c r="AB25" s="206"/>
@@ -16763,11 +16758,11 @@
       <c r="T26" s="206"/>
       <c r="U26" s="206"/>
       <c r="V26" s="206"/>
-      <c r="W26" s="287"/>
-      <c r="X26" s="287"/>
-      <c r="Y26" s="287"/>
-      <c r="Z26" s="287"/>
-      <c r="AA26" s="287"/>
+      <c r="W26" s="276"/>
+      <c r="X26" s="276"/>
+      <c r="Y26" s="276"/>
+      <c r="Z26" s="276"/>
+      <c r="AA26" s="276"/>
       <c r="AB26" s="206"/>
       <c r="AC26" s="206"/>
     </row>
@@ -16816,7 +16811,19 @@
       <c r="C36" s="185"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="26">
+    <mergeCell ref="H17:H19"/>
+    <mergeCell ref="C1:I2"/>
+    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="D5:I5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="F15:H16"/>
+    <mergeCell ref="D15:E16"/>
+    <mergeCell ref="I15:J16"/>
     <mergeCell ref="B15:B19"/>
     <mergeCell ref="W26:AA26"/>
     <mergeCell ref="D17:D19"/>
@@ -16831,17 +16838,6 @@
     <mergeCell ref="F17:F19"/>
     <mergeCell ref="G17:G19"/>
     <mergeCell ref="J17:J19"/>
-    <mergeCell ref="G15:J16"/>
-    <mergeCell ref="D15:F16"/>
-    <mergeCell ref="H17:H19"/>
-    <mergeCell ref="C1:I2"/>
-    <mergeCell ref="D4:I4"/>
-    <mergeCell ref="D5:I5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D12:F12"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="P23">
@@ -16854,7 +16850,7 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="76" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>